<commit_message>
create a .h and .cpp for function
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/192d16467d0539cb/Documents/5.Bricolage/5.StationMeteo/StationMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2439E782-5946-42B6-891B-FC2C74543175}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1C697945-4425-427F-8628-0E5BA3DA59CD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="3924" yWindow="2232" windowWidth="15240" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat a faire" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="222">
   <si>
     <t>Produit</t>
   </si>
@@ -493,15 +493,9 @@
     <t>convertisseur</t>
   </si>
   <si>
-    <t>batterie 2Ah</t>
-  </si>
-  <si>
     <t>capteur</t>
   </si>
   <si>
-    <t>semageek</t>
-  </si>
-  <si>
     <t>adafruit</t>
   </si>
   <si>
@@ -514,9 +508,6 @@
     <t>divers</t>
   </si>
   <si>
-    <t>NEMA box</t>
-  </si>
-  <si>
     <t>capteur luminosité</t>
   </si>
   <si>
@@ -692,6 +683,30 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>chinois</t>
+  </si>
+  <si>
+    <t>antenne</t>
+  </si>
+  <si>
+    <t>connecteur SMA pcb</t>
+  </si>
+  <si>
+    <t>Aliexpress</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>batterie 5Ah</t>
+  </si>
+  <si>
+    <t>ebay</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
 </sst>
 </file>
@@ -1500,7 +1515,7 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1515,15 +1530,15 @@
       </c>
       <c r="J1" s="2">
         <f>SUM(H3:H20)</f>
-        <v>128.6</v>
+        <v>166.11</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
@@ -1538,7 +1553,7 @@
         <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
@@ -1546,10 +1561,13 @@
         <v>147</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
         <v>148</v>
+      </c>
+      <c r="E3" t="s">
+        <v>221</v>
       </c>
       <c r="F3">
         <f>55*1.2</f>
@@ -1566,13 +1584,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D4" t="s">
         <v>149</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>221</v>
       </c>
       <c r="F4" s="1">
         <f>15*1.2</f>
@@ -1582,25 +1600,30 @@
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H16" si="0">G4*F4</f>
+        <f t="shared" ref="H4:H18" si="0">G4*F4</f>
         <v>18</v>
       </c>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>150</v>
+        <v>219</v>
       </c>
       <c r="E5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="1"/>
+        <v>220</v>
+      </c>
+      <c r="F5" s="1">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
       <c r="H5" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I5" s="1"/>
       <c r="K5" s="3"/>
@@ -1617,19 +1640,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" t="s">
         <v>151</v>
       </c>
-      <c r="B8" t="s">
-        <v>153</v>
-      </c>
       <c r="C8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E8" t="s">
-        <v>152</v>
+        <v>221</v>
       </c>
       <c r="F8" s="1">
         <f>18*1.2</f>
@@ -1646,33 +1669,31 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>221</v>
       </c>
       <c r="F9" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9" s="1">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I10" s="1"/>
-      <c r="J10" s="3" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="F11" s="1"/>
@@ -1691,53 +1712,53 @@
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" t="s">
-        <v>161</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" t="s">
+        <v>167</v>
+      </c>
+      <c r="E14" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="1">
         <v>13</v>
       </c>
-      <c r="G13">
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="H13" s="1">
-        <f t="shared" si="0"/>
+      <c r="H14" s="1">
+        <f>G14*F14</f>
         <v>13</v>
-      </c>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="F14" s="1"/>
-      <c r="H14" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>157</v>
-      </c>
-      <c r="F15" s="1"/>
+        <v>173</v>
+      </c>
+      <c r="E15" t="s">
+        <v>218</v>
+      </c>
+      <c r="F15" s="1">
+        <v>20</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
       <c r="H15" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D16" t="s">
-        <v>176</v>
-      </c>
       <c r="F16" s="1"/>
       <c r="H16" s="1">
         <f t="shared" si="0"/>
@@ -1745,41 +1766,72 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F17" s="1"/>
-      <c r="H17" s="1"/>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>214</v>
+      </c>
+      <c r="D17" t="s">
+        <v>215</v>
+      </c>
+      <c r="E17" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="G17">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>8.02</v>
+      </c>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="F18" s="1"/>
-      <c r="H18" s="1"/>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="D18" t="s">
+        <v>216</v>
+      </c>
+      <c r="E18" t="s">
+        <v>217</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1.49</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.49</v>
+      </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
       <c r="F21" s="1"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C25" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F25" s="1">
         <v>25</v>
@@ -1791,10 +1843,13 @@
         <f>G25*F25</f>
         <v>25</v>
       </c>
+      <c r="J25" s="3" t="s">
+        <v>159</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J10" r:id="rId1" xr:uid="{D7F386F0-027E-4C87-B8D1-632360551444}"/>
+    <hyperlink ref="J25" r:id="rId1" xr:uid="{D7F386F0-027E-4C87-B8D1-632360551444}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2269,8 +2324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -2524,10 +2579,16 @@
       <c r="B26" t="s">
         <v>101</v>
       </c>
+      <c r="C26" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -2541,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C64E373-7692-4CBF-88B4-6ED8CB4BCA4C}">
   <dimension ref="A3:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2557,7 +2618,7 @@
   <sheetData>
     <row r="3" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
       <c r="B3" s="46" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C3" s="46"/>
       <c r="D3" s="46"/>
@@ -2575,13 +2636,13 @@
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C4">
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="K4" t="s">
         <v>25</v>
@@ -2595,13 +2656,13 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C5">
         <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="K5" t="s">
         <v>27</v>
@@ -2626,37 +2687,37 @@
     </row>
     <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="46" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B7" s="46"/>
       <c r="C7" s="46"/>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
@@ -2674,21 +2735,21 @@
     </row>
     <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="44" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B12" s="44" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C12" s="44" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D12" s="44" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2697,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="L13" t="s">
         <v>32</v>
@@ -2711,7 +2772,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B14">
         <f>C13+1</f>
@@ -2722,7 +2783,7 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J14" s="45" t="s">
         <v>40</v>
@@ -2745,7 +2806,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B15">
         <f t="shared" ref="B15:B27" si="0">C14+1</f>
@@ -2756,7 +2817,7 @@
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J15" s="45"/>
       <c r="K15" t="s">
@@ -2777,7 +2838,7 @@
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -2788,7 +2849,7 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J16" s="45"/>
       <c r="K16" t="s">
@@ -2809,7 +2870,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -2820,7 +2881,7 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="J17" s="45"/>
       <c r="K17" t="s">
@@ -2836,12 +2897,12 @@
         <v>4</v>
       </c>
       <c r="O17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -2852,7 +2913,7 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J18" s="45"/>
       <c r="K18" t="s">
@@ -2861,7 +2922,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -2872,7 +2933,7 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K19" t="s">
         <v>82</v>
@@ -2880,7 +2941,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
@@ -2891,7 +2952,7 @@
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K20" t="s">
         <v>83</v>
@@ -2902,7 +2963,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
@@ -2913,7 +2974,7 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="N21">
         <f>SUM(N14:N17)+LEN(L14)+LEN(L15)+LEN(L16)+LEN(L17)</f>
@@ -2922,7 +2983,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
@@ -2933,12 +2994,12 @@
         <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
@@ -2949,7 +3010,7 @@
         <v>43</v>
       </c>
       <c r="D23" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -2972,12 +3033,12 @@
         <v>51</v>
       </c>
       <c r="K25" s="45" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
@@ -2988,7 +3049,7 @@
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="K26" s="45"/>
     </row>
@@ -3121,7 +3182,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.0320212544080004E-2</v>
+        <v>1.0318069364450014E-2</v>
       </c>
       <c r="G6" t="s">
         <v>49</v>
@@ -3136,7 +3197,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>96.897229173214185</v>
+        <v>96.917355822922701</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
@@ -3148,18 +3209,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>7.2489681839992435E-3</v>
+        <v>1.0363329666874683E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>7.2489681839992435E-3</v>
+        <v>1.0363329666874683E-2</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-3.1027708267858146E-2</v>
+        <v>-3.0826441770772987E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3168,11 +3229,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0166062676671075E-2</v>
+        <v>2.3091727940016231E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.2917094492671831E-2</v>
+        <v>1.2728398273141548E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3181,11 +3242,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.3032356268755676E-2</v>
+        <v>3.043451298487165E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.2866293592084601E-2</v>
+        <v>7.342785044855419E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3194,11 +3255,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2352004049612861E-2</v>
+        <v>4.0184507481287934E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3196477808571848E-3</v>
+        <v>9.7499944964162845E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3207,11 +3268,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2455174761898961E-2</v>
+        <v>5.0069020673544691E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.01031707122861E-2</v>
+        <v>9.8845131922567567E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3220,11 +3281,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4664556648420898E-2</v>
+        <v>6.2248396758651681E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2209381886521938E-2</v>
+        <v>1.217937608510699E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3233,11 +3294,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3750400233650509E-2</v>
+        <v>7.4306631857063932E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.085843585229611E-3</v>
+        <v>1.2058235098412251E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3246,11 +3307,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2936458109248712E-2</v>
+        <v>8.5055113323021334E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1860578755982025E-3</v>
+        <v>1.0748481465957402E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3259,11 +3320,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3707732327467277E-2</v>
+        <v>9.3655983750694713E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0771274218218566E-2</v>
+        <v>8.6008704276733794E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3272,11 +3333,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10247471228120737</v>
+        <v>0.10262445219057113</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.766979953740095E-3</v>
+        <v>8.9684684398764203E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -3285,11 +3346,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11473688184256559</v>
+        <v>0.11234689109873543</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2262169561358213E-2</v>
+        <v>9.7224389081642937E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3298,11 +3359,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12276645806227254</v>
+        <v>0.12148273148361138</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0295762197069576E-3</v>
+        <v>9.1358403848759567E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3311,11 +3372,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1303470798913936</v>
+        <v>0.13417324957995375</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5806218291210592E-3</v>
+        <v>1.2690518096342362E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3324,11 +3385,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14047067354004875</v>
+        <v>0.14589375402719429</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0123593648655144E-2</v>
+        <v>1.1720504447240543E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3337,11 +3398,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15143655635793915</v>
+        <v>0.1567348360445453</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0965882817890404E-2</v>
+        <v>1.0841082017351011E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -3350,11 +3411,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16391569583856494</v>
+        <v>0.16689191394709177</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2479139480625789E-2</v>
+        <v>1.0157077902546469E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -3363,11 +3424,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17572168593112203</v>
+        <v>0.1776887559238545</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1805990092557089E-2</v>
+        <v>1.0796841976762728E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3376,11 +3437,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18610996535522017</v>
+        <v>0.18717646262361545</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0388279424098146E-2</v>
+        <v>9.487706699760956E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -3389,11 +3450,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19608403833752008</v>
+        <v>0.19604331792455026</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9740729822999086E-3</v>
+        <v>8.8668553009348117E-3</v>
       </c>
     </row>
   </sheetData>
@@ -7419,30 +7480,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B1">
         <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" t="s">
         <v>166</v>
       </c>
-      <c r="B3" t="s">
-        <v>167</v>
-      </c>
-      <c r="C3" t="s">
-        <v>169</v>
-      </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add header to create a library
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1C697945-4425-427F-8628-0E5BA3DA59CD}"/>
   <bookViews>
-    <workbookView xWindow="3924" yWindow="2232" windowWidth="15240" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="3924" yWindow="2232" windowWidth="15240" windowHeight="8964" firstSheet="1" activeTab="4" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat a faire" sheetId="1" r:id="rId1"/>
@@ -2324,7 +2324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -2602,7 +2602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C64E373-7692-4CBF-88B4-6ED8CB4BCA4C}">
   <dimension ref="A3:S29"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -3182,7 +3182,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.0318069364450014E-2</v>
+        <v>1.0214676635111204E-2</v>
       </c>
       <c r="G6" t="s">
         <v>49</v>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>96.917355822922701</v>
+        <v>97.898351139444884</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
@@ -3209,18 +3209,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>1.0363329666874683E-2</v>
+        <v>1.0798235222289865E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>1.0363329666874683E-2</v>
+        <v>1.0798235222289865E-2</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-3.0826441770772987E-2</v>
+        <v>-2.1016488605551161E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -3229,11 +3229,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.3091727940016231E-2</v>
+        <v>2.0743279411307689E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.2728398273141548E-2</v>
+        <v>9.9450441890178241E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -3242,11 +3242,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.043451298487165E-2</v>
+        <v>3.0916305199578373E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>7.342785044855419E-3</v>
+        <v>1.0173025788270684E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -3255,11 +3255,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0184507481287934E-2</v>
+        <v>4.0949386712800948E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7499944964162845E-3</v>
+        <v>1.0033081513222575E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -3268,11 +3268,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0069020673544691E-2</v>
+        <v>5.1549376536012055E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8845131922567567E-3</v>
+        <v>1.0599989823211108E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -3281,11 +3281,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2248396758651681E-2</v>
+        <v>6.1989987034671866E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.217937608510699E-2</v>
+        <v>1.0440610498659811E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -3294,11 +3294,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.4306631857063932E-2</v>
+        <v>7.4579303870795449E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2058235098412251E-2</v>
+        <v>1.2589316836123583E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -3307,11 +3307,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.5055113323021334E-2</v>
+        <v>8.3999527742175492E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0748481465957402E-2</v>
+        <v>9.4202238713800429E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -3320,11 +3320,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.3655983750694713E-2</v>
+        <v>9.1708932887110045E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6008704276733794E-3</v>
+        <v>7.709405144934553E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -3333,11 +3333,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10262445219057113</v>
+        <v>0.10118471894711333</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9684684398764203E-3</v>
+        <v>9.4757860600032801E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -3346,11 +3346,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11234689109873543</v>
+        <v>0.11314828595968046</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7224389081642937E-3</v>
+        <v>1.1963567012567136E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -3359,11 +3359,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12148273148361138</v>
+        <v>0.12108969957065843</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1358403848759567E-3</v>
+        <v>7.9414136109779709E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -3372,11 +3372,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13417324957995375</v>
+        <v>0.12840878392307808</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2690518096342362E-2</v>
+        <v>7.3190843524196525E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -3385,11 +3385,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14589375402719429</v>
+        <v>0.13634132462915621</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1720504447240543E-2</v>
+        <v>7.9325407060781283E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -3398,11 +3398,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1567348360445453</v>
+        <v>0.14721150266704586</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0841082017351011E-2</v>
+        <v>1.0870178037889644E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -3411,11 +3411,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16689191394709177</v>
+        <v>0.15929638582454173</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0157077902546469E-2</v>
+        <v>1.2084883157495868E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -3424,11 +3424,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1776887559238545</v>
+        <v>0.17035582424017148</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0796841976762728E-2</v>
+        <v>1.1059438415629758E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -3437,11 +3437,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18717646262361545</v>
+        <v>0.18227619785412977</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>9.487706699760956E-3</v>
+        <v>1.1920373613958285E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -3450,11 +3450,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19604331792455026</v>
+        <v>0.19407885606711286</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8668553009348117E-3</v>
+        <v>1.1802658212983097E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debut modification code principale
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="580" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD4BB472-C5A0-4A48-829D-470B3A7BEF1D}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="3324" windowWidth="15240" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="7800" yWindow="3324" windowWidth="15240" windowHeight="8964" firstSheet="1" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat a faire" sheetId="1" r:id="rId1"/>
@@ -1578,16 +1578,16 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -31677,7 +31677,7 @@
   <dimension ref="A2:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -31687,7 +31687,7 @@
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.109375" customWidth="1"/>
-    <col min="7" max="7" width="6.109375" style="89" customWidth="1"/>
+    <col min="7" max="7" width="6.109375" style="87" customWidth="1"/>
     <col min="8" max="8" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -31713,7 +31713,7 @@
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
       <c r="D3" s="29"/>
-      <c r="G3" s="89" t="s">
+      <c r="G3" s="87" t="s">
         <v>9</v>
       </c>
     </row>
@@ -31724,7 +31724,7 @@
       <c r="B4" s="20"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="87" t="s">
         <v>10</v>
       </c>
     </row>
@@ -31741,7 +31741,7 @@
       <c r="D5" s="17" t="s">
         <v>105</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="G5" s="87" t="s">
         <v>11</v>
       </c>
     </row>
@@ -31756,7 +31756,7 @@
       <c r="D6" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="89" t="s">
+      <c r="G6" s="87" t="s">
         <v>12</v>
       </c>
       <c r="H6" t="s">
@@ -31772,7 +31772,7 @@
       <c r="D7" s="17" t="s">
         <v>106</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="G7" s="87" t="s">
         <v>13</v>
       </c>
       <c r="H7" t="s">
@@ -31788,7 +31788,7 @@
       <c r="D8" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="89" t="s">
+      <c r="G8" s="87" t="s">
         <v>14</v>
       </c>
       <c r="H8" t="s">
@@ -31804,7 +31804,7 @@
         <v>36</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="G9" s="89" t="s">
+      <c r="G9" s="87" t="s">
         <v>257</v>
       </c>
     </row>
@@ -31819,7 +31819,7 @@
         <v>39</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="G10" s="89" t="s">
+      <c r="G10" s="87" t="s">
         <v>258</v>
       </c>
     </row>
@@ -31830,7 +31830,7 @@
       <c r="B11" s="21"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
-      <c r="G11" s="89" t="s">
+      <c r="G11" s="87" t="s">
         <v>259</v>
       </c>
     </row>
@@ -31843,7 +31843,7 @@
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
-      <c r="G12" s="89" t="s">
+      <c r="G12" s="87" t="s">
         <v>260</v>
       </c>
     </row>
@@ -31860,7 +31860,7 @@
       <c r="D13" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="87" t="s">
         <v>261</v>
       </c>
     </row>
@@ -31877,7 +31877,7 @@
       <c r="D14" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="89" t="s">
+      <c r="G14" s="87" t="s">
         <v>262</v>
       </c>
     </row>
@@ -31894,7 +31894,7 @@
       <c r="D15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="89" t="s">
+      <c r="G15" s="87" t="s">
         <v>263</v>
       </c>
     </row>
@@ -31911,7 +31911,7 @@
       <c r="D16" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="89" t="s">
+      <c r="G16" s="87" t="s">
         <v>264</v>
       </c>
     </row>
@@ -31920,7 +31920,7 @@
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="40"/>
-      <c r="G17" s="89" t="s">
+      <c r="G17" s="87" t="s">
         <v>265</v>
       </c>
     </row>
@@ -31931,7 +31931,7 @@
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
-      <c r="G18" s="89" t="s">
+      <c r="G18" s="87" t="s">
         <v>266</v>
       </c>
     </row>
@@ -31942,7 +31942,7 @@
       <c r="B19" s="20"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
-      <c r="G19" s="89" t="s">
+      <c r="G19" s="87" t="s">
         <v>267</v>
       </c>
     </row>
@@ -31969,7 +31969,7 @@
       <c r="D21" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="89">
+      <c r="G21" s="87">
         <v>1</v>
       </c>
     </row>
@@ -31980,7 +31980,7 @@
       <c r="B22" s="20"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17"/>
-      <c r="G22" s="89">
+      <c r="G22" s="87">
         <v>2</v>
       </c>
       <c r="H22" s="16" t="s">
@@ -31994,18 +31994,18 @@
       <c r="B23" s="22"/>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
-      <c r="G23" s="89">
+      <c r="G23" s="87">
         <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
-      <c r="G24" s="89">
+      <c r="G24" s="87">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G25" s="89">
+      <c r="G25" s="87">
         <v>5</v>
       </c>
     </row>
@@ -32019,7 +32019,7 @@
       <c r="C26" t="s">
         <v>171</v>
       </c>
-      <c r="G26" s="89">
+      <c r="G26" s="87">
         <v>6</v>
       </c>
     </row>
@@ -32030,22 +32030,22 @@
       <c r="C27" t="s">
         <v>172</v>
       </c>
-      <c r="G27" s="89">
+      <c r="G27" s="87">
         <v>7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G28" s="89">
+      <c r="G28" s="87">
         <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G29" s="89">
+      <c r="G29" s="87">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G30" s="89">
+      <c r="G30" s="87">
         <v>10</v>
       </c>
       <c r="H30" t="s">
@@ -32053,37 +32053,37 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G31" s="89">
+      <c r="G31" s="87">
         <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G32" s="89">
+      <c r="G32" s="87">
         <v>12</v>
       </c>
     </row>
     <row r="33" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G33" s="89">
+      <c r="G33" s="87">
         <v>13</v>
       </c>
     </row>
     <row r="34" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G34" s="89">
+      <c r="G34" s="87">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G35" s="89">
+      <c r="G35" s="87">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G36" s="89">
+      <c r="G36" s="87">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G37" s="89">
+      <c r="G37" s="87">
         <v>17</v>
       </c>
       <c r="H37" t="s">
@@ -32091,7 +32091,7 @@
       </c>
     </row>
     <row r="38" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G38" s="89">
+      <c r="G38" s="87">
         <v>18</v>
       </c>
       <c r="H38" t="s">
@@ -32099,7 +32099,7 @@
       </c>
     </row>
     <row r="39" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G39" s="89">
+      <c r="G39" s="87">
         <v>19</v>
       </c>
       <c r="H39" t="s">
@@ -32107,10 +32107,10 @@
       </c>
     </row>
     <row r="40" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G40" s="89">
+      <c r="G40" s="87">
         <v>20</v>
       </c>
-      <c r="H40" s="90" t="s">
+      <c r="H40" s="88" t="s">
         <v>275</v>
       </c>
       <c r="I40" t="s">
@@ -32118,155 +32118,155 @@
       </c>
     </row>
     <row r="41" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G41" s="89">
+      <c r="G41" s="87">
         <v>21</v>
       </c>
-      <c r="H41" s="90" t="s">
+      <c r="H41" s="88" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="42" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G42" s="89">
+      <c r="G42" s="87">
         <v>22</v>
       </c>
     </row>
     <row r="43" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G43" s="89">
+      <c r="G43" s="87">
         <v>23</v>
       </c>
     </row>
     <row r="44" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G44" s="89">
+      <c r="G44" s="87">
         <v>24</v>
       </c>
     </row>
     <row r="45" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G45" s="89">
+      <c r="G45" s="87">
         <v>25</v>
       </c>
     </row>
     <row r="46" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G46" s="89">
+      <c r="G46" s="87">
         <v>26</v>
       </c>
     </row>
     <row r="47" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G47" s="89">
+      <c r="G47" s="87">
         <v>27</v>
       </c>
     </row>
     <row r="48" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G48" s="89">
+      <c r="G48" s="87">
         <v>28</v>
       </c>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G49" s="89">
+      <c r="G49" s="87">
         <v>29</v>
       </c>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G50" s="89">
+      <c r="G50" s="87">
         <v>30</v>
       </c>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G51" s="89">
+      <c r="G51" s="87">
         <v>31</v>
       </c>
     </row>
     <row r="52" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G52" s="89">
+      <c r="G52" s="87">
         <v>32</v>
       </c>
     </row>
     <row r="53" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G53" s="89">
+      <c r="G53" s="87">
         <v>33</v>
       </c>
     </row>
     <row r="54" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G54" s="89">
+      <c r="G54" s="87">
         <v>34</v>
       </c>
     </row>
     <row r="55" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G55" s="89">
+      <c r="G55" s="87">
         <v>35</v>
       </c>
     </row>
     <row r="56" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G56" s="89">
+      <c r="G56" s="87">
         <v>36</v>
       </c>
     </row>
     <row r="57" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G57" s="89">
+      <c r="G57" s="87">
         <v>37</v>
       </c>
     </row>
     <row r="58" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G58" s="89">
+      <c r="G58" s="87">
         <v>38</v>
       </c>
     </row>
     <row r="59" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G59" s="89">
+      <c r="G59" s="87">
         <v>39</v>
       </c>
     </row>
     <row r="60" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G60" s="89">
+      <c r="G60" s="87">
         <v>40</v>
       </c>
     </row>
     <row r="61" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G61" s="89">
+      <c r="G61" s="87">
         <v>41</v>
       </c>
     </row>
     <row r="62" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G62" s="89">
+      <c r="G62" s="87">
         <v>42</v>
       </c>
     </row>
     <row r="63" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G63" s="89">
+      <c r="G63" s="87">
         <v>43</v>
       </c>
     </row>
     <row r="64" spans="7:7" x14ac:dyDescent="0.35">
-      <c r="G64" s="89">
+      <c r="G64" s="87">
         <v>44</v>
       </c>
     </row>
     <row r="65" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G65" s="89">
+      <c r="G65" s="87">
         <v>45</v>
       </c>
     </row>
     <row r="66" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G66" s="89">
+      <c r="G66" s="87">
         <v>46</v>
       </c>
     </row>
     <row r="67" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G67" s="89">
+      <c r="G67" s="87">
         <v>47</v>
       </c>
     </row>
     <row r="68" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G68" s="89">
+      <c r="G68" s="87">
         <v>48</v>
       </c>
     </row>
     <row r="69" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G69" s="89">
+      <c r="G69" s="87">
         <v>49</v>
       </c>
     </row>
     <row r="70" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G70" s="89">
+      <c r="G70" s="87">
         <v>50</v>
       </c>
       <c r="H70" t="s">
@@ -32274,7 +32274,7 @@
       </c>
     </row>
     <row r="71" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G71" s="89">
+      <c r="G71" s="87">
         <v>51</v>
       </c>
       <c r="H71" t="s">
@@ -32282,7 +32282,7 @@
       </c>
     </row>
     <row r="72" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G72" s="89">
+      <c r="G72" s="87">
         <v>52</v>
       </c>
       <c r="H72" t="s">
@@ -32290,12 +32290,12 @@
       </c>
     </row>
     <row r="73" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G73" s="89">
+      <c r="G73" s="87">
         <v>53</v>
       </c>
     </row>
     <row r="74" spans="7:8" x14ac:dyDescent="0.35">
-      <c r="G74" s="89">
+      <c r="G74" s="87">
         <v>54</v>
       </c>
     </row>
@@ -32325,13 +32325,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>176</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
       <c r="K3" s="4" t="s">
         <v>24</v>
       </c>
@@ -32394,11 +32394,11 @@
       </c>
     </row>
     <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="88" t="s">
+      <c r="A7" s="90" t="s">
         <v>185</v>
       </c>
-      <c r="B7" s="88"/>
-      <c r="C7" s="88"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="90"/>
       <c r="D7" t="s">
         <v>210</v>
       </c>
@@ -32508,7 +32508,7 @@
       <c r="G14" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="J14" s="87" t="s">
+      <c r="J14" s="89" t="s">
         <v>40</v>
       </c>
       <c r="K14" t="s">
@@ -32542,7 +32542,7 @@
       <c r="D15" t="s">
         <v>194</v>
       </c>
-      <c r="J15" s="87"/>
+      <c r="J15" s="89"/>
       <c r="K15" t="s">
         <v>34</v>
       </c>
@@ -32574,7 +32574,7 @@
       <c r="D16" t="s">
         <v>197</v>
       </c>
-      <c r="J16" s="87"/>
+      <c r="J16" s="89"/>
       <c r="K16" t="s">
         <v>81</v>
       </c>
@@ -32606,7 +32606,7 @@
       <c r="D17" t="s">
         <v>197</v>
       </c>
-      <c r="J17" s="87"/>
+      <c r="J17" s="89"/>
       <c r="K17" t="s">
         <v>35</v>
       </c>
@@ -32638,7 +32638,7 @@
       <c r="D18" t="s">
         <v>200</v>
       </c>
-      <c r="J18" s="87"/>
+      <c r="J18" s="89"/>
       <c r="K18" t="s">
         <v>80</v>
       </c>
@@ -32755,7 +32755,7 @@
         <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="K25" s="87" t="s">
+      <c r="K25" s="89" t="s">
         <v>175</v>
       </c>
     </row>
@@ -32774,7 +32774,7 @@
       <c r="D26" t="s">
         <v>211</v>
       </c>
-      <c r="K26" s="87"/>
+      <c r="K26" s="89"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -32788,13 +32788,13 @@
         <f t="shared" si="1"/>
         <v>59</v>
       </c>
-      <c r="K27" s="87"/>
+      <c r="K27" s="89"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K28" s="87"/>
+      <c r="K28" s="89"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K29" s="87"/>
+      <c r="K29" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -32908,7 +32908,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.0352551792847858E-2</v>
+        <v>1.0787916392060205E-2</v>
       </c>
       <c r="G6" t="s">
         <v>49</v>
@@ -32923,7 +32923,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>96.594542100321377</v>
+        <v>92.696306094473414</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
@@ -32935,18 +32935,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>7.2074704134743196E-3</v>
+        <v>1.2303014081487625E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>7.2074704134743196E-3</v>
+        <v>1.2303014081487625E-2</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-3.4054578996786232E-2</v>
+        <v>-7.3036939055265857E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -32955,11 +32955,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7820630280110765E-2</v>
+        <v>2.4699063770361081E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.0613159866636445E-2</v>
+        <v>1.2396049688873456E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -32968,11 +32968,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0817672648950915E-2</v>
+        <v>3.2544779911512618E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.299704236884015E-2</v>
+        <v>7.8457161411515375E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -32981,11 +32981,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1058606305057151E-2</v>
+        <v>4.1312418461255933E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0240933656106236E-2</v>
+        <v>8.7676385497433146E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -32994,11 +32994,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1662060524272385E-2</v>
+        <v>5.216503885700384E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0603454219215235E-2</v>
+        <v>1.0852620395747907E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -33007,11 +33007,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1035316521562674E-2</v>
+        <v>6.445905439288184E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.373255997290289E-3</v>
+        <v>1.2294015535878E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -33020,11 +33020,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3618079772825543E-2</v>
+        <v>7.4021969866322784E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2582763251262868E-2</v>
+        <v>9.5629154734409444E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33033,11 +33033,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2668465354426221E-2</v>
+        <v>8.6558036911726588E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>9.0503855816006784E-3</v>
+        <v>1.2536067045403804E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -33046,11 +33046,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9858552925422788E-2</v>
+        <v>9.6962436025597523E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1900875709965673E-3</v>
+        <v>1.0404399113870935E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -33059,11 +33059,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10282967408457397</v>
+        <v>0.1051320072445472</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.297112115915118E-2</v>
+        <v>8.1695712189496783E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -33072,11 +33072,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11034698235980497</v>
+        <v>0.11369978335163825</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.517308275231005E-3</v>
+        <v>8.5677761070910435E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -33085,11 +33085,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12185613360341653</v>
+        <v>0.1243101345273718</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1509151243611557E-2</v>
+        <v>1.0610351175733557E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -33098,11 +33098,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1345643351820805</v>
+        <v>0.13396033582676142</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2708201578663966E-2</v>
+        <v>9.6502012993896213E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -33111,11 +33111,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1459852956080876</v>
+        <v>0.14686050733311476</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1420960426007098E-2</v>
+        <v>1.2900171506353336E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -33124,11 +33124,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15547688353854958</v>
+        <v>0.15633576872859523</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>9.491587930461981E-3</v>
+        <v>9.4752613954804665E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -33137,11 +33137,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16349091783092493</v>
+        <v>0.16854793038301677</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0140342923753494E-3</v>
+        <v>1.2212161654421544E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -33150,11 +33150,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17378110998433066</v>
+        <v>0.18135567129654717</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0290192153405736E-2</v>
+        <v>1.2807740913530402E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -33163,11 +33163,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18547577362339407</v>
+        <v>0.19397912321328886</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1694663639063407E-2</v>
+        <v>1.262345191674169E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -33176,11 +33176,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19669848406410931</v>
+        <v>0.20497041144914391</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1222710440715239E-2</v>
+        <v>1.0991288235855046E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
function for batteryLevel and wind speed
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/192d16467d0539cb/Documents/5.Bricolage/5.StationMeteo/StationMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6B7F110C-B5AA-4935-92D8-4FDFA7EBDF16}"/>
+  <xr:revisionPtr revIDLastSave="595" documentId="13_ncr:1_{49D4E897-6CFC-4372-BC7E-4324AD2FDE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0A905B60-7ED1-4575-AE3A-B5B7858F5AA1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat a faire" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="280">
   <si>
     <t>Produit</t>
   </si>
@@ -917,6 +917,9 @@
   </si>
   <si>
     <t>DS18B20</t>
+  </si>
+  <si>
+    <t>ref 3V3 du BME</t>
   </si>
 </sst>
 </file>
@@ -33649,8 +33652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:I74"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -33779,6 +33782,9 @@
       <c r="D9" s="17"/>
       <c r="G9" s="87" t="s">
         <v>257</v>
+      </c>
+      <c r="H9" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -34881,7 +34887,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.949415008538548E-3</v>
+        <v>9.9513062848477097E-3</v>
       </c>
       <c r="G6" t="s">
         <v>49</v>
@@ -34896,7 +34902,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>100.5084217656821</v>
+        <v>100.4893198315726</v>
       </c>
       <c r="G7" t="s">
         <v>47</v>
@@ -34908,18 +34914,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>8.4684453329703594E-3</v>
+        <v>7.3870317791040561E-3</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>8.4684453329703594E-3</v>
+        <v>7.3870317791040561E-3</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>5.084217656821011E-3</v>
+        <v>4.893198315726011E-3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -34928,11 +34934,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.111678096128336E-2</v>
+        <v>1.4913853720893898E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.2648335628313001E-2</v>
+        <v>7.5268219417898418E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -34941,11 +34947,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2488148831591117E-2</v>
+        <v>2.5861292412549926E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.1371367870307757E-2</v>
+        <v>1.0947438691656028E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -34954,11 +34960,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0130542254254033E-2</v>
+        <v>3.5917839888635415E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6423934226629159E-3</v>
+        <v>1.0056547476085489E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -34967,11 +34973,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7824137780423645E-2</v>
+        <v>4.721618110971397E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6935955261696123E-3</v>
+        <v>1.1298341221078555E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -34980,11 +34986,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7277348096541766E-2</v>
+        <v>6.0186935203701421E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4532103161181213E-3</v>
+        <v>1.2970754093987451E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -34993,11 +34999,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9360639638281443E-2</v>
+        <v>7.2993736415432234E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2083291541739677E-2</v>
+        <v>1.2806801211730813E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -35006,11 +35012,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7909502935660679E-2</v>
+        <v>8.1930150984270422E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>8.5488632973792361E-3</v>
+        <v>8.9364145688381885E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -35019,11 +35025,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6665713444741749E-2</v>
+        <v>9.1875706355069808E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7562105090810693E-3</v>
+        <v>9.945555370799386E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -35032,11 +35038,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.4784712740401747E-2</v>
+        <v>0.10349301279324301</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1189992956599982E-3</v>
+        <v>1.16173064381732E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -35045,11 +35051,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10235501095773231</v>
+        <v>0.11090726053205326</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5702982173305594E-3</v>
+        <v>7.4142477388102479E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -35058,11 +35064,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1103828843933868</v>
+        <v>0.12338628823272681</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0278734356544895E-3</v>
+        <v>1.2479027700673551E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -35071,11 +35077,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1193792566247352</v>
+        <v>0.13179539583690508</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9963722313484012E-3</v>
+        <v>8.4091076041782759E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -35084,11 +35090,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13212296072094259</v>
+        <v>0.14382761581588852</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2743704096207398E-2</v>
+        <v>1.2032219978983433E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -35097,11 +35103,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14479062520578853</v>
+        <v>0.15159814445553349</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2667664484845936E-2</v>
+        <v>7.7705286396449746E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -35110,11 +35116,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15547344707225816</v>
+        <v>0.16253883728518614</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0682821866469627E-2</v>
+        <v>1.0940692829652654E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -35123,11 +35129,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16441894606032656</v>
+        <v>0.17150415354773396</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>8.945498988068401E-3</v>
+        <v>8.9653162625478178E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -35136,11 +35142,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17631721867530012</v>
+        <v>0.18004435886928849</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.189827261497356E-2</v>
+        <v>8.5402053215545282E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -35149,11 +35155,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18903888516223241</v>
+        <v>0.18907481941210649</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2721666486932293E-2</v>
+        <v>9.0304605428180029E-3</v>
       </c>
     </row>
   </sheetData>
@@ -35165,7 +35171,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7DA879-7295-4B28-AB1F-AC4478E5196C}">
   <dimension ref="A2:S58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
réorganisation du dossier + nouveau capteur
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EFD74C-D2EE-4D08-8E3E-7BAC17C945B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFBCD2D-DF38-4ECF-B49F-B2B1C4A385F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="6696" yWindow="2784" windowWidth="17280" windowHeight="8964" firstSheet="5" activeTab="6" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste grandeur" sheetId="15" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="276">
   <si>
     <t>Produit</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>Bus I2C</t>
-  </si>
-  <si>
-    <t>Pression</t>
   </si>
   <si>
     <t>Humidité</t>
@@ -506,37 +503,10 @@
     <t>vitesse vent</t>
   </si>
   <si>
-    <t>Temperature (DS18B20)</t>
-  </si>
-  <si>
-    <t>Temperature (BME280)</t>
-  </si>
-  <si>
-    <t>Humidité (BME280)</t>
-  </si>
-  <si>
-    <t>Pression (BME280)</t>
-  </si>
-  <si>
-    <t>Luminosité UV</t>
-  </si>
-  <si>
-    <t>Luminosité Visible</t>
-  </si>
-  <si>
-    <t>Luminosité IR</t>
-  </si>
-  <si>
-    <t>Altitude (BME280)</t>
-  </si>
-  <si>
     <t>m</t>
   </si>
   <si>
     <t>idem pour unsigned int</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
   <si>
     <t>antenne</t>
@@ -636,21 +606,6 @@
     <t>Vitesse vent</t>
   </si>
   <si>
-    <t>temp DS18</t>
-  </si>
-  <si>
-    <t>temp BME</t>
-  </si>
-  <si>
-    <t>Light UV</t>
-  </si>
-  <si>
-    <t>Light visible</t>
-  </si>
-  <si>
-    <t>Light IR</t>
-  </si>
-  <si>
     <t>battery temp</t>
   </si>
   <si>
@@ -717,13 +672,7 @@
     <t>Temp  °C</t>
   </si>
   <si>
-    <t>Temp °C</t>
-  </si>
-  <si>
     <t>Pression Pa</t>
-  </si>
-  <si>
-    <t>indexUV</t>
   </si>
   <si>
     <t>V</t>
@@ -920,6 +869,48 @@
   <si>
     <t>Bat T+V</t>
   </si>
+  <si>
+    <t>tempDHT22</t>
+  </si>
+  <si>
+    <t>HumiditéDHT22</t>
+  </si>
+  <si>
+    <t>TempBMP280</t>
+  </si>
+  <si>
+    <t>PressionBMP</t>
+  </si>
+  <si>
+    <t>Luminosité</t>
+  </si>
+  <si>
+    <t>Temperature (DHT22)</t>
+  </si>
+  <si>
+    <t>Humidité (DHT22)</t>
+  </si>
+  <si>
+    <t>Température (BMP280)</t>
+  </si>
+  <si>
+    <t>Pression (BMP280)</t>
+  </si>
+  <si>
+    <t>Luminosité BH1745</t>
+  </si>
+  <si>
+    <t>Lux</t>
+  </si>
+  <si>
+    <t>DewPoint</t>
+  </si>
+  <si>
+    <t>Icing point</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
 </sst>
 </file>
 
@@ -929,7 +920,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000000E+00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1035,6 +1026,13 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1403,7 +1401,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1518,6 +1516,14 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1533,14 +1539,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -12111,7 +12110,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="7886700" y="213360"/>
+          <a:off x="7612380" y="327660"/>
           <a:ext cx="1577340" cy="3002280"/>
           <a:chOff x="487680" y="266700"/>
           <a:chExt cx="1577340" cy="3002280"/>
@@ -15915,10 +15914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526E76B6-68A2-48DF-95E8-365FAB976DDF}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15928,10 +15927,10 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D2" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
@@ -15939,65 +15938,68 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D5" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>183</v>
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>184</v>
+        <v>262</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>185</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>59</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>187</v>
+        <v>266</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>190</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -16031,7 +16033,7 @@
         <v>41</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>40</v>
@@ -16667,7 +16669,7 @@
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O22" s="7" t="str">
         <f>_xlfn.CONCAT("if(WindAngle &lt; ",K22+5, ") return(""",M22,""");")</f>
@@ -16695,7 +16697,7 @@
         <v>22.5</v>
       </c>
       <c r="M23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O23" s="7" t="str">
         <f t="shared" ref="O23:O37" si="13">_xlfn.CONCAT("if(WindAngle &lt; ",K23+5, ") return(""",M23,""");")</f>
@@ -16723,7 +16725,7 @@
         <v>45</v>
       </c>
       <c r="M24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O24" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16751,7 +16753,7 @@
         <v>67.5</v>
       </c>
       <c r="M25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O25" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16779,7 +16781,7 @@
         <v>90</v>
       </c>
       <c r="M26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O26" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16807,7 +16809,7 @@
         <v>112.5</v>
       </c>
       <c r="M27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O27" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16835,7 +16837,7 @@
         <v>135</v>
       </c>
       <c r="M28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O28" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16863,7 +16865,7 @@
         <v>157.5</v>
       </c>
       <c r="M29" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O29" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16891,7 +16893,7 @@
         <v>180</v>
       </c>
       <c r="M30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O30" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16919,7 +16921,7 @@
         <v>202.5</v>
       </c>
       <c r="M31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O31" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16947,7 +16949,7 @@
         <v>225</v>
       </c>
       <c r="M32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O32" s="7" t="str">
         <f t="shared" si="13"/>
@@ -16975,7 +16977,7 @@
         <v>247.5</v>
       </c>
       <c r="M33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O33" s="7" t="str">
         <f t="shared" si="13"/>
@@ -17003,7 +17005,7 @@
         <v>270</v>
       </c>
       <c r="M34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O34" s="7" t="str">
         <f t="shared" si="13"/>
@@ -17031,7 +17033,7 @@
         <v>292.5</v>
       </c>
       <c r="M35" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O35" s="7" t="str">
         <f t="shared" si="13"/>
@@ -17059,7 +17061,7 @@
         <v>315</v>
       </c>
       <c r="M36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O36" s="7" t="str">
         <f t="shared" si="13"/>
@@ -17087,7 +17089,7 @@
         <v>337.5</v>
       </c>
       <c r="M37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="O37" s="7" t="str">
         <f t="shared" si="13"/>
@@ -17101,10 +17103,10 @@
     </row>
     <row r="42" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42" s="13" t="s">
         <v>62</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
@@ -17422,30 +17424,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B1">
         <v>80</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
         <v>121</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D3" t="s">
         <v>122</v>
       </c>
-      <c r="C3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" t="s">
-        <v>123</v>
-      </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -17871,30 +17873,30 @@
   <sheetData>
     <row r="1" spans="1:18" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="C1" s="45" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="D1" s="46"/>
       <c r="F1" s="48" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="G1" s="49"/>
       <c r="H1" s="46" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="J1" s="47" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="K1" s="47" t="s">
         <v>38</v>
       </c>
       <c r="L1" s="47" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="N1" s="50"/>
       <c r="O1" s="50"/>
@@ -27095,21 +27097,21 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="68" t="s">
-        <v>202</v>
-      </c>
-      <c r="C2" s="68"/>
+      <c r="B2" s="72" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="72"/>
       <c r="D2" s="64">
         <f>SUM(D5:D19)</f>
         <v>487.51</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="65"/>
-      <c r="G2" s="68" t="s">
-        <v>204</v>
-      </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="G2" s="72" t="s">
+        <v>189</v>
+      </c>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
       <c r="J2" s="64">
         <f>SUM(J5:J19)</f>
         <v>0</v>
@@ -27120,30 +27122,30 @@
     </row>
     <row r="4" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" t="s">
         <v>108</v>
-      </c>
-      <c r="C5" t="s">
-        <v>109</v>
       </c>
       <c r="D5" s="1">
         <v>163.81</v>
@@ -27156,7 +27158,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="1">
         <v>2.72</v>
@@ -27169,7 +27171,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1">
         <v>6.69</v>
@@ -27183,7 +27185,7 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D8" s="1">
         <v>2.35</v>
@@ -27196,7 +27198,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D9" s="1">
         <v>3.7</v>
@@ -27209,7 +27211,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1">
         <v>6.99</v>
@@ -27222,7 +27224,7 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D11" s="1">
         <v>40.76</v>
@@ -27235,7 +27237,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D12" s="1">
         <v>7.99</v>
@@ -27248,7 +27250,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="1">
         <v>8.99</v>
@@ -27258,10 +27260,10 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="D14" s="1">
         <v>13</v>
@@ -27270,10 +27272,10 @@
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -27282,10 +27284,10 @@
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D16" s="1">
         <v>8.02</v>
@@ -27295,10 +27297,10 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1">
         <v>1.49</v>
@@ -27311,7 +27313,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>181</v>
       </c>
       <c r="D18" s="1">
         <v>57</v>
@@ -27321,10 +27323,10 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
       <c r="D19" s="1">
         <v>144</v>
@@ -27375,25 +27377,25 @@
   <sheetData>
     <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3">
         <f>SUMPRODUCT(B11:B17,F11:F17)*3600/1000</f>
         <v>157.5</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G3" s="7">
         <f>B5/(B3-B4)</f>
@@ -27402,17 +27404,17 @@
     </row>
     <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4">
         <f>D27</f>
         <v>129.6</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G4" s="7">
         <f>G3/24</f>
@@ -27421,17 +27423,17 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5">
         <f>E20</f>
         <v>180</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="7">
         <f>G4/365</f>
@@ -27440,29 +27442,29 @@
     </row>
     <row r="8" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E10" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C10" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>85</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -27515,7 +27517,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B16" s="60">
         <f>SUMPRODUCT(B11:B15,F11:F15)*0.05</f>
@@ -27534,19 +27536,19 @@
     </row>
     <row r="19" spans="1:5" ht="44.4" x14ac:dyDescent="0.4">
       <c r="A19" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>95</v>
+      </c>
+      <c r="D19" t="s">
         <v>87</v>
       </c>
-      <c r="C19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -27574,23 +27576,23 @@
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.4">
       <c r="A25" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C26" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D26" t="s">
         <v>100</v>
-      </c>
-      <c r="D26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27">
         <v>6</v>
@@ -27613,289 +27615,391 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D1C501-6ABF-4FF7-B1E1-C49F27E96A4F}">
   <dimension ref="B1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="3" width="17.77734375" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
-        <v>269</v>
-      </c>
-      <c r="C1" t="s">
-        <v>270</v>
-      </c>
-      <c r="D1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F1" t="s">
-        <v>262</v>
+    <row r="1" spans="2:6" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="77" t="s">
+        <v>252</v>
+      </c>
+      <c r="C1" s="77" t="s">
+        <v>253</v>
+      </c>
+      <c r="D1" s="77" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1" s="77" t="s">
+        <v>244</v>
+      </c>
+      <c r="F1" s="77" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C2" t="s">
-        <v>271</v>
-      </c>
-      <c r="D2" t="s">
-        <v>265</v>
+      <c r="B2" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C2" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="D2" s="73" t="s">
+        <v>248</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
       <c r="E3">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
       <c r="E4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>264</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>263</v>
-      </c>
-      <c r="C6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" t="s">
-        <v>222</v>
+      <c r="B6" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C6" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>205</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
       <c r="E7">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
       <c r="E8">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>263</v>
-      </c>
-      <c r="C9" t="s">
-        <v>271</v>
-      </c>
-      <c r="D9" t="s">
-        <v>266</v>
+      <c r="B9" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C9" s="73" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>249</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
       <c r="E10">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
       <c r="E11">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
       <c r="E12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>263</v>
-      </c>
-      <c r="C13" t="s">
-        <v>272</v>
-      </c>
-      <c r="D13" t="s">
-        <v>267</v>
+      <c r="B13" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C13" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>250</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
       <c r="E14">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
       <c r="E15">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="73"/>
+      <c r="C16" s="73"/>
+      <c r="D16" s="73"/>
       <c r="E16">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>263</v>
-      </c>
-      <c r="C17" t="s">
-        <v>272</v>
-      </c>
-      <c r="D17" t="s">
-        <v>182</v>
+      <c r="B17" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>172</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="73"/>
+      <c r="C18" s="73"/>
+      <c r="D18" s="73"/>
       <c r="E18">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>263</v>
-      </c>
-      <c r="C19" t="s">
-        <v>272</v>
-      </c>
-      <c r="D19" t="s">
-        <v>238</v>
+      <c r="B19" s="73" t="s">
+        <v>246</v>
+      </c>
+      <c r="C19" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>221</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="73"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
       <c r="E20">
         <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
       <c r="E21">
         <v>3</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>268</v>
-      </c>
-      <c r="C22" t="s">
-        <v>273</v>
-      </c>
-      <c r="D22" t="s">
-        <v>274</v>
+      <c r="B22" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="C22" s="73" t="s">
+        <v>256</v>
+      </c>
+      <c r="D22" s="73" t="s">
+        <v>257</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="73"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="73"/>
       <c r="E23">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
       <c r="E24">
         <v>3</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B25" s="73"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="73"/>
       <c r="E25">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="73"/>
+      <c r="C26" s="73"/>
+      <c r="D26" s="73"/>
       <c r="E26">
         <v>5</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
-        <v>268</v>
-      </c>
-      <c r="C27" t="s">
-        <v>273</v>
-      </c>
-      <c r="D27" t="s">
-        <v>275</v>
+      <c r="B27" s="73" t="s">
+        <v>251</v>
+      </c>
+      <c r="C27" s="73" t="s">
+        <v>256</v>
+      </c>
+      <c r="D27" s="73" t="s">
+        <v>258</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="73"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="73"/>
       <c r="E28">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="73"/>
+      <c r="C29" s="73"/>
+      <c r="D29" s="73"/>
       <c r="E29">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>272</v>
-      </c>
-      <c r="C30" t="s">
-        <v>276</v>
-      </c>
-      <c r="D30" t="s">
-        <v>277</v>
+      <c r="B30" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="C30" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="D30" s="73" t="s">
+        <v>260</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B31" s="73"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
       <c r="E31">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>272</v>
-      </c>
-      <c r="C32" t="s">
-        <v>276</v>
-      </c>
-      <c r="D32" t="s">
-        <v>278</v>
+      <c r="B32" s="73" t="s">
+        <v>255</v>
+      </c>
+      <c r="C32" s="73" t="s">
+        <v>259</v>
+      </c>
+      <c r="D32" s="73" t="s">
+        <v>261</v>
       </c>
       <c r="E32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" s="73"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="73"/>
       <c r="E33">
         <v>2</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="D27:D29"/>
+    <mergeCell ref="D22:D26"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D13:D16"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -27903,7 +28007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="B7" workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -27913,7 +28017,7 @@
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="73"/>
+    <col min="7" max="7" width="11.5546875" style="68"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.4">
@@ -27925,10 +28029,10 @@
         <v>11</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H2" s="67" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
@@ -27938,17 +28042,17 @@
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
       <c r="D3" s="29"/>
-      <c r="G3" s="74">
+      <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="69" t="s">
-        <v>182</v>
+      <c r="J3" s="73" t="s">
+        <v>172</v>
       </c>
       <c r="K3" t="s">
-        <v>252</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>253</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
@@ -27958,15 +28062,15 @@
       <c r="B4" s="20"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
-      <c r="G4" s="74">
+      <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="69"/>
+      <c r="J4" s="73"/>
       <c r="K4" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="L4" t="s">
-        <v>256</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
@@ -27980,20 +28084,20 @@
         <v>17</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="G5" s="74">
+        <v>75</v>
+      </c>
+      <c r="G5" s="69">
         <v>2</v>
       </c>
       <c r="H5" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="69"/>
+      <c r="J5" s="73"/>
       <c r="K5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="L5" t="s">
-        <v>255</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
@@ -28007,18 +28111,18 @@
       <c r="D6" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="69">
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" s="69"/>
+        <v>75</v>
+      </c>
+      <c r="J6" s="73"/>
       <c r="K6" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="L6" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -28028,13 +28132,13 @@
       <c r="B7" s="21"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="74">
+        <v>76</v>
+      </c>
+      <c r="G7" s="69">
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>251</v>
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -28046,11 +28150,11 @@
       <c r="D8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="74">
+      <c r="G8" s="69">
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -28062,7 +28166,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="G9" s="74">
+      <c r="G9" s="69">
         <v>6</v>
       </c>
     </row>
@@ -28071,13 +28175,13 @@
         <v>7</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="17"/>
-      <c r="G10" s="74">
+      <c r="G10" s="69">
         <v>7</v>
       </c>
     </row>
@@ -28088,7 +28192,7 @@
       <c r="B11" s="21"/>
       <c r="C11" s="16"/>
       <c r="D11" s="17"/>
-      <c r="G11" s="74">
+      <c r="G11" s="69">
         <v>8</v>
       </c>
     </row>
@@ -28101,7 +28205,7 @@
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="17"/>
-      <c r="G12" s="74">
+      <c r="G12" s="69">
         <v>9</v>
       </c>
     </row>
@@ -28118,7 +28222,7 @@
       <c r="D13" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="74">
+      <c r="G13" s="69">
         <v>10</v>
       </c>
       <c r="H13" t="s">
@@ -28138,11 +28242,11 @@
       <c r="D14" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="74">
+      <c r="G14" s="69">
         <v>11</v>
       </c>
       <c r="H14" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -28158,11 +28262,11 @@
       <c r="D15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="74">
+      <c r="G15" s="69">
         <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -28178,11 +28282,11 @@
       <c r="D16" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="74">
+      <c r="G16" s="69">
         <v>13</v>
       </c>
       <c r="H16" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -28190,7 +28294,7 @@
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="40"/>
-      <c r="G17" s="74"/>
+      <c r="G17" s="69"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="37" t="s">
@@ -28199,7 +28303,7 @@
       <c r="B18" s="27"/>
       <c r="C18" s="28"/>
       <c r="D18" s="29"/>
-      <c r="G18" s="75" t="s">
+      <c r="G18" s="70" t="s">
         <v>5</v>
       </c>
     </row>
@@ -28210,7 +28314,7 @@
       <c r="B19" s="20"/>
       <c r="C19" s="16"/>
       <c r="D19" s="17"/>
-      <c r="G19" s="75" t="s">
+      <c r="G19" s="70" t="s">
         <v>6</v>
       </c>
     </row>
@@ -28223,11 +28327,11 @@
       </c>
       <c r="C20" s="16"/>
       <c r="D20" s="17"/>
-      <c r="G20" s="75" t="s">
+      <c r="G20" s="70" t="s">
         <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -28243,11 +28347,11 @@
       <c r="D21" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="75" t="s">
+      <c r="G21" s="70" t="s">
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -28257,11 +28361,11 @@
       <c r="B22" s="20"/>
       <c r="C22" s="16"/>
       <c r="D22" s="17"/>
-      <c r="G22" s="75" t="s">
+      <c r="G22" s="70" t="s">
         <v>9</v>
       </c>
       <c r="H22" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -28271,28 +28375,28 @@
       <c r="B23" s="22"/>
       <c r="C23" s="18"/>
       <c r="D23" s="19"/>
-      <c r="G23" s="75" t="s">
+      <c r="G23" s="70" t="s">
         <v>10</v>
       </c>
       <c r="H23" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
-      <c r="G24" s="76" t="s">
-        <v>175</v>
+      <c r="G24" s="71" t="s">
+        <v>165</v>
       </c>
       <c r="H24" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G25" s="76" t="s">
-        <v>176</v>
+      <c r="G25" s="71" t="s">
+        <v>166</v>
       </c>
       <c r="H25" t="s">
-        <v>259</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -28300,18 +28404,18 @@
         <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -28344,16 +28448,16 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="15" t="s">
-        <v>216</v>
+        <v>199</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>217</v>
+        <v>200</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>219</v>
+        <v>202</v>
       </c>
       <c r="E1" s="15"/>
       <c r="F1" s="15" t="s">
@@ -28361,33 +28465,33 @@
       </c>
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
-      <c r="I1" s="70" t="s">
-        <v>233</v>
-      </c>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
+      <c r="I1" s="74" t="s">
+        <v>216</v>
+      </c>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="C2">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>221</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="69" t="s">
-        <v>238</v>
+      <c r="I2" s="73" t="s">
+        <v>221</v>
       </c>
       <c r="J2" s="59" t="s">
-        <v>234</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -28395,20 +28499,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" s="59" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="69"/>
+      <c r="I3" s="73"/>
       <c r="J3" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -28416,22 +28520,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="D4" s="59" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="F4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="69" t="s">
-        <v>239</v>
+      <c r="I4" s="73" t="s">
+        <v>222</v>
       </c>
       <c r="J4" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -28439,20 +28543,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" s="59" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="69"/>
+      <c r="I5" s="73"/>
       <c r="J5" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -28460,22 +28564,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
       <c r="F6" t="s">
-        <v>228</v>
-      </c>
-      <c r="I6" s="69" t="s">
-        <v>227</v>
+        <v>211</v>
+      </c>
+      <c r="I6" s="73" t="s">
+        <v>210</v>
       </c>
       <c r="J6" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -28483,20 +28587,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" s="59" t="s">
-        <v>230</v>
+        <v>213</v>
       </c>
       <c r="F7" t="s">
-        <v>228</v>
-      </c>
-      <c r="I7" s="69"/>
+        <v>211</v>
+      </c>
+      <c r="I7" s="73"/>
       <c r="J7" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -28504,20 +28608,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>231</v>
+        <v>214</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" s="59" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="F8" t="s">
-        <v>232</v>
-      </c>
-      <c r="I8" s="69"/>
+        <v>215</v>
+      </c>
+      <c r="I8" s="73"/>
       <c r="J8" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -28525,40 +28629,40 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C9">
         <v>4</v>
       </c>
       <c r="D9" s="59" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="F9" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="69"/>
+        <v>71</v>
+      </c>
+      <c r="I9" s="73"/>
       <c r="J9" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I10" s="69" t="s">
-        <v>243</v>
+      <c r="I10" s="73" t="s">
+        <v>226</v>
       </c>
       <c r="J10" t="s">
-        <v>240</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11" s="69"/>
+      <c r="I11" s="73"/>
       <c r="J11" t="s">
-        <v>241</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12" s="69"/>
+      <c r="I12" s="73"/>
       <c r="J12" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -28577,10 +28681,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C64E373-7692-4CBF-88B4-6ED8CB4BCA4C}">
-  <dimension ref="A3:L29"/>
+  <dimension ref="A3:L28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:S9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -28594,26 +28698,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
+      <c r="B3" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
       <c r="K3" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4">
         <v>62</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K4" t="s">
         <v>21</v>
@@ -28624,13 +28728,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C5">
         <v>61</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K5" t="s">
         <v>23</v>
@@ -28648,38 +28752,38 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="72" t="s">
-        <v>138</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
+      <c r="A7" s="76" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
       <c r="D7" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B9">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="18" x14ac:dyDescent="0.35">
@@ -28687,24 +28791,24 @@
     </row>
     <row r="12" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B12" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>134</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="D12" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="D12" s="42" t="s">
-        <v>136</v>
-      </c>
       <c r="F12" s="42" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -28713,18 +28817,18 @@
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="F13" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="G13" s="59" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B14">
         <f>C13+1</f>
@@ -28735,36 +28839,36 @@
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="F14" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="G14" s="59" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="J14" s="66"/>
     </row>
     <row r="15" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:B27" si="0">C14+1</f>
+        <f t="shared" ref="B15:B26" si="0">C14+1</f>
         <v>8</v>
       </c>
       <c r="C15">
-        <f t="shared" ref="C15:C27" si="1">B15+3</f>
+        <f t="shared" ref="C15:C26" si="1">B15+3</f>
         <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="J15" s="66"/>
     </row>
     <row r="16" spans="1:12" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>146</v>
+        <v>267</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
@@ -28775,13 +28879,13 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="J16" s="66"/>
     </row>
     <row r="17" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>147</v>
+        <v>268</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
@@ -28792,13 +28896,13 @@
         <v>19</v>
       </c>
       <c r="D17" t="s">
-        <v>211</v>
+        <v>59</v>
       </c>
       <c r="J17" s="66"/>
     </row>
     <row r="18" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>269</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
@@ -28809,13 +28913,13 @@
         <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>195</v>
       </c>
       <c r="J18" s="66"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>149</v>
+        <v>270</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
@@ -28826,139 +28930,125 @@
         <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>275</v>
       </c>
       <c r="B20">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B20:B26" si="2">C19+1</f>
         <v>28</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C20:C26" si="3">B20+3</f>
         <v>31</v>
       </c>
       <c r="D20" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>150</v>
+        <v>271</v>
       </c>
       <c r="B21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>213</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>151</v>
-      </c>
       <c r="B22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>36</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="D22" t="s">
-        <v>156</v>
-      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>152</v>
-      </c>
       <c r="B23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>43</v>
-      </c>
-      <c r="D23" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>47</v>
+      </c>
+      <c r="K24" s="75" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>48</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="K25" s="71" t="s">
-        <v>128</v>
-      </c>
+      <c r="K25" s="75"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>52</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>214</v>
-      </c>
-      <c r="K26" s="71"/>
+        <v>197</v>
+      </c>
+      <c r="K26" s="75"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B27">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B27" si="4">C26+1</f>
         <v>56</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C27" si="5">B27+3</f>
         <v>59</v>
       </c>
       <c r="D27" t="s">
-        <v>215</v>
-      </c>
-      <c r="K27" s="71"/>
+        <v>198</v>
+      </c>
+      <c r="K27" s="75"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K28" s="71"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K29" s="71"/>
+      <c r="K28" s="75"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="K25:K29"/>
+    <mergeCell ref="K24:K28"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="A7:C7"/>
   </mergeCells>
@@ -28979,7 +29069,7 @@
   <sheetData>
     <row r="3" spans="10:11" ht="18" x14ac:dyDescent="0.35">
       <c r="J3" s="5" t="s">
-        <v>198</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="10:11" x14ac:dyDescent="0.3">
@@ -28987,7 +29077,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="10:11" x14ac:dyDescent="0.3">
@@ -28995,7 +29085,7 @@
         <v>2</v>
       </c>
       <c r="K5" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="10:11" x14ac:dyDescent="0.3">
@@ -29003,7 +29093,7 @@
         <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="10:11" x14ac:dyDescent="0.3">
@@ -29011,7 +29101,7 @@
         <v>4</v>
       </c>
       <c r="K7" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="10:11" x14ac:dyDescent="0.3">
@@ -29019,7 +29109,7 @@
         <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -29084,7 +29174,7 @@
         <v>32</v>
       </c>
       <c r="I3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J3" s="60">
         <f>J2/2.4</f>
@@ -29102,7 +29192,7 @@
         <v>0.3</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -29116,7 +29206,7 @@
         <v>34</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J5" s="60">
         <f>J4*J3</f>
@@ -29129,7 +29219,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.5245825484330734E-3</v>
+        <v>1.0935177735114128E-2</v>
       </c>
       <c r="G6" t="s">
         <v>32</v>
@@ -29144,7 +29234,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>104.99147809522781</v>
+        <v>91.447987789799114</v>
       </c>
       <c r="G7" t="s">
         <v>30</v>
@@ -29156,18 +29246,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>9.2352095772295934E-3</v>
+        <v>1.1757520068629701E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>9.2352095772295934E-3</v>
+        <v>1.1757520068629701E-2</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>4.9914780952278054E-2</v>
+        <v>-8.552012210200885E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -29176,11 +29266,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7603398736014769E-2</v>
+        <v>2.0572267434334088E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>8.3681891587851758E-3</v>
+        <v>8.8147473657043864E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -29189,11 +29279,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9846376358314785E-2</v>
+        <v>3.2543169481701058E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.2242977622300016E-2</v>
+        <v>1.197090204736697E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -29202,11 +29292,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.9024191722007433E-2</v>
+        <v>4.5437253426693497E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1778153636926478E-3</v>
+        <v>1.2894083944992439E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -29215,11 +29305,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7473938253126124E-2</v>
+        <v>5.3657585431516816E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>8.4497465311186917E-3</v>
+        <v>8.2203320048233192E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -29228,11 +29318,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7435826744969255E-2</v>
+        <v>6.6500477570086591E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.9618884918431308E-3</v>
+        <v>1.2842892138569775E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -29241,11 +29331,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4556566171690921E-2</v>
+        <v>7.4121262666395127E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1207394267216659E-3</v>
+        <v>7.6207850963085355E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -29254,11 +29344,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5556309518636053E-2</v>
+        <v>8.4239760948427153E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0999743346945132E-2</v>
+        <v>1.0118498282032026E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -29267,11 +29357,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4286482942086821E-2</v>
+        <v>9.6889806305596154E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7301734234507683E-3</v>
+        <v>1.2650045357169001E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -29280,11 +29370,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5762263920823848E-2</v>
+        <v>0.10906602552841144</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1475780978737027E-2</v>
+        <v>1.2176219222815282E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -29293,11 +29383,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10641926327653511</v>
+        <v>0.12132300657217431</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0656999355711266E-2</v>
+        <v>1.2256981043762868E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -29306,11 +29396,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11580713793856016</v>
+        <v>0.13413628220706258</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3878746620250503E-3</v>
+        <v>1.281327563488828E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -29319,11 +29409,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12467081723652605</v>
+        <v>0.14506434585102523</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8636792979658874E-3</v>
+        <v>1.0928063643962649E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -29332,11 +29422,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13167499216078848</v>
+        <v>0.15599208832399206</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0041749242624324E-3</v>
+        <v>1.0927742472966823E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -29345,11 +29435,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14377512625283054</v>
+        <v>0.16579887034236607</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2100134092042053E-2</v>
+        <v>9.8067820183740106E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -29358,11 +29448,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15246328463183106</v>
+        <v>0.17709148981304074</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6881583790005268E-3</v>
+        <v>1.129261947067467E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -29371,11 +29461,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16023518596277386</v>
+        <v>0.18606055973480384</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7719013309427987E-3</v>
+        <v>8.9690699217631065E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -29384,11 +29474,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16997910870989233</v>
+        <v>0.19483014618627309</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>9.7439227471184664E-3</v>
+        <v>8.7695864514692468E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -29397,11 +29487,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18096706842022839</v>
+        <v>0.20776837696716843</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0987959710336059E-2</v>
+        <v>1.2938230780895343E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit avant refonte de la bibliothèque
les capteurs vont être définis dans le code principal et non plus dans le fichiers.cpp
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9A77D9-CEB9-4B2C-895E-EC576C403DAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A149D57-FB58-44C2-A206-CFBBE06314A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2904" yWindow="0" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="299">
   <si>
     <t>Produit</t>
   </si>
@@ -934,6 +934,51 @@
   <si>
     <t>XXXX</t>
   </si>
+  <si>
+    <t>Couleur fil</t>
+  </si>
+  <si>
+    <t>blanc</t>
+  </si>
+  <si>
+    <t>jaune</t>
+  </si>
+  <si>
+    <t>vert</t>
+  </si>
+  <si>
+    <t>bleu</t>
+  </si>
+  <si>
+    <t>rouge</t>
+  </si>
+  <si>
+    <t>noir</t>
+  </si>
+  <si>
+    <t>cable</t>
+  </si>
+  <si>
+    <t>carte</t>
+  </si>
+  <si>
+    <t>Noir</t>
+  </si>
+  <si>
+    <t>Rouge</t>
+  </si>
+  <si>
+    <t>Jaune</t>
+  </si>
+  <si>
+    <t>Blanc</t>
+  </si>
+  <si>
+    <t>gris</t>
+  </si>
+  <si>
+    <t>violet</t>
+  </si>
 </sst>
 </file>
 
@@ -1503,7 +1548,7 @@
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1630,8 +1675,40 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="6" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="26" xfId="6" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="25" xfId="7" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1645,38 +1722,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="25" xfId="6" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="26" xfId="6" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="25" xfId="7" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" xfId="7" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="25" xfId="5" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="6" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Insatisfaisant" xfId="6" builtinId="27"/>
@@ -14647,16 +14693,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>297180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -14671,7 +14717,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6096000" y="137160"/>
+          <a:off x="13936980" y="297180"/>
           <a:ext cx="1645920" cy="3489960"/>
           <a:chOff x="342900" y="562200"/>
           <a:chExt cx="1645920" cy="2706780"/>
@@ -15116,16 +15162,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>191721</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>237441</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>20254</xdr:rowOff>
+      <xdr:rowOff>142174</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -15140,7 +15186,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6080760" y="3749040"/>
+          <a:off x="12466320" y="3870960"/>
           <a:ext cx="3125421" cy="1765234"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -18549,21 +18595,21 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="76" t="s">
+      <c r="B2" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="90"/>
       <c r="D2" s="64">
         <f>SUM(D5:D19)</f>
         <v>487.51</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="65"/>
-      <c r="G2" s="76" t="s">
+      <c r="G2" s="90" t="s">
         <v>172</v>
       </c>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
+      <c r="H2" s="90"/>
+      <c r="I2" s="90"/>
       <c r="J2" s="64">
         <f>SUM(J5:J19)</f>
         <v>0</v>
@@ -30425,10 +30471,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D1C501-6ABF-4FF7-B1E1-C49F27E96A4F}">
-  <dimension ref="B1:N25"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30437,6 +30483,7 @@
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="24" thickBot="1" x14ac:dyDescent="0.5">
@@ -30455,431 +30502,574 @@
       <c r="F1" s="72" t="s">
         <v>200</v>
       </c>
+      <c r="G1" s="72" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C2" s="81" t="s">
+      <c r="C2" s="91" t="s">
         <v>207</v>
       </c>
-      <c r="D2" s="81" t="s">
+      <c r="D2" s="91" t="s">
         <v>203</v>
       </c>
-      <c r="E2" s="82">
+      <c r="E2" s="76">
         <v>1</v>
       </c>
-      <c r="F2" s="95" t="s">
+      <c r="F2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="L2" s="81" t="s">
+      <c r="L2" s="91" t="s">
         <v>210</v>
       </c>
-      <c r="M2" s="82">
+      <c r="M2" s="76">
         <v>1</v>
       </c>
-      <c r="N2" s="82"/>
+      <c r="N2" s="76"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="97"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="92"/>
+      <c r="D3" s="92"/>
       <c r="E3" s="68">
         <v>2</v>
       </c>
-      <c r="F3" s="94" t="s">
+      <c r="F3" s="86" t="s">
         <v>257</v>
       </c>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
       <c r="M3" s="68">
         <v>2</v>
       </c>
       <c r="N3" s="68"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="97"/>
-      <c r="C4" s="83"/>
-      <c r="D4" s="83"/>
+      <c r="B4" s="95"/>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
       <c r="E4" s="68">
         <v>3</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
+      <c r="J4" s="92"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
       <c r="M4" s="68">
         <v>3</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="98"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="85">
+      <c r="B5" s="96"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="77">
         <v>4</v>
       </c>
-      <c r="F5" s="88" t="s">
+      <c r="F5" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
       <c r="M5" s="68">
         <v>4</v>
       </c>
       <c r="N5" s="68"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="91" t="s">
         <v>207</v>
       </c>
-      <c r="D6" s="81" t="s">
+      <c r="D6" s="91" t="s">
         <v>182</v>
       </c>
-      <c r="E6" s="82">
+      <c r="E6" s="76">
         <v>1</v>
       </c>
-      <c r="F6" s="90" t="s">
+      <c r="F6" s="82" t="s">
         <v>184</v>
       </c>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="85">
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
+      <c r="M6" s="77">
         <v>5</v>
       </c>
-      <c r="N6" s="85"/>
+      <c r="N6" s="77"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="97"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
       <c r="E7" s="68">
         <v>2</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="86" t="s">
         <v>282</v>
       </c>
-      <c r="J7" s="81" t="s">
+      <c r="J7" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="K7" s="81" t="s">
+      <c r="K7" s="91" t="s">
         <v>209</v>
       </c>
-      <c r="L7" s="81" t="s">
+      <c r="L7" s="91" t="s">
         <v>211</v>
       </c>
-      <c r="M7" s="82">
+      <c r="M7" s="76">
         <v>1</v>
       </c>
-      <c r="N7" s="82" t="s">
+      <c r="N7" s="76" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="98"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="85">
+      <c r="B8" s="96"/>
+      <c r="C8" s="93"/>
+      <c r="D8" s="93"/>
+      <c r="E8" s="77">
         <v>3</v>
       </c>
-      <c r="F8" s="88" t="s">
+      <c r="F8" s="80" t="s">
         <v>202</v>
       </c>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
+      <c r="J8" s="92"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
       <c r="M8" s="68">
         <v>2</v>
       </c>
-      <c r="N8" s="99" t="s">
+      <c r="N8" s="88" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="91" t="s">
         <v>207</v>
       </c>
-      <c r="D9" s="81" t="s">
+      <c r="D9" s="91" t="s">
         <v>281</v>
       </c>
-      <c r="E9" s="82">
+      <c r="E9" s="76">
         <v>1</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="85">
+      <c r="J9" s="93"/>
+      <c r="K9" s="93"/>
+      <c r="L9" s="93"/>
+      <c r="M9" s="77">
         <v>3</v>
       </c>
-      <c r="N9" s="87" t="s">
+      <c r="N9" s="79" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="97"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
+      <c r="B10" s="95"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
       <c r="E10" s="68">
         <v>2</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="J10" s="81" t="s">
+      <c r="J10" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="K10" s="81" t="s">
+      <c r="K10" s="91" t="s">
         <v>212</v>
       </c>
-      <c r="L10" s="81" t="s">
+      <c r="L10" s="91" t="s">
         <v>213</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
-      <c r="N10" s="86" t="s">
+      <c r="N10" s="78" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="97"/>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
+      <c r="B11" s="95"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
       <c r="E11" s="68">
         <v>3</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="81" t="s">
         <v>202</v>
       </c>
-      <c r="J11" s="77"/>
-      <c r="K11" s="77"/>
-      <c r="L11" s="77"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
       <c r="M11">
         <v>2</v>
       </c>
-      <c r="N11" s="100" t="s">
+      <c r="N11" s="89" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="98"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="85">
+      <c r="B12" s="96"/>
+      <c r="C12" s="93"/>
+      <c r="D12" s="93"/>
+      <c r="E12" s="77">
         <v>4</v>
       </c>
-      <c r="F12" s="91" t="s">
+      <c r="F12" s="83" t="s">
         <v>184</v>
       </c>
-      <c r="J12" s="81" t="s">
+      <c r="J12" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="K12" s="81" t="s">
+      <c r="K12" s="91" t="s">
         <v>212</v>
       </c>
-      <c r="L12" s="81" t="s">
+      <c r="L12" s="91" t="s">
         <v>214</v>
       </c>
-      <c r="M12" s="82">
+      <c r="M12" s="76">
         <v>1</v>
       </c>
-      <c r="N12" s="82" t="s">
+      <c r="N12" s="76" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="91" t="s">
         <v>207</v>
       </c>
-      <c r="D13" s="81" t="s">
+      <c r="D13" s="91" t="s">
         <v>192</v>
       </c>
-      <c r="E13" s="82">
+      <c r="E13" s="76">
         <v>1</v>
       </c>
-      <c r="F13" s="92" t="s">
+      <c r="F13" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J13" s="83"/>
-      <c r="K13" s="83"/>
-      <c r="L13" s="83"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
       <c r="M13" s="68">
         <v>2</v>
       </c>
-      <c r="N13" s="86" t="s">
+      <c r="N13" s="78" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="97"/>
-      <c r="C14" s="83"/>
-      <c r="D14" s="83"/>
+      <c r="B14" s="95"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
       <c r="E14" s="68">
         <v>2</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="85" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="97"/>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
       <c r="E15" s="68">
         <v>3</v>
       </c>
-      <c r="F15" s="89" t="s">
+      <c r="F15" s="81" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="98"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="85">
+      <c r="B16" s="96"/>
+      <c r="C16" s="93"/>
+      <c r="D16" s="93"/>
+      <c r="E16" s="77">
         <v>4</v>
       </c>
-      <c r="F16" s="91" t="s">
+      <c r="F16" s="83" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="96" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="D17" s="81" t="s">
+      <c r="D17" s="91" t="s">
         <v>279</v>
       </c>
-      <c r="E17" s="82">
+      <c r="E17" s="76">
         <v>1</v>
       </c>
-      <c r="F17" s="92" t="s">
+      <c r="F17" s="84" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="97"/>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
+      <c r="G17" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="95"/>
+      <c r="C18" s="92"/>
+      <c r="D18" s="92"/>
       <c r="E18" s="68">
         <v>2</v>
       </c>
-      <c r="F18" s="93" t="s">
+      <c r="F18" s="85" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="83"/>
-      <c r="D19" s="83"/>
+      <c r="G18" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B19" s="95"/>
+      <c r="C19" s="92"/>
+      <c r="D19" s="92"/>
       <c r="E19" s="68">
         <v>3</v>
       </c>
-      <c r="F19" s="94" t="s">
+      <c r="F19" s="86" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="97"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="83"/>
+      <c r="G19" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B20" s="95"/>
+      <c r="C20" s="92"/>
+      <c r="D20" s="92"/>
       <c r="E20" s="68">
         <v>4</v>
       </c>
-      <c r="F20" s="94" t="s">
+      <c r="F20" s="86" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="97"/>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
+      <c r="G20" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="95"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="92"/>
       <c r="E21" s="68">
         <v>5</v>
       </c>
-      <c r="F21" s="94" t="s">
+      <c r="F21" s="86" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="22" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="98"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="85">
+      <c r="G21" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="96"/>
+      <c r="C22" s="93"/>
+      <c r="D22" s="93"/>
+      <c r="E22" s="77">
         <v>6</v>
       </c>
-      <c r="F22" s="94" t="s">
+      <c r="F22" s="86" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="96" t="s">
+      <c r="G22" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="94" t="s">
         <v>201</v>
       </c>
-      <c r="C23" s="81" t="s">
+      <c r="C23" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="91" t="s">
         <v>185</v>
       </c>
-      <c r="E23" s="82">
+      <c r="E23" s="76">
         <v>1</v>
       </c>
-      <c r="F23" s="90" t="s">
+      <c r="F23" s="82" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="97"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
+      <c r="G23" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B24" s="95"/>
+      <c r="C24" s="92"/>
+      <c r="D24" s="92"/>
       <c r="E24" s="68">
         <v>2</v>
       </c>
-      <c r="F24" s="89" t="s">
+      <c r="F24" s="81" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="98"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="85">
+      <c r="G24" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="96"/>
+      <c r="C25" s="93"/>
+      <c r="D25" s="93"/>
+      <c r="E25" s="77">
         <v>3</v>
       </c>
-      <c r="F25" s="91" t="s">
+      <c r="F25" s="83" t="s">
         <v>280</v>
       </c>
+      <c r="G25" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>291</v>
+      </c>
+      <c r="C29" t="s">
+        <v>292</v>
+      </c>
+      <c r="D29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="97" t="s">
+        <v>70</v>
+      </c>
+      <c r="B30" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C30" t="s">
+        <v>295</v>
+      </c>
+      <c r="D30" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="97"/>
+      <c r="B31" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="C31" t="s">
+        <v>296</v>
+      </c>
+      <c r="D31" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="97"/>
+      <c r="B32" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C32" t="s">
+        <v>293</v>
+      </c>
+      <c r="D32" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="97"/>
+      <c r="B33" s="101" t="s">
+        <v>184</v>
+      </c>
+      <c r="C33" t="s">
+        <v>294</v>
+      </c>
+      <c r="D33" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>295</v>
+      </c>
+      <c r="D34" s="76" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="97"/>
+      <c r="B35" s="85" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>296</v>
+      </c>
+      <c r="D35" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="97"/>
+      <c r="B36" s="81" t="s">
+        <v>202</v>
+      </c>
+      <c r="C36" t="s">
+        <v>293</v>
+      </c>
+      <c r="D36" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="97"/>
+      <c r="B37" s="83" t="s">
+        <v>280</v>
+      </c>
+      <c r="C37" t="s">
+        <v>294</v>
+      </c>
+      <c r="D37" t="s">
+        <v>298</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="32">
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
     <mergeCell ref="L12:L13"/>
     <mergeCell ref="K12:K13"/>
     <mergeCell ref="J12:J13"/>
@@ -30897,13 +31087,13 @@
     <mergeCell ref="C23:C25"/>
     <mergeCell ref="C17:C22"/>
     <mergeCell ref="B17:B22"/>
+    <mergeCell ref="D17:D22"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="D6:D8"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D17:D22"/>
     <mergeCell ref="D13:D16"/>
     <mergeCell ref="C13:C16"/>
     <mergeCell ref="B13:B16"/>
@@ -30922,8 +31112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -30960,7 +31150,7 @@
       <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="77" t="s">
+      <c r="J3" s="97" t="s">
         <v>161</v>
       </c>
       <c r="K3" t="s">
@@ -30980,7 +31170,7 @@
       <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="77"/>
+      <c r="J4" s="97"/>
       <c r="K4" t="s">
         <v>192</v>
       </c>
@@ -31007,7 +31197,7 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="77"/>
+      <c r="J5" s="97"/>
       <c r="K5" t="s">
         <v>70</v>
       </c>
@@ -31032,7 +31222,7 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="77"/>
+      <c r="J6" s="97"/>
       <c r="K6" t="s">
         <v>183</v>
       </c>
@@ -31362,13 +31552,13 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:12" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="79" t="s">
+      <c r="B3" s="99" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
@@ -31416,11 +31606,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="99" t="s">
         <v>126</v>
       </c>
-      <c r="B7" s="79"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="99"/>
       <c r="D7" t="s">
         <v>135</v>
       </c>
@@ -31661,7 +31851,7 @@
         <f t="shared" si="3"/>
         <v>47</v>
       </c>
-      <c r="K24" s="78" t="s">
+      <c r="K24" s="98" t="s">
         <v>116</v>
       </c>
     </row>
@@ -31674,7 +31864,7 @@
         <f t="shared" si="3"/>
         <v>51</v>
       </c>
-      <c r="K25" s="78"/>
+      <c r="K25" s="98"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
@@ -31691,7 +31881,7 @@
       <c r="D26" t="s">
         <v>180</v>
       </c>
-      <c r="K26" s="78"/>
+      <c r="K26" s="98"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
@@ -31708,10 +31898,10 @@
       <c r="D27" t="s">
         <v>181</v>
       </c>
-      <c r="K27" s="78"/>
+      <c r="K27" s="98"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="K28" s="78"/>
+      <c r="K28" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31739,10 +31929,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="100" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="80"/>
+      <c r="B1" s="100"/>
       <c r="D1" t="s">
         <v>277</v>
       </c>
@@ -32385,10 +32575,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="100" t="s">
         <v>270</v>
       </c>
-      <c r="B22" s="80"/>
+      <c r="B22" s="100"/>
       <c r="C22" t="s">
         <v>271</v>
       </c>
@@ -32433,7 +32623,7 @@
         <v>0</v>
       </c>
       <c r="F25" t="str">
-        <f>MID(D$22,B25+1,4)</f>
+        <f t="shared" ref="F25:F39" si="19">MID(D$22,B25+1,4)</f>
         <v>00F0</v>
       </c>
       <c r="G25">
@@ -32464,11 +32654,11 @@
         <v>0</v>
       </c>
       <c r="F26" t="str">
-        <f>MID(D$22,B26+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0546</v>
       </c>
       <c r="G26">
-        <f t="shared" ref="G26:G39" si="19">HEX2DEC(F26)</f>
+        <f t="shared" ref="G26:G39" si="20">HEX2DEC(F26)</f>
         <v>1350</v>
       </c>
       <c r="H26">
@@ -32481,11 +32671,11 @@
         <v>244</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:B37" si="20">B26+4</f>
+        <f t="shared" ref="B27:B37" si="21">B26+4</f>
         <v>8</v>
       </c>
       <c r="C27">
-        <f t="shared" ref="C27:C37" si="21">C26+4</f>
+        <f t="shared" ref="C27:C37" si="22">C26+4</f>
         <v>11</v>
       </c>
       <c r="D27" t="s">
@@ -32495,11 +32685,11 @@
         <v>0</v>
       </c>
       <c r="F27" t="str">
-        <f>MID(D$22,B27+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0140</v>
       </c>
       <c r="G27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>320</v>
       </c>
       <c r="H27">
@@ -32512,11 +32702,11 @@
         <v>245</v>
       </c>
       <c r="B28">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>12</v>
       </c>
       <c r="C28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>15</v>
       </c>
       <c r="D28" t="s">
@@ -32526,11 +32716,11 @@
         <v>1</v>
       </c>
       <c r="F28" t="str">
-        <f>MID(D$22,B28+1,4)</f>
+        <f t="shared" si="19"/>
         <v>027B</v>
       </c>
       <c r="G28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>635</v>
       </c>
       <c r="H28">
@@ -32543,11 +32733,11 @@
         <v>246</v>
       </c>
       <c r="B29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>16</v>
       </c>
       <c r="C29">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>19</v>
       </c>
       <c r="D29" t="s">
@@ -32557,11 +32747,11 @@
         <v>0</v>
       </c>
       <c r="F29" t="str">
-        <f>MID(D$22,B29+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0320</v>
       </c>
       <c r="G29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>800</v>
       </c>
       <c r="H29">
@@ -32574,11 +32764,11 @@
         <v>247</v>
       </c>
       <c r="B30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>20</v>
       </c>
       <c r="C30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>23</v>
       </c>
       <c r="D30" t="s">
@@ -32588,11 +32778,11 @@
         <v>1</v>
       </c>
       <c r="F30" t="str">
-        <f>MID(D$22,B30+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0289</v>
       </c>
       <c r="G30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>649</v>
       </c>
       <c r="H30">
@@ -32605,11 +32795,11 @@
         <v>248</v>
       </c>
       <c r="B31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>24</v>
       </c>
       <c r="C31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>27</v>
       </c>
       <c r="D31" t="s">
@@ -32619,11 +32809,11 @@
         <v>0</v>
       </c>
       <c r="F31" t="str">
-        <f>MID(D$22,B31+1,4)</f>
+        <f t="shared" si="19"/>
         <v>2A30</v>
       </c>
       <c r="G31">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>10800</v>
       </c>
       <c r="H31">
@@ -32636,11 +32826,11 @@
         <v>249</v>
       </c>
       <c r="B32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>28</v>
       </c>
       <c r="C32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>31</v>
       </c>
       <c r="D32" t="s">
@@ -32650,11 +32840,11 @@
         <v>0</v>
       </c>
       <c r="F32" t="str">
-        <f>MID(D$22,B32+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0BB8</v>
       </c>
       <c r="G32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>3000</v>
       </c>
       <c r="H32">
@@ -32667,11 +32857,11 @@
         <v>250</v>
       </c>
       <c r="B33">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>32</v>
       </c>
       <c r="C33">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>35</v>
       </c>
       <c r="D33" t="s">
@@ -32681,11 +32871,11 @@
         <v>0</v>
       </c>
       <c r="F33" t="str">
-        <f>MID(D$22,B33+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0064</v>
       </c>
       <c r="G33">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>100</v>
       </c>
       <c r="H33">
@@ -32698,11 +32888,11 @@
         <v>251</v>
       </c>
       <c r="B34">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>36</v>
       </c>
       <c r="C34">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>39</v>
       </c>
       <c r="D34" t="s">
@@ -32712,11 +32902,11 @@
         <v>1</v>
       </c>
       <c r="F34" t="str">
-        <f>MID(D$22,B34+1,4)</f>
+        <f t="shared" si="19"/>
         <v>02BC</v>
       </c>
       <c r="G34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>700</v>
       </c>
       <c r="H34">
@@ -32729,22 +32919,22 @@
         <v>252</v>
       </c>
       <c r="B35">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>40</v>
       </c>
       <c r="C35">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>43</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
       <c r="F35" t="str">
-        <f>MID(D$22,B35+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0000</v>
       </c>
       <c r="G35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H35">
@@ -32757,22 +32947,22 @@
         <v>253</v>
       </c>
       <c r="B36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>44</v>
       </c>
       <c r="C36">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>47</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
       </c>
       <c r="F36" t="str">
-        <f>MID(D$22,B36+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0000</v>
       </c>
       <c r="G36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H36">
@@ -32785,22 +32975,22 @@
         <v>254</v>
       </c>
       <c r="B37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>48</v>
       </c>
       <c r="C37">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>51</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
       <c r="F37" t="str">
-        <f>MID(D$22,B37+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0000</v>
       </c>
       <c r="G37">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H37">
@@ -32827,11 +33017,11 @@
         <v>0</v>
       </c>
       <c r="F38" t="str">
-        <f>MID(D$22,B38+1,4)</f>
+        <f t="shared" si="19"/>
         <v>0025</v>
       </c>
       <c r="G38">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>37</v>
       </c>
       <c r="H38">
@@ -32858,11 +33048,11 @@
         <v>1</v>
       </c>
       <c r="F39" t="str">
-        <f>MID(D$22,B39+1,4)</f>
+        <f t="shared" si="19"/>
         <v>03E8</v>
       </c>
       <c r="G39">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>1000</v>
       </c>
       <c r="H39">
@@ -33043,7 +33233,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.8725239675447728E-3</v>
+        <v>9.9247741549602971E-3</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -33058,7 +33248,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>101.29122028849254</v>
+        <v>100.75796027058314</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -33070,18 +33260,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>7.9825393492710447E-3</v>
+        <v>1.0576874966191455E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>7.9825393492710447E-3</v>
+        <v>1.0576874966191455E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>1.2912202884925393E-2</v>
+        <v>7.579602705831405E-3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -33090,11 +33280,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.7543390421934982E-2</v>
+        <v>2.0323812632535652E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>9.5608510726639378E-3</v>
+        <v>9.7469376663441975E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -33103,11 +33293,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9948791236490847E-2</v>
+        <v>2.8763493374342364E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.2405400814555864E-2</v>
+        <v>8.4396807418067113E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -33116,11 +33306,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.731646444582977E-2</v>
+        <v>4.0028622149871657E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3676732093389229E-3</v>
+        <v>1.1265128775529293E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -33129,11 +33319,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.0257121364178925E-2</v>
+        <v>4.8915458434067721E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2940656918349155E-2</v>
+        <v>8.8868362841960646E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -33142,11 +33332,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7585849620118597E-2</v>
+        <v>5.6895181812828079E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3287282559396719E-3</v>
+        <v>7.9797233787603575E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -33155,11 +33345,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.727871520974564E-2</v>
+        <v>6.6247562718540501E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.6928655896270435E-3</v>
+        <v>9.3523809057124221E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33168,11 +33358,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7654029130117264E-2</v>
+        <v>7.3926485073214643E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0375313920371623E-2</v>
+        <v>7.678922354674142E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -33181,11 +33371,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7386286916993489E-2</v>
+        <v>8.5747937835073187E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>9.732257786876225E-3</v>
+        <v>1.1821452761858545E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -33194,11 +33384,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10019951140173675</v>
+        <v>9.5881910523806513E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2813224484743257E-2</v>
+        <v>1.0133972688733325E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -33207,11 +33397,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10979410986939131</v>
+        <v>0.10514673958882985</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5945984676545637E-3</v>
+        <v>9.2648290650233361E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -33220,11 +33410,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11689786336581179</v>
+        <v>0.11373883561533524</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1037534964204785E-3</v>
+        <v>8.5920960265053886E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -33233,11 +33423,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12526162053291653</v>
+        <v>0.1210235801283313</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3637571671047461E-3</v>
+        <v>7.2847445129960581E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -33246,11 +33436,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13454997484667919</v>
+        <v>0.13218223305150692</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2883543137626534E-3</v>
+        <v>1.1158652923175624E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -33259,11 +33449,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14567955808650287</v>
+        <v>0.14310002408175779</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1129583239823687E-2</v>
+        <v>1.0917791030250867E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -33272,11 +33462,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15432656579751405</v>
+        <v>0.15121934565591852</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6470077110111787E-3</v>
+        <v>8.1193215741607316E-3</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -33285,11 +33475,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16728822317333117</v>
+        <v>0.16275285755826832</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2961657375817115E-2</v>
+        <v>1.1533511902349802E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -33298,11 +33488,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17776426881449073</v>
+        <v>0.17558911852321835</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0476045641159559E-2</v>
+        <v>1.2836260964950025E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -33311,11 +33501,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18757795538335068</v>
+        <v>0.18857070894424563</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8136865688599473E-3</v>
+        <v>1.2981590421027284E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test codage radio debut, suite et fin
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1461BFA-564F-4122-99E0-03E6F257208C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F89DADB-274B-4DC4-B123-B369A61FD8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="300">
   <si>
     <t>Produit</t>
   </si>
@@ -976,6 +976,12 @@
   <si>
     <t>Pression hPa (environ 1000hPa)</t>
   </si>
+  <si>
+    <t>FFFFFFF000046500401007B20020300FFFFFF89200502800FFFFFFB8B0064000FFFFFFBC20000000000000025000FFFFFFE830000</t>
+  </si>
+  <si>
+    <t>FFFFFFF0</t>
+  </si>
 </sst>
 </file>
 
@@ -1690,9 +1696,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1709,6 +1712,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -30504,13 +30510,13 @@
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="93" t="s">
+      <c r="D2" s="92" t="s">
         <v>202</v>
       </c>
       <c r="E2" s="76">
@@ -30519,13 +30525,13 @@
       <c r="F2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="93" t="s">
+      <c r="J2" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="93" t="s">
+      <c r="K2" s="92" t="s">
         <v>208</v>
       </c>
-      <c r="L2" s="93" t="s">
+      <c r="L2" s="92" t="s">
         <v>209</v>
       </c>
       <c r="M2" s="76">
@@ -30534,67 +30540,67 @@
       <c r="N2" s="76"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="97"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
       <c r="E3" s="68">
         <v>2</v>
       </c>
       <c r="F3" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93"/>
+      <c r="L3" s="93"/>
       <c r="M3" s="68">
         <v>2</v>
       </c>
       <c r="N3" s="68"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="97"/>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
+      <c r="B4" s="96"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
       <c r="E4" s="68">
         <v>3</v>
       </c>
       <c r="F4" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
+      <c r="J4" s="93"/>
+      <c r="K4" s="93"/>
+      <c r="L4" s="93"/>
       <c r="M4" s="68">
         <v>3</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="98"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
       <c r="E5" s="77">
         <v>4</v>
       </c>
       <c r="F5" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="J5" s="94"/>
-      <c r="K5" s="94"/>
-      <c r="L5" s="94"/>
+      <c r="J5" s="93"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="93"/>
       <c r="M5" s="68">
         <v>4</v>
       </c>
       <c r="N5" s="68"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="92" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="76">
@@ -30603,31 +30609,31 @@
       <c r="F6" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="95"/>
-      <c r="K6" s="95"/>
-      <c r="L6" s="95"/>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
+      <c r="L6" s="94"/>
       <c r="M6" s="77">
         <v>5</v>
       </c>
       <c r="N6" s="77"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="97"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
       <c r="E7" s="68">
         <v>2</v>
       </c>
       <c r="F7" s="86" t="s">
         <v>280</v>
       </c>
-      <c r="J7" s="93" t="s">
+      <c r="J7" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="K7" s="93" t="s">
+      <c r="K7" s="92" t="s">
         <v>208</v>
       </c>
-      <c r="L7" s="93" t="s">
+      <c r="L7" s="92" t="s">
         <v>210</v>
       </c>
       <c r="M7" s="76">
@@ -30638,18 +30644,18 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="98"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
+      <c r="B8" s="97"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
       <c r="E8" s="77">
         <v>3</v>
       </c>
       <c r="F8" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="J8" s="93"/>
+      <c r="K8" s="93"/>
+      <c r="L8" s="93"/>
       <c r="M8" s="68">
         <v>2</v>
       </c>
@@ -30658,13 +30664,13 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="D9" s="93" t="s">
+      <c r="D9" s="92" t="s">
         <v>279</v>
       </c>
       <c r="E9" s="76">
@@ -30673,9 +30679,9 @@
       <c r="F9" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
+      <c r="J9" s="94"/>
+      <c r="K9" s="94"/>
+      <c r="L9" s="94"/>
       <c r="M9" s="77">
         <v>3</v>
       </c>
@@ -30684,22 +30690,22 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="97"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
+      <c r="B10" s="96"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="93"/>
       <c r="E10" s="68">
         <v>2</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="J10" s="93" t="s">
+      <c r="J10" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="K10" s="93" t="s">
+      <c r="K10" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="L10" s="93" t="s">
+      <c r="L10" s="92" t="s">
         <v>212</v>
       </c>
       <c r="M10">
@@ -30710,18 +30716,18 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="97"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="93"/>
+      <c r="D11" s="93"/>
       <c r="E11" s="68">
         <v>3</v>
       </c>
       <c r="F11" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="J11" s="92"/>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
       <c r="M11">
         <v>2</v>
       </c>
@@ -30730,22 +30736,22 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="98"/>
-      <c r="C12" s="95"/>
-      <c r="D12" s="95"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="94"/>
+      <c r="D12" s="94"/>
       <c r="E12" s="77">
         <v>4</v>
       </c>
       <c r="F12" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="93" t="s">
+      <c r="J12" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="K12" s="93" t="s">
+      <c r="K12" s="92" t="s">
         <v>211</v>
       </c>
-      <c r="L12" s="93" t="s">
+      <c r="L12" s="92" t="s">
         <v>213</v>
       </c>
       <c r="M12" s="76">
@@ -30756,13 +30762,13 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="96" t="s">
+      <c r="B13" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="92" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="92" t="s">
         <v>191</v>
       </c>
       <c r="E13" s="76">
@@ -30771,9 +30777,9 @@
       <c r="F13" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J13" s="94"/>
-      <c r="K13" s="94"/>
-      <c r="L13" s="94"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="93"/>
+      <c r="L13" s="93"/>
       <c r="M13" s="68">
         <v>2</v>
       </c>
@@ -30782,9 +30788,9 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="97"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="93"/>
+      <c r="D14" s="93"/>
       <c r="E14" s="68">
         <v>2</v>
       </c>
@@ -30793,9 +30799,9 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="97"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
+      <c r="B15" s="96"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
       <c r="E15" s="68">
         <v>3</v>
       </c>
@@ -30804,9 +30810,9 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="98"/>
-      <c r="C16" s="95"/>
-      <c r="D16" s="95"/>
+      <c r="B16" s="97"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="94"/>
       <c r="E16" s="77">
         <v>4</v>
       </c>
@@ -30815,13 +30821,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="96" t="s">
+      <c r="B17" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="93" t="s">
+      <c r="D17" s="92" t="s">
         <v>277</v>
       </c>
       <c r="E17" s="76">
@@ -30835,9 +30841,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="97"/>
-      <c r="C18" s="94"/>
-      <c r="D18" s="94"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
       <c r="E18" s="68">
         <v>2</v>
       </c>
@@ -30849,9 +30855,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="97"/>
-      <c r="C19" s="94"/>
-      <c r="D19" s="94"/>
+      <c r="B19" s="96"/>
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
       <c r="E19" s="68">
         <v>3</v>
       </c>
@@ -30863,9 +30869,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="97"/>
-      <c r="C20" s="94"/>
-      <c r="D20" s="94"/>
+      <c r="B20" s="96"/>
+      <c r="C20" s="93"/>
+      <c r="D20" s="93"/>
       <c r="E20" s="68">
         <v>4</v>
       </c>
@@ -30877,9 +30883,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="97"/>
-      <c r="C21" s="94"/>
-      <c r="D21" s="94"/>
+      <c r="B21" s="96"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
       <c r="E21" s="68">
         <v>5</v>
       </c>
@@ -30891,9 +30897,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="98"/>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
+      <c r="B22" s="97"/>
+      <c r="C22" s="94"/>
+      <c r="D22" s="94"/>
       <c r="E22" s="77">
         <v>6</v>
       </c>
@@ -30905,13 +30911,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="96" t="s">
+      <c r="B23" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="93" t="s">
+      <c r="C23" s="92" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="93" t="s">
+      <c r="D23" s="92" t="s">
         <v>184</v>
       </c>
       <c r="E23" s="76">
@@ -30925,9 +30931,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="97"/>
-      <c r="C24" s="94"/>
-      <c r="D24" s="94"/>
+      <c r="B24" s="96"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
       <c r="E24" s="68">
         <v>2</v>
       </c>
@@ -30939,9 +30945,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="98"/>
-      <c r="C25" s="95"/>
-      <c r="D25" s="95"/>
+      <c r="B25" s="97"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
       <c r="E25" s="77">
         <v>3</v>
       </c>
@@ -30964,7 +30970,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="92" t="s">
+      <c r="A30" s="98" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="84" t="s">
@@ -30978,7 +30984,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="92"/>
+      <c r="A31" s="98"/>
       <c r="B31" s="85" t="s">
         <v>160</v>
       </c>
@@ -30990,7 +30996,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="92"/>
+      <c r="A32" s="98"/>
       <c r="B32" s="81" t="s">
         <v>201</v>
       </c>
@@ -31002,7 +31008,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="92"/>
+      <c r="A33" s="98"/>
       <c r="B33" s="90" t="s">
         <v>183</v>
       </c>
@@ -31014,7 +31020,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="92" t="s">
+      <c r="A34" s="98" t="s">
         <v>191</v>
       </c>
       <c r="B34" s="84" t="s">
@@ -31028,7 +31034,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="92"/>
+      <c r="A35" s="98"/>
       <c r="B35" s="85" t="s">
         <v>160</v>
       </c>
@@ -31040,7 +31046,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="92"/>
+      <c r="A36" s="98"/>
       <c r="B36" s="81" t="s">
         <v>201</v>
       </c>
@@ -31052,7 +31058,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="92"/>
+      <c r="A37" s="98"/>
       <c r="B37" s="83" t="s">
         <v>278</v>
       </c>
@@ -31065,6 +31071,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="J7:J9"/>
     <mergeCell ref="L2:L6"/>
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="J2:J6"/>
@@ -31081,22 +31103,6 @@
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="B6:B8"/>
     <mergeCell ref="D13:D16"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="B13:B16"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31109,7 +31115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -31147,7 +31153,7 @@
       <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="92" t="s">
+      <c r="J3" s="98" t="s">
         <v>161</v>
       </c>
       <c r="K3" t="s">
@@ -31167,7 +31173,7 @@
       <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="92"/>
+      <c r="J4" s="98"/>
       <c r="K4" t="s">
         <v>191</v>
       </c>
@@ -31194,7 +31200,7 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="92"/>
+      <c r="J5" s="98"/>
       <c r="K5" t="s">
         <v>70</v>
       </c>
@@ -31219,7 +31225,7 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="92"/>
+      <c r="J6" s="98"/>
       <c r="K6" t="s">
         <v>182</v>
       </c>
@@ -31913,10 +31919,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526E76B6-68A2-48DF-95E8-365FAB976DDF}">
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32579,9 +32585,8 @@
       <c r="C22" t="s">
         <v>270</v>
       </c>
-      <c r="D22" t="str">
-        <f>E1</f>
-        <v>00F005460140027B0320028928500BB8006402BC000000000000002503E8</v>
+      <c r="D22" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -32620,17 +32625,16 @@
       <c r="E25" t="b">
         <v>0</v>
       </c>
-      <c r="F25" t="str">
-        <f t="shared" ref="F25:F39" si="19">MID(D$22,B25+1,4)</f>
-        <v>00F0</v>
+      <c r="F25" t="s">
+        <v>299</v>
       </c>
       <c r="G25">
         <f>HEX2DEC(F25)</f>
-        <v>240</v>
+        <v>4294967280</v>
       </c>
       <c r="H25">
         <f>IF('Codage-décodage Radio'!E25,'Codage-décodage Radio'!G25/10-40,'Codage-décodage Radio'!G25/10)</f>
-        <v>24</v>
+        <v>429496728</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -32652,16 +32656,16 @@
         <v>0</v>
       </c>
       <c r="F26" t="str">
-        <f t="shared" si="19"/>
-        <v>0546</v>
+        <f t="shared" ref="F26:F39" si="19">MID(D$22,2*(B26+1),2*4)</f>
+        <v>00465004</v>
       </c>
       <c r="G26">
         <f t="shared" ref="G26:G39" si="20">HEX2DEC(F26)</f>
-        <v>1350</v>
+        <v>4608004</v>
       </c>
       <c r="H26">
         <f>IF('Codage-décodage Radio'!E26,'Codage-décodage Radio'!G26/10-40,'Codage-décodage Radio'!G26/10)</f>
-        <v>135</v>
+        <v>460800.4</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -32684,15 +32688,15 @@
       </c>
       <c r="F27" t="str">
         <f t="shared" si="19"/>
-        <v>0140</v>
+        <v>01007B20</v>
       </c>
       <c r="G27">
         <f t="shared" si="20"/>
-        <v>320</v>
+        <v>16808736</v>
       </c>
       <c r="H27">
         <f>IF('Codage-décodage Radio'!E27,'Codage-décodage Radio'!G27/10-40,'Codage-décodage Radio'!G27/10)</f>
-        <v>32</v>
+        <v>1680873.6</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -32715,15 +32719,15 @@
       </c>
       <c r="F28" t="str">
         <f t="shared" si="19"/>
-        <v>027B</v>
+        <v>020300FF</v>
       </c>
       <c r="G28">
         <f t="shared" si="20"/>
-        <v>635</v>
+        <v>33751295</v>
       </c>
       <c r="H28">
         <f>IF('Codage-décodage Radio'!E28,'Codage-décodage Radio'!G28/10-40,'Codage-décodage Radio'!G28/10)</f>
-        <v>23.5</v>
+        <v>3375089.5</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -32746,15 +32750,15 @@
       </c>
       <c r="F29" t="str">
         <f t="shared" si="19"/>
-        <v>0320</v>
+        <v>FFFF8920</v>
       </c>
       <c r="G29">
         <f t="shared" si="20"/>
-        <v>800</v>
+        <v>4294936864</v>
       </c>
       <c r="H29">
         <f>IF('Codage-décodage Radio'!E29,'Codage-décodage Radio'!G29/10-40,'Codage-décodage Radio'!G29/10)</f>
-        <v>80</v>
+        <v>429493686.39999998</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -32777,15 +32781,15 @@
       </c>
       <c r="F30" t="str">
         <f t="shared" si="19"/>
-        <v>0289</v>
+        <v>0502800F</v>
       </c>
       <c r="G30">
         <f t="shared" si="20"/>
-        <v>649</v>
+        <v>84049935</v>
       </c>
       <c r="H30">
         <f>IF('Codage-décodage Radio'!E30,'Codage-décodage Radio'!G30/10-40,'Codage-décodage Radio'!G30/10)</f>
-        <v>24.900000000000006</v>
+        <v>8404953.5</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -32808,15 +32812,15 @@
       </c>
       <c r="F31" t="str">
         <f t="shared" si="19"/>
-        <v>2850</v>
+        <v>FFFFFB8B</v>
       </c>
       <c r="G31">
         <f t="shared" si="20"/>
-        <v>10320</v>
+        <v>4294966155</v>
       </c>
       <c r="H31">
         <f>IF('Codage-décodage Radio'!E31,'Codage-décodage Radio'!G31/10-40,'Codage-décodage Radio'!G31/10)</f>
-        <v>1032</v>
+        <v>429496615.5</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -32839,15 +32843,15 @@
       </c>
       <c r="F32" t="str">
         <f t="shared" si="19"/>
-        <v>0BB8</v>
+        <v>0064000F</v>
       </c>
       <c r="G32">
         <f t="shared" si="20"/>
-        <v>3000</v>
+        <v>6553615</v>
       </c>
       <c r="H32">
         <f>IF('Codage-décodage Radio'!E32,'Codage-décodage Radio'!G32/10-40,'Codage-décodage Radio'!G32/10)</f>
-        <v>300</v>
+        <v>655361.5</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -32870,15 +32874,15 @@
       </c>
       <c r="F33" t="str">
         <f t="shared" si="19"/>
-        <v>0064</v>
+        <v>FFFFFBC2</v>
       </c>
       <c r="G33">
         <f t="shared" si="20"/>
-        <v>100</v>
+        <v>4294966210</v>
       </c>
       <c r="H33">
         <f>IF('Codage-décodage Radio'!E33,'Codage-décodage Radio'!G33/10-40,'Codage-décodage Radio'!G33/10)</f>
-        <v>10</v>
+        <v>429496621</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -32901,15 +32905,15 @@
       </c>
       <c r="F34" t="str">
         <f t="shared" si="19"/>
-        <v>02BC</v>
+        <v>00000000</v>
       </c>
       <c r="G34">
         <f t="shared" si="20"/>
-        <v>700</v>
+        <v>0</v>
       </c>
       <c r="H34">
         <f>IF('Codage-décodage Radio'!E34,'Codage-décodage Radio'!G34/10-40,'Codage-décodage Radio'!G34/10)</f>
-        <v>30</v>
+        <v>-40</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -32929,15 +32933,15 @@
       </c>
       <c r="F35" t="str">
         <f t="shared" si="19"/>
-        <v>0000</v>
+        <v>00000025</v>
       </c>
       <c r="G35">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="H35">
         <f>IF('Codage-décodage Radio'!E35,'Codage-décodage Radio'!G35/10-40,'Codage-décodage Radio'!G35/10)</f>
-        <v>0</v>
+        <v>3.7</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -32957,15 +32961,15 @@
       </c>
       <c r="F36" t="str">
         <f t="shared" si="19"/>
-        <v>0000</v>
+        <v>000FFFFF</v>
       </c>
       <c r="G36">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1048575</v>
       </c>
       <c r="H36">
         <f>IF('Codage-décodage Radio'!E36,'Codage-décodage Radio'!G36/10-40,'Codage-décodage Radio'!G36/10)</f>
-        <v>0</v>
+        <v>104857.5</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -32985,15 +32989,15 @@
       </c>
       <c r="F37" t="str">
         <f t="shared" si="19"/>
-        <v>0000</v>
+        <v>FE830000</v>
       </c>
       <c r="G37">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>4269998080</v>
       </c>
       <c r="H37">
         <f>IF('Codage-décodage Radio'!E37,'Codage-décodage Radio'!G37/10-40,'Codage-décodage Radio'!G37/10)</f>
-        <v>0</v>
+        <v>426999808</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -33016,15 +33020,15 @@
       </c>
       <c r="F38" t="str">
         <f t="shared" si="19"/>
-        <v>0025</v>
+        <v/>
       </c>
       <c r="G38">
         <f t="shared" si="20"/>
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="H38">
         <f>IF('Codage-décodage Radio'!E38,'Codage-décodage Radio'!G38/10-40,'Codage-décodage Radio'!G38/10)</f>
-        <v>3.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -33047,15 +33051,25 @@
       </c>
       <c r="F39" t="str">
         <f t="shared" si="19"/>
-        <v>03E8</v>
+        <v/>
       </c>
       <c r="G39">
         <f t="shared" si="20"/>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="H39">
         <f>IF('Codage-décodage Radio'!E39,'Codage-décodage Radio'!G39/10-40,'Codage-décodage Radio'!G39/10)</f>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f>B39+4</f>
         <v>60</v>
+      </c>
+      <c r="C40">
+        <f>C39+4</f>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -33231,7 +33245,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.7978622223663797E-3</v>
+        <v>1.0051609890995851E-2</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -33246,7 +33260,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>102.06308042556655</v>
+        <v>99.486550994760719</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -33258,18 +33272,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>9.5021517761640396E-3</v>
+        <v>1.291265385046139E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>9.5021517761640396E-3</v>
+        <v>1.291265385046139E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>2.0630804255665536E-2</v>
+        <v>-5.1344900523928065E-3</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -33278,11 +33292,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.8205752605634999E-2</v>
+        <v>2.106675714830844E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>8.7036008294709595E-3</v>
+        <v>8.1541032978470502E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -33291,11 +33305,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5664937645518058E-2</v>
+        <v>2.9862774500316106E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>7.4591850398830588E-3</v>
+        <v>8.7960173520076658E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -33304,11 +33318,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6629433309434918E-2</v>
+        <v>4.0341745761296809E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.096449566391686E-2</v>
+        <v>1.0478971260980702E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -33317,11 +33331,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9117013794542835E-2</v>
+        <v>5.2686771903536211E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2487580485107917E-2</v>
+        <v>1.2345026142239403E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -33330,11 +33344,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.0608157852936585E-2</v>
+        <v>6.218470307830732E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>1.149114405839375E-2</v>
+        <v>9.4979311747711084E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -33343,11 +33357,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7609628764998778E-2</v>
+        <v>7.0240866834778204E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0014709120621924E-3</v>
+        <v>8.0561637564708841E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33356,11 +33370,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.5738352736541351E-2</v>
+        <v>7.7778402694171467E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>8.128723971542573E-3</v>
+        <v>7.5375358593932629E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -33369,11 +33383,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4983294198751877E-2</v>
+        <v>8.8930854158608158E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2449414622105264E-3</v>
+        <v>1.1152451464436691E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -33382,11 +33396,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.7930717511080151E-2</v>
+        <v>9.8135539498220806E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2947423312328274E-2</v>
+        <v>9.2046853396126477E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -33395,11 +33409,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10839733838339517</v>
+        <v>0.10889480482865095</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0466620872315022E-2</v>
+        <v>1.0759265330430146E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -33408,11 +33422,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11988020017399791</v>
+        <v>0.11772823905109414</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1482861790602733E-2</v>
+        <v>8.83343422244319E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -33421,11 +33435,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12751163016832187</v>
+        <v>0.12948176619920576</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6314299943239655E-3</v>
+        <v>1.175352714811162E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -33434,11 +33448,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1378093815165046</v>
+        <v>0.13817228882067401</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0297751348182727E-2</v>
+        <v>8.6905226214682441E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -33447,11 +33461,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14790230195290038</v>
+        <v>0.15030386798577866</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0092920436395786E-2</v>
+        <v>1.2131579165104656E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -33460,11 +33474,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15629639624326067</v>
+        <v>0.16227852032526702</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3940942903602822E-3</v>
+        <v>1.1974652339488356E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -33473,11 +33487,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16405536932531875</v>
+        <v>0.1728642212256131</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>7.7589730820580849E-3</v>
+        <v>1.0585700900346079E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -33486,11 +33500,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17534051897497396</v>
+        <v>0.18168051816520628</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1285149649655213E-2</v>
+        <v>8.8162969395931823E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -33499,11 +33513,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1861593822249612</v>
+        <v>0.19098058792892117</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0818863249987237E-2</v>
+        <v>9.300069763714891E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test interrupt dans le code
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F89DADB-274B-4DC4-B123-B369A61FD8EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{735E73A8-6B79-4A1C-A99F-7D2C69CB6405}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -1696,6 +1696,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1712,9 +1715,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -30476,8 +30476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97D1C501-6ABF-4FF7-B1E1-C49F27E96A4F}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -30510,13 +30510,13 @@
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C2" s="92" t="s">
+      <c r="C2" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="D2" s="92" t="s">
+      <c r="D2" s="93" t="s">
         <v>202</v>
       </c>
       <c r="E2" s="76">
@@ -30525,13 +30525,13 @@
       <c r="F2" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="92" t="s">
+      <c r="J2" s="93" t="s">
         <v>203</v>
       </c>
-      <c r="K2" s="92" t="s">
+      <c r="K2" s="93" t="s">
         <v>208</v>
       </c>
-      <c r="L2" s="92" t="s">
+      <c r="L2" s="93" t="s">
         <v>209</v>
       </c>
       <c r="M2" s="76">
@@ -30540,67 +30540,67 @@
       <c r="N2" s="76"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="96"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
       <c r="E3" s="68">
         <v>2</v>
       </c>
       <c r="F3" s="86" t="s">
         <v>256</v>
       </c>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
+      <c r="L3" s="94"/>
       <c r="M3" s="68">
         <v>2</v>
       </c>
       <c r="N3" s="68"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="96"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="94"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="68">
         <v>3</v>
       </c>
       <c r="F4" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="93"/>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
+      <c r="L4" s="94"/>
       <c r="M4" s="68">
         <v>3</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="97"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="95"/>
       <c r="E5" s="77">
         <v>4</v>
       </c>
       <c r="F5" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="J5" s="93"/>
-      <c r="K5" s="93"/>
-      <c r="L5" s="93"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="94"/>
       <c r="M5" s="68">
         <v>4</v>
       </c>
       <c r="N5" s="68"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="95" t="s">
+      <c r="B6" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="D6" s="92" t="s">
+      <c r="D6" s="93" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="76">
@@ -30609,31 +30609,31 @@
       <c r="F6" s="82" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
       <c r="M6" s="77">
         <v>5</v>
       </c>
       <c r="N6" s="77"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B7" s="96"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
+      <c r="B7" s="97"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
       <c r="E7" s="68">
         <v>2</v>
       </c>
       <c r="F7" s="86" t="s">
         <v>280</v>
       </c>
-      <c r="J7" s="92" t="s">
+      <c r="J7" s="93" t="s">
         <v>203</v>
       </c>
-      <c r="K7" s="92" t="s">
+      <c r="K7" s="93" t="s">
         <v>208</v>
       </c>
-      <c r="L7" s="92" t="s">
+      <c r="L7" s="93" t="s">
         <v>210</v>
       </c>
       <c r="M7" s="76">
@@ -30644,18 +30644,18 @@
       </c>
     </row>
     <row r="8" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="97"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
       <c r="E8" s="77">
         <v>3</v>
       </c>
       <c r="F8" s="80" t="s">
         <v>201</v>
       </c>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
       <c r="M8" s="68">
         <v>2</v>
       </c>
@@ -30664,13 +30664,13 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="95" t="s">
+      <c r="B9" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="93" t="s">
         <v>279</v>
       </c>
       <c r="E9" s="76">
@@ -30679,9 +30679,9 @@
       <c r="F9" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
       <c r="M9" s="77">
         <v>3</v>
       </c>
@@ -30690,22 +30690,22 @@
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B10" s="96"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="94"/>
       <c r="E10" s="68">
         <v>2</v>
       </c>
       <c r="F10" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="J10" s="92" t="s">
+      <c r="J10" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="K10" s="92" t="s">
+      <c r="K10" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="L10" s="92" t="s">
+      <c r="L10" s="93" t="s">
         <v>212</v>
       </c>
       <c r="M10">
@@ -30716,18 +30716,18 @@
       </c>
     </row>
     <row r="11" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="96"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
+      <c r="B11" s="97"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="94"/>
       <c r="E11" s="68">
         <v>3</v>
       </c>
       <c r="F11" s="81" t="s">
         <v>201</v>
       </c>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-      <c r="L11" s="98"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
       <c r="M11">
         <v>2</v>
       </c>
@@ -30736,22 +30736,22 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="97"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="95"/>
       <c r="E12" s="77">
         <v>4</v>
       </c>
       <c r="F12" s="83" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="92" t="s">
+      <c r="J12" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="K12" s="92" t="s">
+      <c r="K12" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="L12" s="92" t="s">
+      <c r="L12" s="93" t="s">
         <v>213</v>
       </c>
       <c r="M12" s="76">
@@ -30762,13 +30762,13 @@
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C13" s="92" t="s">
+      <c r="C13" s="93" t="s">
         <v>206</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="93" t="s">
         <v>191</v>
       </c>
       <c r="E13" s="76">
@@ -30777,9 +30777,9 @@
       <c r="F13" s="84" t="s">
         <v>159</v>
       </c>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
+      <c r="J13" s="94"/>
+      <c r="K13" s="94"/>
+      <c r="L13" s="94"/>
       <c r="M13" s="68">
         <v>2</v>
       </c>
@@ -30788,9 +30788,9 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="96"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
+      <c r="B14" s="97"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="94"/>
       <c r="E14" s="68">
         <v>2</v>
       </c>
@@ -30799,9 +30799,9 @@
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="96"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
       <c r="E15" s="68">
         <v>3</v>
       </c>
@@ -30810,9 +30810,9 @@
       </c>
     </row>
     <row r="16" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="97"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
       <c r="E16" s="77">
         <v>4</v>
       </c>
@@ -30821,13 +30821,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C17" s="92" t="s">
+      <c r="C17" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="93" t="s">
         <v>277</v>
       </c>
       <c r="E17" s="76">
@@ -30841,9 +30841,9 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="96"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
       <c r="E18" s="68">
         <v>2</v>
       </c>
@@ -30855,9 +30855,9 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="96"/>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
+      <c r="B19" s="97"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
       <c r="E19" s="68">
         <v>3</v>
       </c>
@@ -30869,9 +30869,9 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="96"/>
-      <c r="C20" s="93"/>
-      <c r="D20" s="93"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="94"/>
+      <c r="D20" s="94"/>
       <c r="E20" s="68">
         <v>4</v>
       </c>
@@ -30883,9 +30883,9 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="96"/>
-      <c r="C21" s="93"/>
-      <c r="D21" s="93"/>
+      <c r="B21" s="97"/>
+      <c r="C21" s="94"/>
+      <c r="D21" s="94"/>
       <c r="E21" s="68">
         <v>5</v>
       </c>
@@ -30897,9 +30897,9 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="97"/>
-      <c r="C22" s="94"/>
-      <c r="D22" s="94"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
       <c r="E22" s="77">
         <v>6</v>
       </c>
@@ -30911,13 +30911,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="95" t="s">
+      <c r="B23" s="96" t="s">
         <v>200</v>
       </c>
-      <c r="C23" s="92" t="s">
+      <c r="C23" s="93" t="s">
         <v>207</v>
       </c>
-      <c r="D23" s="92" t="s">
+      <c r="D23" s="93" t="s">
         <v>184</v>
       </c>
       <c r="E23" s="76">
@@ -30931,9 +30931,9 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24" s="96"/>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
+      <c r="B24" s="97"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
       <c r="E24" s="68">
         <v>2</v>
       </c>
@@ -30945,9 +30945,9 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="97"/>
-      <c r="C25" s="94"/>
-      <c r="D25" s="94"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
       <c r="E25" s="77">
         <v>3</v>
       </c>
@@ -30970,7 +30970,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="92" t="s">
         <v>70</v>
       </c>
       <c r="B30" s="84" t="s">
@@ -30984,7 +30984,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="98"/>
+      <c r="A31" s="92"/>
       <c r="B31" s="85" t="s">
         <v>160</v>
       </c>
@@ -30996,7 +30996,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="98"/>
+      <c r="A32" s="92"/>
       <c r="B32" s="81" t="s">
         <v>201</v>
       </c>
@@ -31008,7 +31008,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="98"/>
+      <c r="A33" s="92"/>
       <c r="B33" s="90" t="s">
         <v>183</v>
       </c>
@@ -31020,7 +31020,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="98" t="s">
+      <c r="A34" s="92" t="s">
         <v>191</v>
       </c>
       <c r="B34" s="84" t="s">
@@ -31034,7 +31034,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="98"/>
+      <c r="A35" s="92"/>
       <c r="B35" s="85" t="s">
         <v>160</v>
       </c>
@@ -31046,7 +31046,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="98"/>
+      <c r="A36" s="92"/>
       <c r="B36" s="81" t="s">
         <v>201</v>
       </c>
@@ -31058,7 +31058,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="98"/>
+      <c r="A37" s="92"/>
       <c r="B37" s="83" t="s">
         <v>278</v>
       </c>
@@ -31071,6 +31071,22 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="L2:L6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C17:C22"/>
+    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="D2:D5"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="D6:D8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="D13:D16"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A37"/>
     <mergeCell ref="L12:L13"/>
@@ -31087,22 +31103,6 @@
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="K7:K9"/>
     <mergeCell ref="J7:J9"/>
-    <mergeCell ref="L2:L6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C17:C22"/>
-    <mergeCell ref="B17:B22"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="D2:D5"/>
-    <mergeCell ref="C2:C5"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="D13:D16"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -31115,8 +31115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:L27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -31153,7 +31153,7 @@
       <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="98" t="s">
+      <c r="J3" s="92" t="s">
         <v>161</v>
       </c>
       <c r="K3" t="s">
@@ -31173,7 +31173,7 @@
       <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="98"/>
+      <c r="J4" s="92"/>
       <c r="K4" t="s">
         <v>191</v>
       </c>
@@ -31200,7 +31200,7 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="98"/>
+      <c r="J5" s="92"/>
       <c r="K5" t="s">
         <v>70</v>
       </c>
@@ -31225,7 +31225,7 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="98"/>
+      <c r="J6" s="92"/>
       <c r="K6" t="s">
         <v>182</v>
       </c>
@@ -31921,7 +31921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526E76B6-68A2-48DF-95E8-365FAB976DDF}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -33005,11 +33005,11 @@
         <v>254</v>
       </c>
       <c r="B38">
-        <f>B37+4</f>
+        <f t="shared" ref="B38:C40" si="23">B37+4</f>
         <v>52</v>
       </c>
       <c r="C38">
-        <f>C37+4</f>
+        <f t="shared" si="23"/>
         <v>55</v>
       </c>
       <c r="D38" t="s">
@@ -33036,11 +33036,11 @@
         <v>255</v>
       </c>
       <c r="B39">
-        <f>B38+4</f>
+        <f t="shared" si="23"/>
         <v>56</v>
       </c>
       <c r="C39">
-        <f>C38+4</f>
+        <f t="shared" si="23"/>
         <v>59</v>
       </c>
       <c r="D39" t="s">
@@ -33064,11 +33064,11 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B40">
-        <f>B39+4</f>
+        <f t="shared" si="23"/>
         <v>60</v>
       </c>
       <c r="C40">
-        <f>C39+4</f>
+        <f t="shared" si="23"/>
         <v>63</v>
       </c>
     </row>
@@ -33245,7 +33245,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.0051609890995851E-2</v>
+        <v>9.8732050932364493E-3</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -33260,7 +33260,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>99.486550994760719</v>
+        <v>101.28423248140982</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -33272,18 +33272,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>1.291265385046139E-2</v>
+        <v>1.1956318822002165E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>1.291265385046139E-2</v>
+        <v>1.1956318822002165E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-5.1344900523928065E-3</v>
+        <v>1.2842324814098163E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -33292,11 +33292,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.106675714830844E-2</v>
+        <v>2.1694553104806506E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>8.1541032978470502E-3</v>
+        <v>9.7382342828043408E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -33305,11 +33305,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9862774500316106E-2</v>
+        <v>2.9495779755394233E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>8.7960173520076658E-3</v>
+        <v>7.8012266505877274E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -33318,11 +33318,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.0341745761296809E-2</v>
+        <v>3.9203290683806978E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0478971260980702E-2</v>
+        <v>9.707510928412745E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -33331,11 +33331,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.2686771903536211E-2</v>
+        <v>4.7221631374983336E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2345026142239403E-2</v>
+        <v>8.018340691176358E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -33344,11 +33344,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.218470307830732E-2</v>
+        <v>5.8111045038033153E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4979311747711084E-3</v>
+        <v>1.0889413663049817E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -33357,11 +33357,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.0240866834778204E-2</v>
+        <v>6.7438554478885027E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0561637564708841E-3</v>
+        <v>9.3275094408518736E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -33370,11 +33370,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7778402694171467E-2</v>
+        <v>7.4763934677148064E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5375358593932629E-3</v>
+        <v>7.3253801982630373E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -33383,11 +33383,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8930854158608158E-2</v>
+        <v>8.296880988139417E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1152451464436691E-2</v>
+        <v>8.2048752042461065E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -33396,11 +33396,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8135539498220806E-2</v>
+        <v>9.4424854485291893E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2046853396126477E-3</v>
+        <v>1.1456044603897722E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -33409,11 +33409,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10889480482865095</v>
+        <v>0.10738386898444177</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0759265330430146E-2</v>
+        <v>1.2959014499149879E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -33422,11 +33422,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11772823905109414</v>
+        <v>0.11575784391098649</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.83343422244319E-3</v>
+        <v>8.3739749265447222E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -33435,11 +33435,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12948176619920576</v>
+        <v>0.127738284328414</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.175352714811162E-2</v>
+        <v>1.1980440417427504E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -33448,11 +33448,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13817228882067401</v>
+        <v>0.13679910082977542</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6905226214682441E-3</v>
+        <v>9.0608165013614239E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -33461,11 +33461,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15030386798577866</v>
+        <v>0.14841544781695951</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2131579165104656E-2</v>
+        <v>1.1616346987184084E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -33474,11 +33474,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16227852032526702</v>
+        <v>0.15851095763339867</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1974652339488356E-2</v>
+        <v>1.0095509816439169E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -33487,11 +33487,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1728642212256131</v>
+        <v>0.16812236898102237</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0585700900346079E-2</v>
+        <v>9.611411347623694E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -33500,11 +33500,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18168051816520628</v>
+        <v>0.18033640390292344</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8162969395931823E-3</v>
+        <v>1.2214034921901068E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -33513,11 +33513,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19098058792892117</v>
+        <v>0.18759089677149254</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>9.300069763714891E-3</v>
+        <v>7.2544928685691068E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sd et adafruit IO sur receiver v2
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505EE4C0-3CA6-4EC9-A3F0-EE2595FF5665}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A1238F-ECD1-48F6-84CB-D6F4E8062AAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-948" yWindow="10620" windowWidth="13824" windowHeight="7176" activeTab="1" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -1864,9 +1864,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1883,6 +1880,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -23195,6 +23195,55 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>324999</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>148918</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{171C7F47-00B1-4119-B970-2CBF59C632A6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5989320" y="388620"/>
+          <a:ext cx="4637919" cy="3600778"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
@@ -23308,7 +23357,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -23956,7 +24005,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -26669,7 +26718,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -26746,7 +26795,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -47599,8 +47648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C7B145-5B10-4776-B200-74A4976CCC04}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47798,6 +47847,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -52948,13 +52998,13 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="103" t="s">
         <v>197</v>
       </c>
       <c r="E3" s="76">
@@ -52965,13 +53015,13 @@
       </c>
       <c r="G3" s="76"/>
       <c r="H3" s="76"/>
-      <c r="J3" s="104" t="s">
+      <c r="J3" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="104" t="s">
+      <c r="K3" s="103" t="s">
         <v>203</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="103" t="s">
         <v>204</v>
       </c>
       <c r="M3" s="76">
@@ -52980,9 +53030,9 @@
       <c r="N3" s="76"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
       <c r="E4" s="68">
         <v>2</v>
       </c>
@@ -52991,18 +53041,18 @@
       </c>
       <c r="G4" s="68"/>
       <c r="H4" s="68"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
+      <c r="J4" s="104"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
       <c r="M4" s="68">
         <v>2</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="108"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="104"/>
+      <c r="D5" s="104"/>
       <c r="E5" s="68">
         <v>3</v>
       </c>
@@ -53011,18 +53061,18 @@
       </c>
       <c r="G5" s="68"/>
       <c r="H5" s="68"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
+      <c r="J5" s="104"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
       <c r="M5" s="68">
         <v>3</v>
       </c>
       <c r="N5" s="68"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="109"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
+      <c r="B6" s="108"/>
+      <c r="C6" s="105"/>
+      <c r="D6" s="105"/>
       <c r="E6" s="77">
         <v>4</v>
       </c>
@@ -53031,22 +53081,22 @@
       </c>
       <c r="G6" s="77"/>
       <c r="H6" s="77"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
+      <c r="J6" s="104"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
       <c r="M6" s="68">
         <v>4</v>
       </c>
       <c r="N6" s="68"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="103" t="s">
         <v>176</v>
       </c>
       <c r="E7" s="76">
@@ -53059,18 +53109,18 @@
         <v>284</v>
       </c>
       <c r="H7" s="76"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
+      <c r="J7" s="105"/>
+      <c r="K7" s="105"/>
+      <c r="L7" s="105"/>
       <c r="M7" s="77">
         <v>5</v>
       </c>
       <c r="N7" s="77"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="108"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="104"/>
+      <c r="D8" s="104"/>
       <c r="E8" s="68">
         <v>2</v>
       </c>
@@ -53081,13 +53131,13 @@
         <v>292</v>
       </c>
       <c r="H8" s="68"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="103" t="s">
         <v>198</v>
       </c>
-      <c r="K8" s="104" t="s">
+      <c r="K8" s="103" t="s">
         <v>203</v>
       </c>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="103" t="s">
         <v>205</v>
       </c>
       <c r="M8" s="76">
@@ -53098,9 +53148,9 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="109"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="105"/>
+      <c r="D9" s="105"/>
       <c r="E9" s="77">
         <v>3</v>
       </c>
@@ -53111,9 +53161,9 @@
         <v>283</v>
       </c>
       <c r="H9" s="77"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
+      <c r="J9" s="104"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="104"/>
       <c r="M9" s="68">
         <v>2</v>
       </c>
@@ -53122,13 +53172,13 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="103" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="76">
@@ -53143,9 +53193,9 @@
       <c r="H10" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J10" s="106"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="106"/>
+      <c r="J10" s="105"/>
+      <c r="K10" s="105"/>
+      <c r="L10" s="105"/>
       <c r="M10" s="77">
         <v>3</v>
       </c>
@@ -53154,9 +53204,9 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="108"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="104"/>
+      <c r="D11" s="104"/>
       <c r="E11" s="68">
         <v>2</v>
       </c>
@@ -53169,13 +53219,13 @@
       <c r="H11" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="J11" s="104" t="s">
+      <c r="J11" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="103" t="s">
         <v>206</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="103" t="s">
         <v>207</v>
       </c>
       <c r="M11">
@@ -53186,9 +53236,9 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="108"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
+      <c r="B12" s="107"/>
+      <c r="C12" s="104"/>
+      <c r="D12" s="104"/>
       <c r="E12" s="68">
         <v>3</v>
       </c>
@@ -53201,9 +53251,9 @@
       <c r="H12" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
+      <c r="J12" s="109"/>
+      <c r="K12" s="109"/>
+      <c r="L12" s="109"/>
       <c r="M12">
         <v>2</v>
       </c>
@@ -53212,9 +53262,9 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="109"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
+      <c r="B13" s="108"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
       <c r="E13" s="77">
         <v>4</v>
       </c>
@@ -53227,13 +53277,13 @@
       <c r="H13" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="J13" s="104" t="s">
+      <c r="J13" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="K13" s="104" t="s">
+      <c r="K13" s="103" t="s">
         <v>206</v>
       </c>
-      <c r="L13" s="104" t="s">
+      <c r="L13" s="103" t="s">
         <v>208</v>
       </c>
       <c r="M13" s="76">
@@ -53244,13 +53294,13 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="103" t="s">
         <v>177</v>
       </c>
       <c r="E14" s="76">
@@ -53265,16 +53315,16 @@
       <c r="H14" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
+      <c r="J14" s="104"/>
+      <c r="K14" s="104"/>
+      <c r="L14" s="104"/>
       <c r="M14" s="68"/>
       <c r="N14" s="68"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="108"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
       <c r="E15" s="68">
         <v>2</v>
       </c>
@@ -53287,16 +53337,16 @@
       <c r="H15" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
+      <c r="J15" s="104"/>
+      <c r="K15" s="104"/>
+      <c r="L15" s="104"/>
       <c r="M15" s="68"/>
       <c r="N15" s="68"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="108"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="104"/>
+      <c r="D16" s="104"/>
       <c r="E16" s="68">
         <v>3</v>
       </c>
@@ -53309,16 +53359,16 @@
       <c r="H16" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
+      <c r="J16" s="104"/>
+      <c r="K16" s="104"/>
+      <c r="L16" s="104"/>
       <c r="M16" s="68"/>
       <c r="N16" s="68"/>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="109"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="105"/>
+      <c r="D17" s="105"/>
       <c r="E17" s="77">
         <v>4</v>
       </c>
@@ -53331,20 +53381,20 @@
       <c r="H17" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="104"/>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="103" t="s">
         <v>201</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="103" t="s">
         <v>186</v>
       </c>
       <c r="E18" s="76">
@@ -53359,9 +53409,9 @@
       <c r="H18" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
+      <c r="J18" s="104"/>
+      <c r="K18" s="104"/>
+      <c r="L18" s="104"/>
       <c r="M18" s="68">
         <v>2</v>
       </c>
@@ -53370,9 +53420,9 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="108"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
+      <c r="B19" s="107"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="104"/>
       <c r="E19" s="68">
         <v>2</v>
       </c>
@@ -53387,9 +53437,9 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="108"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="104"/>
       <c r="E20" s="68">
         <v>3</v>
       </c>
@@ -53404,9 +53454,9 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="109"/>
-      <c r="C21" s="106"/>
-      <c r="D21" s="106"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="105"/>
+      <c r="D21" s="105"/>
       <c r="E21" s="77">
         <v>4</v>
       </c>
@@ -53421,13 +53471,13 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="104" t="s">
+      <c r="D22" s="103" t="s">
         <v>270</v>
       </c>
       <c r="E22" s="76">
@@ -53442,9 +53492,9 @@
       <c r="H22" s="76"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="108"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
+      <c r="B23" s="107"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
       <c r="E23" s="68">
         <v>2</v>
       </c>
@@ -53457,9 +53507,9 @@
       <c r="H23" s="68"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="108"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
+      <c r="B24" s="107"/>
+      <c r="C24" s="104"/>
+      <c r="D24" s="104"/>
       <c r="E24" s="68">
         <v>3</v>
       </c>
@@ -53472,9 +53522,9 @@
       <c r="H24" s="68"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="108"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
+      <c r="B25" s="107"/>
+      <c r="C25" s="104"/>
+      <c r="D25" s="104"/>
       <c r="E25" s="68">
         <v>4</v>
       </c>
@@ -53487,9 +53537,9 @@
       <c r="H25" s="68"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="108"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
+      <c r="B26" s="107"/>
+      <c r="C26" s="104"/>
+      <c r="D26" s="104"/>
       <c r="E26" s="68">
         <v>5</v>
       </c>
@@ -53502,9 +53552,9 @@
       <c r="H26" s="68"/>
     </row>
     <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="109"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="105"/>
+      <c r="D27" s="105"/>
       <c r="E27" s="77">
         <v>6</v>
       </c>
@@ -53517,13 +53567,13 @@
       <c r="H27" s="77"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="106" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C28" s="103" t="s">
         <v>202</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="103" t="s">
         <v>179</v>
       </c>
       <c r="E28" s="76">
@@ -53538,9 +53588,9 @@
       <c r="H28" s="76"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="108"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="104"/>
+      <c r="D29" s="104"/>
       <c r="E29" s="68">
         <v>2</v>
       </c>
@@ -53553,9 +53603,9 @@
       <c r="H29" s="68"/>
     </row>
     <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="109"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
+      <c r="B30" s="108"/>
+      <c r="C30" s="105"/>
+      <c r="D30" s="105"/>
       <c r="E30" s="77">
         <v>3</v>
       </c>
@@ -53579,7 +53629,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="103" t="s">
+      <c r="A35" s="109" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="82" t="s">
@@ -53593,7 +53643,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="103"/>
+      <c r="A36" s="109"/>
       <c r="B36" s="83" t="s">
         <v>155</v>
       </c>
@@ -53605,7 +53655,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="103"/>
+      <c r="A37" s="109"/>
       <c r="B37" s="80" t="s">
         <v>196</v>
       </c>
@@ -53617,7 +53667,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="103"/>
+      <c r="A38" s="109"/>
       <c r="B38" s="86" t="s">
         <v>178</v>
       </c>
@@ -53629,7 +53679,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="103" t="s">
+      <c r="A39" s="109" t="s">
         <v>186</v>
       </c>
       <c r="B39" s="82" t="s">
@@ -53643,7 +53693,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="103"/>
+      <c r="A40" s="109"/>
       <c r="B40" s="83" t="s">
         <v>155</v>
       </c>
@@ -53655,7 +53705,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="103"/>
+      <c r="A41" s="109"/>
       <c r="B41" s="80" t="s">
         <v>196</v>
       </c>
@@ -53667,7 +53717,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="103"/>
+      <c r="A42" s="109"/>
       <c r="B42" s="81" t="s">
         <v>271</v>
       </c>
@@ -53680,25 +53730,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D14:D17"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="L13:L18"/>
@@ -53715,6 +53746,25 @@
     <mergeCell ref="L8:L10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="D22:D27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G3:H13 G18:H30">
@@ -53799,7 +53849,7 @@
       <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="109" t="s">
         <v>156</v>
       </c>
       <c r="K3" t="s">
@@ -53819,7 +53869,7 @@
       <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="103"/>
+      <c r="J4" s="109"/>
       <c r="K4" t="s">
         <v>186</v>
       </c>
@@ -53846,7 +53896,7 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="103"/>
+      <c r="J5" s="109"/>
       <c r="K5" t="s">
         <v>70</v>
       </c>
@@ -53871,7 +53921,7 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="103"/>
+      <c r="J6" s="109"/>
       <c r="K6" t="s">
         <v>177</v>
       </c>
@@ -55893,7 +55943,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.7634659255523611E-3</v>
+        <v>1.0658505663181128E-2</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -55908,7 +55958,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>102.42264454294448</v>
+        <v>93.821782490055071</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -55920,18 +55970,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>1.1172021563293621E-2</v>
+        <v>1.1632443647707626E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>1.1172021563293621E-2</v>
+        <v>1.1632443647707626E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>2.4226445429444823E-2</v>
+        <v>-6.1782175099449291E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -55940,11 +55990,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.2596911117739166E-2</v>
+        <v>2.2994393040451876E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.1424889554445546E-2</v>
+        <v>1.136194939274425E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -55953,11 +56003,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1622805453820457E-2</v>
+        <v>3.1056310665964305E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>9.0258943360812909E-3</v>
+        <v>8.0619176255124284E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -55966,11 +56016,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.1130321821549409E-2</v>
+        <v>3.9250518522211744E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.507516367728952E-3</v>
+        <v>8.1942078562474395E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -55979,11 +56029,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.1143304792457052E-2</v>
+        <v>4.9090183580146753E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0012982970907643E-2</v>
+        <v>9.8396650579350084E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -55992,11 +56042,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.103621176537375E-2</v>
+        <v>6.1832360582107351E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8929069729166985E-3</v>
+        <v>1.2742177001960599E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -56005,11 +56055,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.8391623155258499E-2</v>
+        <v>7.0803144297631751E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3554113898847487E-3</v>
+        <v>8.9707837155243997E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -56018,11 +56068,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.014319276934502E-2</v>
+        <v>8.3551258913263482E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1751569614086521E-2</v>
+        <v>1.2748114615631731E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -56031,11 +56081,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8076686245579253E-2</v>
+        <v>9.6313033093838901E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9334934762342324E-3</v>
+        <v>1.2761774180575419E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -56044,11 +56094,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8087260557275416E-2</v>
+        <v>0.10585321440857554</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0010574311696163E-2</v>
+        <v>9.5401813147366343E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -56057,11 +56107,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10576656291658432</v>
+        <v>0.11706279500405965</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.679302359308901E-3</v>
+        <v>1.1209580595484117E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -56070,11 +56120,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11465287600310954</v>
+        <v>0.13003676934641004</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8863130865252243E-3</v>
+        <v>1.2973974342350383E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -56083,11 +56133,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12299280840383767</v>
+        <v>0.14003045902143196</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.3399324007281256E-3</v>
+        <v>9.9936896750219273E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -56096,11 +56146,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13166245420702519</v>
+        <v>0.15219893228662651</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.6696458031875201E-3</v>
+        <v>1.2168473265194546E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -56109,11 +56159,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13986663404244976</v>
+        <v>0.16383384166195283</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2041798354245687E-3</v>
+        <v>1.1634909375326324E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -56122,11 +56172,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15056034170019186</v>
+        <v>0.17421516441022744</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0693707657742108E-2</v>
+        <v>1.0381322748274607E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -56135,11 +56185,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16153096735208206</v>
+        <v>0.18319773390206939</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0970625651890192E-2</v>
+        <v>8.9825694918419519E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -56148,11 +56198,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.173284671186485</v>
+        <v>0.19196738381427733</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.175370383440294E-2</v>
+        <v>8.7696499122079385E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -56161,11 +56211,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18550585258549487</v>
+        <v>0.20251160760044146</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2221181399009878E-2</v>
+        <v>1.0544223786164125E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
display and save on a other library
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\service cloud\OneDrive\Documents\5.Bricolage\5.StationMeteo\StationMeteo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4DEA8F9-FECF-4508-898F-D5A65320F945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F98DBA7-53B2-4003-8019-AB278A2AE038}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="5" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="3" activeTab="5" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -1897,11 +1897,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1921,6 +1920,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1930,8 +1932,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Insatisfaisant" xfId="6" builtinId="27"/>
@@ -31648,21 +31648,21 @@
       <c r="H1" s="2"/>
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="104" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="102"/>
+      <c r="C2" s="104"/>
       <c r="D2" s="64">
         <f>SUM(D5:D22)</f>
         <v>534.23</v>
       </c>
       <c r="E2" s="63"/>
       <c r="F2" s="65"/>
-      <c r="G2" s="102" t="s">
+      <c r="G2" s="104" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
+      <c r="H2" s="104"/>
+      <c r="I2" s="104"/>
       <c r="J2" s="64">
         <f>SUM(J5:J19)</f>
         <v>0</v>
@@ -57386,13 +57386,13 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="107" t="s">
+      <c r="B3" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C3" s="104" t="s">
+      <c r="C3" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D3" s="104" t="s">
+      <c r="D3" s="105" t="s">
         <v>197</v>
       </c>
       <c r="E3" s="76">
@@ -57403,13 +57403,13 @@
       </c>
       <c r="G3" s="76"/>
       <c r="H3" s="76"/>
-      <c r="J3" s="104" t="s">
+      <c r="J3" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="K3" s="104" t="s">
+      <c r="K3" s="105" t="s">
         <v>203</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="105" t="s">
         <v>204</v>
       </c>
       <c r="M3" s="76">
@@ -57418,9 +57418,9 @@
       <c r="N3" s="76"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="108"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
+      <c r="B4" s="109"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
       <c r="E4" s="68">
         <v>2</v>
       </c>
@@ -57429,18 +57429,18 @@
       </c>
       <c r="G4" s="68"/>
       <c r="H4" s="68"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
       <c r="M4" s="68">
         <v>2</v>
       </c>
       <c r="N4" s="68"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="108"/>
-      <c r="C5" s="105"/>
-      <c r="D5" s="105"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="106"/>
       <c r="E5" s="68">
         <v>3</v>
       </c>
@@ -57449,18 +57449,18 @@
       </c>
       <c r="G5" s="68"/>
       <c r="H5" s="68"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="105"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
       <c r="M5" s="68">
         <v>3</v>
       </c>
       <c r="N5" s="68"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="109"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="106"/>
+      <c r="B6" s="110"/>
+      <c r="C6" s="107"/>
+      <c r="D6" s="107"/>
       <c r="E6" s="77">
         <v>4</v>
       </c>
@@ -57469,22 +57469,22 @@
       </c>
       <c r="G6" s="77"/>
       <c r="H6" s="77"/>
-      <c r="J6" s="105"/>
-      <c r="K6" s="105"/>
-      <c r="L6" s="105"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
       <c r="M6" s="68">
         <v>4</v>
       </c>
       <c r="N6" s="68"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="107" t="s">
+      <c r="B7" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D7" s="104" t="s">
+      <c r="D7" s="105" t="s">
         <v>176</v>
       </c>
       <c r="E7" s="76">
@@ -57497,18 +57497,18 @@
         <v>284</v>
       </c>
       <c r="H7" s="76"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
+      <c r="J7" s="107"/>
+      <c r="K7" s="107"/>
+      <c r="L7" s="107"/>
       <c r="M7" s="77">
         <v>5</v>
       </c>
       <c r="N7" s="77"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="108"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
+      <c r="B8" s="109"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="106"/>
       <c r="E8" s="68">
         <v>2</v>
       </c>
@@ -57519,13 +57519,13 @@
         <v>292</v>
       </c>
       <c r="H8" s="68"/>
-      <c r="J8" s="104" t="s">
+      <c r="J8" s="105" t="s">
         <v>198</v>
       </c>
-      <c r="K8" s="104" t="s">
+      <c r="K8" s="105" t="s">
         <v>203</v>
       </c>
-      <c r="L8" s="104" t="s">
+      <c r="L8" s="105" t="s">
         <v>205</v>
       </c>
       <c r="M8" s="76">
@@ -57536,9 +57536,9 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="109"/>
-      <c r="C9" s="106"/>
-      <c r="D9" s="106"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
       <c r="E9" s="77">
         <v>3</v>
       </c>
@@ -57549,9 +57549,9 @@
         <v>283</v>
       </c>
       <c r="H9" s="77"/>
-      <c r="J9" s="105"/>
-      <c r="K9" s="105"/>
-      <c r="L9" s="105"/>
+      <c r="J9" s="106"/>
+      <c r="K9" s="106"/>
+      <c r="L9" s="106"/>
       <c r="M9" s="68">
         <v>2</v>
       </c>
@@ -57560,13 +57560,13 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="107" t="s">
+      <c r="B10" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C10" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D10" s="104" t="s">
+      <c r="D10" s="105" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="76">
@@ -57581,9 +57581,9 @@
       <c r="H10" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J10" s="106"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="106"/>
+      <c r="J10" s="107"/>
+      <c r="K10" s="107"/>
+      <c r="L10" s="107"/>
       <c r="M10" s="77">
         <v>3</v>
       </c>
@@ -57592,9 +57592,9 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="108"/>
-      <c r="C11" s="105"/>
-      <c r="D11" s="105"/>
+      <c r="B11" s="109"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="106"/>
       <c r="E11" s="68">
         <v>2</v>
       </c>
@@ -57607,13 +57607,13 @@
       <c r="H11" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="J11" s="104" t="s">
+      <c r="J11" s="105" t="s">
         <v>202</v>
       </c>
-      <c r="K11" s="104" t="s">
+      <c r="K11" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="L11" s="104" t="s">
+      <c r="L11" s="105" t="s">
         <v>207</v>
       </c>
       <c r="M11">
@@ -57624,9 +57624,9 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="108"/>
-      <c r="C12" s="105"/>
-      <c r="D12" s="105"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="106"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="68">
         <v>3</v>
       </c>
@@ -57639,9 +57639,9 @@
       <c r="H12" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="J12" s="103"/>
-      <c r="K12" s="103"/>
-      <c r="L12" s="103"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
+      <c r="L12" s="111"/>
       <c r="M12">
         <v>2</v>
       </c>
@@ -57650,9 +57650,9 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="109"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
       <c r="E13" s="77">
         <v>4</v>
       </c>
@@ -57665,13 +57665,13 @@
       <c r="H13" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="J13" s="104" t="s">
+      <c r="J13" s="105" t="s">
         <v>202</v>
       </c>
-      <c r="K13" s="104" t="s">
+      <c r="K13" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="L13" s="104" t="s">
+      <c r="L13" s="105" t="s">
         <v>208</v>
       </c>
       <c r="M13" s="76">
@@ -57682,13 +57682,13 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D14" s="104" t="s">
+      <c r="D14" s="105" t="s">
         <v>177</v>
       </c>
       <c r="E14" s="76">
@@ -57703,16 +57703,16 @@
       <c r="H14" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
+      <c r="J14" s="106"/>
+      <c r="K14" s="106"/>
+      <c r="L14" s="106"/>
       <c r="M14" s="68"/>
       <c r="N14" s="68"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="108"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
+      <c r="B15" s="109"/>
+      <c r="C15" s="106"/>
+      <c r="D15" s="106"/>
       <c r="E15" s="68">
         <v>2</v>
       </c>
@@ -57725,16 +57725,16 @@
       <c r="H15" s="68" t="s">
         <v>278</v>
       </c>
-      <c r="J15" s="105"/>
-      <c r="K15" s="105"/>
-      <c r="L15" s="105"/>
+      <c r="J15" s="106"/>
+      <c r="K15" s="106"/>
+      <c r="L15" s="106"/>
       <c r="M15" s="68"/>
       <c r="N15" s="68"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="108"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
+      <c r="B16" s="109"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
       <c r="E16" s="68">
         <v>3</v>
       </c>
@@ -57747,16 +57747,16 @@
       <c r="H16" s="68" t="s">
         <v>277</v>
       </c>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
-      <c r="L16" s="105"/>
+      <c r="J16" s="106"/>
+      <c r="K16" s="106"/>
+      <c r="L16" s="106"/>
       <c r="M16" s="68"/>
       <c r="N16" s="68"/>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="109"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="107"/>
+      <c r="D17" s="107"/>
       <c r="E17" s="77">
         <v>4</v>
       </c>
@@ -57769,20 +57769,20 @@
       <c r="H17" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="J17" s="105"/>
-      <c r="K17" s="105"/>
-      <c r="L17" s="105"/>
+      <c r="J17" s="106"/>
+      <c r="K17" s="106"/>
+      <c r="L17" s="106"/>
       <c r="M17" s="68"/>
       <c r="N17" s="68"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="107" t="s">
+      <c r="B18" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="105" t="s">
         <v>201</v>
       </c>
-      <c r="D18" s="104" t="s">
+      <c r="D18" s="105" t="s">
         <v>186</v>
       </c>
       <c r="E18" s="76">
@@ -57797,9 +57797,9 @@
       <c r="H18" s="76" t="s">
         <v>287</v>
       </c>
-      <c r="J18" s="105"/>
-      <c r="K18" s="105"/>
-      <c r="L18" s="105"/>
+      <c r="J18" s="106"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="106"/>
       <c r="M18" s="68">
         <v>2</v>
       </c>
@@ -57808,9 +57808,9 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="108"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="105"/>
+      <c r="B19" s="109"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
       <c r="E19" s="68">
         <v>2</v>
       </c>
@@ -57825,9 +57825,9 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="108"/>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
+      <c r="B20" s="109"/>
+      <c r="C20" s="106"/>
+      <c r="D20" s="106"/>
       <c r="E20" s="68">
         <v>3</v>
       </c>
@@ -57842,9 +57842,9 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="109"/>
-      <c r="C21" s="106"/>
-      <c r="D21" s="106"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="107"/>
+      <c r="D21" s="107"/>
       <c r="E21" s="77">
         <v>4</v>
       </c>
@@ -57859,13 +57859,13 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C22" s="104" t="s">
+      <c r="C22" s="105" t="s">
         <v>202</v>
       </c>
-      <c r="D22" s="104" t="s">
+      <c r="D22" s="105" t="s">
         <v>270</v>
       </c>
       <c r="E22" s="76">
@@ -57880,9 +57880,9 @@
       <c r="H22" s="76"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="108"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
+      <c r="B23" s="109"/>
+      <c r="C23" s="106"/>
+      <c r="D23" s="106"/>
       <c r="E23" s="68">
         <v>2</v>
       </c>
@@ -57895,9 +57895,9 @@
       <c r="H23" s="68"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="108"/>
-      <c r="C24" s="105"/>
-      <c r="D24" s="105"/>
+      <c r="B24" s="109"/>
+      <c r="C24" s="106"/>
+      <c r="D24" s="106"/>
       <c r="E24" s="68">
         <v>3</v>
       </c>
@@ -57910,9 +57910,9 @@
       <c r="H24" s="68"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="108"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="105"/>
+      <c r="B25" s="109"/>
+      <c r="C25" s="106"/>
+      <c r="D25" s="106"/>
       <c r="E25" s="68">
         <v>4</v>
       </c>
@@ -57925,9 +57925,9 @@
       <c r="H25" s="68"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="108"/>
-      <c r="C26" s="105"/>
-      <c r="D26" s="105"/>
+      <c r="B26" s="109"/>
+      <c r="C26" s="106"/>
+      <c r="D26" s="106"/>
       <c r="E26" s="68">
         <v>5</v>
       </c>
@@ -57940,9 +57940,9 @@
       <c r="H26" s="68"/>
     </row>
     <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="109"/>
-      <c r="C27" s="106"/>
-      <c r="D27" s="106"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="107"/>
+      <c r="D27" s="107"/>
       <c r="E27" s="77">
         <v>6</v>
       </c>
@@ -57955,13 +57955,13 @@
       <c r="H27" s="77"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C28" s="104" t="s">
+      <c r="C28" s="105" t="s">
         <v>202</v>
       </c>
-      <c r="D28" s="104" t="s">
+      <c r="D28" s="105" t="s">
         <v>179</v>
       </c>
       <c r="E28" s="76">
@@ -57976,9 +57976,9 @@
       <c r="H28" s="76"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="108"/>
-      <c r="C29" s="105"/>
-      <c r="D29" s="105"/>
+      <c r="B29" s="109"/>
+      <c r="C29" s="106"/>
+      <c r="D29" s="106"/>
       <c r="E29" s="68">
         <v>2</v>
       </c>
@@ -57991,9 +57991,9 @@
       <c r="H29" s="68"/>
     </row>
     <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="109"/>
-      <c r="C30" s="106"/>
-      <c r="D30" s="106"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="107"/>
+      <c r="D30" s="107"/>
       <c r="E30" s="77">
         <v>3</v>
       </c>
@@ -58017,7 +58017,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="103" t="s">
+      <c r="A35" s="111" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="82" t="s">
@@ -58031,7 +58031,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="103"/>
+      <c r="A36" s="111"/>
       <c r="B36" s="83" t="s">
         <v>155</v>
       </c>
@@ -58043,7 +58043,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="103"/>
+      <c r="A37" s="111"/>
       <c r="B37" s="80" t="s">
         <v>196</v>
       </c>
@@ -58055,7 +58055,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="103"/>
+      <c r="A38" s="111"/>
       <c r="B38" s="86" t="s">
         <v>178</v>
       </c>
@@ -58067,7 +58067,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="103" t="s">
+      <c r="A39" s="111" t="s">
         <v>186</v>
       </c>
       <c r="B39" s="82" t="s">
@@ -58081,7 +58081,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="103"/>
+      <c r="A40" s="111"/>
       <c r="B40" s="83" t="s">
         <v>155</v>
       </c>
@@ -58093,7 +58093,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="103"/>
+      <c r="A41" s="111"/>
       <c r="B41" s="80" t="s">
         <v>196</v>
       </c>
@@ -58105,7 +58105,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="103"/>
+      <c r="A42" s="111"/>
       <c r="B42" s="81" t="s">
         <v>271</v>
       </c>
@@ -58118,25 +58118,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="D22:D27"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D14:D17"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="L13:L18"/>
@@ -58153,6 +58134,25 @@
     <mergeCell ref="L8:L10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="J8:J10"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D14:D17"/>
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="D22:D27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G3:H13 G18:H30">
@@ -58237,7 +58237,7 @@
       <c r="G3" s="69">
         <v>0</v>
       </c>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="111" t="s">
         <v>156</v>
       </c>
       <c r="K3" t="s">
@@ -58257,7 +58257,7 @@
       <c r="G4" s="69">
         <v>1</v>
       </c>
-      <c r="J4" s="103"/>
+      <c r="J4" s="111"/>
       <c r="K4" t="s">
         <v>186</v>
       </c>
@@ -58284,7 +58284,7 @@
       <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="103"/>
+      <c r="J5" s="111"/>
       <c r="K5" t="s">
         <v>70</v>
       </c>
@@ -58309,7 +58309,7 @@
       <c r="H6" t="s">
         <v>74</v>
       </c>
-      <c r="J6" s="103"/>
+      <c r="J6" s="111"/>
       <c r="K6" t="s">
         <v>177</v>
       </c>
@@ -58627,8 +58627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C64E373-7692-4CBF-88B4-6ED8CB4BCA4C}">
   <dimension ref="A1:S245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -58658,13 +58658,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B3" s="111" t="s">
+      <c r="B3" s="113" t="s">
         <v>116</v>
       </c>
-      <c r="C3" s="111"/>
-      <c r="D3" s="111"/>
-      <c r="E3" s="111"/>
-      <c r="F3" s="111"/>
+      <c r="C3" s="113"/>
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="113"/>
       <c r="K3" s="4" t="s">
         <v>19</v>
       </c>
@@ -58679,7 +58679,7 @@
         <f>COUNTIF(P6:P245,"=2")/COUNT(P6:P245)</f>
         <v>0.4</v>
       </c>
-      <c r="R3" s="113"/>
+      <c r="R3" s="102"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -58737,14 +58737,14 @@
         <f>MOD(N6,O$2)</f>
         <v>1</v>
       </c>
-      <c r="S6" s="114"/>
+      <c r="S6" s="103"/>
     </row>
     <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A7" s="111" t="s">
+      <c r="A7" s="113" t="s">
         <v>122</v>
       </c>
-      <c r="B7" s="111"/>
-      <c r="C7" s="111"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
       <c r="D7" t="s">
         <v>130</v>
       </c>
@@ -58763,7 +58763,7 @@
         <f t="shared" ref="R7:R29" si="2">MOD(N7,O$2)</f>
         <v>2</v>
       </c>
-      <c r="S7" s="114"/>
+      <c r="S7" s="103"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -58804,7 +58804,7 @@
       <c r="D9" t="s">
         <v>126</v>
       </c>
-      <c r="K9" s="110" t="s">
+      <c r="K9" s="112" t="s">
         <v>334</v>
       </c>
       <c r="N9">
@@ -58824,7 +58824,7 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K10" s="110"/>
+      <c r="K10" s="112"/>
       <c r="N10">
         <v>5</v>
       </c>
@@ -58842,7 +58842,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="K11" s="110"/>
+      <c r="K11" s="112"/>
       <c r="N11">
         <v>6</v>
       </c>
@@ -58875,7 +58875,7 @@
       <c r="F12" s="42" t="s">
         <v>144</v>
       </c>
-      <c r="K12" s="110"/>
+      <c r="K12" s="112"/>
       <c r="N12">
         <v>7</v>
       </c>
@@ -58911,7 +58911,7 @@
       <c r="G13" s="59" t="s">
         <v>146</v>
       </c>
-      <c r="K13" s="110"/>
+      <c r="K13" s="112"/>
       <c r="N13">
         <v>8</v>
       </c>
@@ -62232,10 +62232,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="114" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="112"/>
+      <c r="B1" s="114"/>
       <c r="D1" t="s">
         <v>269</v>
       </c>
@@ -62878,10 +62878,10 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A22" s="112" t="s">
+      <c r="A22" s="114" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="112"/>
+      <c r="B22" s="114"/>
       <c r="C22" t="s">
         <v>263</v>
       </c>
@@ -63545,7 +63545,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.1082718949271052E-2</v>
+        <v>1.0422644228664443E-2</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -63560,7 +63560,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>90.230565674118566</v>
+        <v>95.944942383219001</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -63572,18 +63572,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>1.2681324326882635E-2</v>
+        <v>7.9919854188129635E-3</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>1.2681324326882635E-2</v>
+        <v>7.9919854188129635E-3</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-9.7694343258814348E-2</v>
+        <v>-4.0550576167809993E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -63592,11 +63592,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1600434277607824E-2</v>
+        <v>1.7972750533567443E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>8.9191099507251893E-3</v>
+        <v>9.9807651147544793E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -63605,11 +63605,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.2963473115538135E-2</v>
+        <v>2.9926145030120251E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.1363038837930311E-2</v>
+        <v>1.1953394496552808E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -63618,11 +63618,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.5194249397483961E-2</v>
+        <v>4.2331081389093098E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2230776281945827E-2</v>
+        <v>1.2404936358972846E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -63631,11 +63631,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7165193551014945E-2</v>
+        <v>5.3524832925377616E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1970944153530984E-2</v>
+        <v>1.1193751536284519E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -63644,11 +63644,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4687789750799585E-2</v>
+        <v>6.5120103415611474E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.5225961997846397E-3</v>
+        <v>1.1595270490233858E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -63657,11 +63657,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3796429195134502E-2</v>
+        <v>7.773547461833355E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1086394443349178E-3</v>
+        <v>1.2615371202722075E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -63670,11 +63670,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.6701156104453878E-2</v>
+        <v>8.6448444127002616E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2904726909319375E-2</v>
+        <v>8.7129695086690662E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -63683,11 +63683,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8821948113513011E-2</v>
+        <v>9.5587742529743114E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2120792009059134E-2</v>
+        <v>9.1392984027404978E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -63696,11 +63696,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1113272376067504</v>
+        <v>0.10410014191718162</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2505289493237384E-2</v>
+        <v>8.5123993874385018E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -63709,11 +63709,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12385767087147538</v>
+        <v>0.11520377705109616</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2530433264724986E-2</v>
+        <v>1.1103635133914547E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -63722,11 +63722,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13567126021317186</v>
+        <v>0.12564214629496234</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1813589341696476E-2</v>
+        <v>1.043836924386618E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -63735,11 +63735,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14743359108481435</v>
+        <v>0.13513911495991784</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1762330871642496E-2</v>
+        <v>9.4969686649555018E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -63748,11 +63748,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15551009929592871</v>
+        <v>0.14398827976518119</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0765082111143582E-3</v>
+        <v>8.8491648052633487E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -63761,11 +63761,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16562045237394515</v>
+        <v>0.15115998837019118</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0110353078016443E-2</v>
+        <v>7.1717086050099854E-3</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -63774,11 +63774,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17858830620713972</v>
+        <v>0.16262083630141083</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.296785383319457E-2</v>
+        <v>1.1460847931219653E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -63787,11 +63787,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18672827376430781</v>
+        <v>0.17361336873837308</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>8.1399675571680874E-3</v>
+        <v>1.0992532436962243E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -63800,11 +63800,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19845419416709933</v>
+        <v>0.18628669304093479</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1725920402791523E-2</v>
+        <v>1.2673324302561711E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -63813,11 +63813,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.21057166003614999</v>
+        <v>0.19803024034462441</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2117465869050659E-2</v>
+        <v>1.1743547303689622E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
MaJ radio sans ACK (exemple adafruit) et excel calib RTC pcf8523
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/192d16467d0539cb/Documents/5.Bricolage/5.StationMeteo/StationMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="114_{C9647BBB-41EC-4EA6-96B8-FA8F7AF2B1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F895993F-2F06-4894-AB9C-9C9FCA553CEA}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="114_{C9647BBB-41EC-4EA6-96B8-FA8F7AF2B1B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{074831A9-236D-45F4-A08A-081DBF3D58AE}"/>
   <bookViews>
-    <workbookView xWindow="-10152" yWindow="5040" windowWidth="17280" windowHeight="8964" firstSheet="3" activeTab="4" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -1951,6 +1951,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1967,9 +1970,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2246,7 +2246,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-30</c:v>
+                  <c:v>-15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-90</c:v>
@@ -52056,8 +52056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C7B145-5B10-4776-B200-74A4976CCC04}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -52086,7 +52086,7 @@
         <v>336</v>
       </c>
       <c r="L3">
-        <v>-30</v>
+        <v>-15</v>
       </c>
       <c r="M3">
         <v>100</v>
@@ -52134,7 +52134,7 @@
         <v>338</v>
       </c>
       <c r="L6">
-        <v>-30</v>
+        <v>-15</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -52147,7 +52147,7 @@
         <v>339</v>
       </c>
       <c r="L8" s="7">
-        <f>(5/3)*L6+150</f>
+        <f>(4/3)*L6+120</f>
         <v>100</v>
       </c>
     </row>
@@ -57447,13 +57447,13 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="106" t="s">
+      <c r="B3" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C3" s="103" t="s">
+      <c r="C3" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="103" t="s">
+      <c r="D3" s="104" t="s">
         <v>188</v>
       </c>
       <c r="E3" s="72">
@@ -57464,13 +57464,13 @@
       </c>
       <c r="G3" s="72"/>
       <c r="H3" s="72"/>
-      <c r="J3" s="103" t="s">
+      <c r="J3" s="104" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="103" t="s">
+      <c r="K3" s="104" t="s">
         <v>194</v>
       </c>
-      <c r="L3" s="103" t="s">
+      <c r="L3" s="104" t="s">
         <v>195</v>
       </c>
       <c r="M3" s="72">
@@ -57479,9 +57479,9 @@
       <c r="N3" s="72"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="107"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
+      <c r="B4" s="108"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
       <c r="E4" s="67">
         <v>2</v>
       </c>
@@ -57490,18 +57490,18 @@
       </c>
       <c r="G4" s="67"/>
       <c r="H4" s="67"/>
-      <c r="J4" s="104"/>
-      <c r="K4" s="104"/>
-      <c r="L4" s="104"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
       <c r="M4" s="67">
         <v>2</v>
       </c>
       <c r="N4" s="67"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="107"/>
-      <c r="C5" s="104"/>
-      <c r="D5" s="104"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="105"/>
+      <c r="D5" s="105"/>
       <c r="E5" s="67">
         <v>3</v>
       </c>
@@ -57510,18 +57510,18 @@
       </c>
       <c r="G5" s="67"/>
       <c r="H5" s="67"/>
-      <c r="J5" s="104"/>
-      <c r="K5" s="104"/>
-      <c r="L5" s="104"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
       <c r="M5" s="67">
         <v>3</v>
       </c>
       <c r="N5" s="67"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="108"/>
-      <c r="C6" s="105"/>
-      <c r="D6" s="105"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="106"/>
+      <c r="D6" s="106"/>
       <c r="E6" s="73">
         <v>4</v>
       </c>
@@ -57530,22 +57530,22 @@
       </c>
       <c r="G6" s="73"/>
       <c r="H6" s="73"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
+      <c r="J6" s="105"/>
+      <c r="K6" s="105"/>
+      <c r="L6" s="105"/>
       <c r="M6" s="67">
         <v>4</v>
       </c>
       <c r="N6" s="67"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="D7" s="103" t="s">
+      <c r="D7" s="104" t="s">
         <v>171</v>
       </c>
       <c r="E7" s="72">
@@ -57558,18 +57558,18 @@
         <v>275</v>
       </c>
       <c r="H7" s="72"/>
-      <c r="J7" s="105"/>
-      <c r="K7" s="105"/>
-      <c r="L7" s="105"/>
+      <c r="J7" s="106"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
       <c r="M7" s="73">
         <v>5</v>
       </c>
       <c r="N7" s="73"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="107"/>
-      <c r="C8" s="104"/>
-      <c r="D8" s="104"/>
+      <c r="B8" s="108"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
       <c r="E8" s="67">
         <v>2</v>
       </c>
@@ -57580,13 +57580,13 @@
         <v>283</v>
       </c>
       <c r="H8" s="67"/>
-      <c r="J8" s="103" t="s">
+      <c r="J8" s="104" t="s">
         <v>189</v>
       </c>
-      <c r="K8" s="103" t="s">
+      <c r="K8" s="104" t="s">
         <v>194</v>
       </c>
-      <c r="L8" s="103" t="s">
+      <c r="L8" s="104" t="s">
         <v>196</v>
       </c>
       <c r="M8" s="72">
@@ -57597,9 +57597,9 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="108"/>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
+      <c r="B9" s="109"/>
+      <c r="C9" s="106"/>
+      <c r="D9" s="106"/>
       <c r="E9" s="73">
         <v>3</v>
       </c>
@@ -57610,9 +57610,9 @@
         <v>274</v>
       </c>
       <c r="H9" s="73"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
+      <c r="J9" s="105"/>
+      <c r="K9" s="105"/>
+      <c r="L9" s="105"/>
       <c r="M9" s="67">
         <v>2</v>
       </c>
@@ -57621,13 +57621,13 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="106" t="s">
+      <c r="B10" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C10" s="103" t="s">
+      <c r="C10" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="103" t="s">
+      <c r="D10" s="104" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="72">
@@ -57642,9 +57642,9 @@
       <c r="H10" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J10" s="105"/>
-      <c r="K10" s="105"/>
-      <c r="L10" s="105"/>
+      <c r="J10" s="106"/>
+      <c r="K10" s="106"/>
+      <c r="L10" s="106"/>
       <c r="M10" s="73">
         <v>3</v>
       </c>
@@ -57653,9 +57653,9 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="107"/>
-      <c r="C11" s="104"/>
-      <c r="D11" s="104"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="105"/>
+      <c r="D11" s="105"/>
       <c r="E11" s="67">
         <v>2</v>
       </c>
@@ -57668,13 +57668,13 @@
       <c r="H11" s="67" t="s">
         <v>269</v>
       </c>
-      <c r="J11" s="103" t="s">
+      <c r="J11" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="K11" s="103" t="s">
+      <c r="K11" s="104" t="s">
         <v>197</v>
       </c>
-      <c r="L11" s="103" t="s">
+      <c r="L11" s="104" t="s">
         <v>198</v>
       </c>
       <c r="M11">
@@ -57685,9 +57685,9 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="107"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="105"/>
       <c r="E12" s="67">
         <v>3</v>
       </c>
@@ -57700,9 +57700,9 @@
       <c r="H12" s="67" t="s">
         <v>268</v>
       </c>
-      <c r="J12" s="109"/>
-      <c r="K12" s="109"/>
-      <c r="L12" s="109"/>
+      <c r="J12" s="103"/>
+      <c r="K12" s="103"/>
+      <c r="L12" s="103"/>
       <c r="M12">
         <v>2</v>
       </c>
@@ -57711,9 +57711,9 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="108"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="106"/>
       <c r="E13" s="73">
         <v>4</v>
       </c>
@@ -57726,13 +57726,13 @@
       <c r="H13" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="J13" s="103" t="s">
+      <c r="J13" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="K13" s="103" t="s">
+      <c r="K13" s="104" t="s">
         <v>197</v>
       </c>
-      <c r="L13" s="103" t="s">
+      <c r="L13" s="104" t="s">
         <v>199</v>
       </c>
       <c r="M13" s="72">
@@ -57743,13 +57743,13 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="103" t="s">
+      <c r="D14" s="104" t="s">
         <v>172</v>
       </c>
       <c r="E14" s="72">
@@ -57764,16 +57764,16 @@
       <c r="H14" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J14" s="104"/>
-      <c r="K14" s="104"/>
-      <c r="L14" s="104"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
+      <c r="L14" s="105"/>
       <c r="M14" s="67"/>
       <c r="N14" s="67"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="107"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="104"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="105"/>
+      <c r="D15" s="105"/>
       <c r="E15" s="67">
         <v>2</v>
       </c>
@@ -57786,16 +57786,16 @@
       <c r="H15" s="67" t="s">
         <v>269</v>
       </c>
-      <c r="J15" s="104"/>
-      <c r="K15" s="104"/>
-      <c r="L15" s="104"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
+      <c r="L15" s="105"/>
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="107"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
+      <c r="B16" s="108"/>
+      <c r="C16" s="105"/>
+      <c r="D16" s="105"/>
       <c r="E16" s="67">
         <v>3</v>
       </c>
@@ -57808,16 +57808,16 @@
       <c r="H16" s="67" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="104"/>
-      <c r="K16" s="104"/>
-      <c r="L16" s="104"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
+      <c r="L16" s="105"/>
       <c r="M16" s="67"/>
       <c r="N16" s="67"/>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="108"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="105"/>
+      <c r="B17" s="109"/>
+      <c r="C17" s="106"/>
+      <c r="D17" s="106"/>
       <c r="E17" s="73">
         <v>4</v>
       </c>
@@ -57830,20 +57830,20 @@
       <c r="H17" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="J17" s="104"/>
-      <c r="K17" s="104"/>
-      <c r="L17" s="104"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
+      <c r="L17" s="105"/>
       <c r="M17" s="67"/>
       <c r="N17" s="67"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C18" s="103" t="s">
+      <c r="C18" s="104" t="s">
         <v>192</v>
       </c>
-      <c r="D18" s="103" t="s">
+      <c r="D18" s="104" t="s">
         <v>179</v>
       </c>
       <c r="E18" s="72">
@@ -57858,9 +57858,9 @@
       <c r="H18" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J18" s="104"/>
-      <c r="K18" s="104"/>
-      <c r="L18" s="104"/>
+      <c r="J18" s="105"/>
+      <c r="K18" s="105"/>
+      <c r="L18" s="105"/>
       <c r="M18" s="67">
         <v>2</v>
       </c>
@@ -57869,9 +57869,9 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="107"/>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
       <c r="E19" s="67">
         <v>2</v>
       </c>
@@ -57886,9 +57886,9 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="107"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="104"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="105"/>
+      <c r="D20" s="105"/>
       <c r="E20" s="67">
         <v>3</v>
       </c>
@@ -57903,9 +57903,9 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="108"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="106"/>
+      <c r="D21" s="106"/>
       <c r="E21" s="73">
         <v>4</v>
       </c>
@@ -57920,13 +57920,13 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="106" t="s">
+      <c r="B22" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="103" t="s">
+      <c r="C22" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="103" t="s">
+      <c r="D22" s="104" t="s">
         <v>261</v>
       </c>
       <c r="E22" s="72">
@@ -57941,9 +57941,9 @@
       <c r="H22" s="72"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="107"/>
-      <c r="C23" s="104"/>
-      <c r="D23" s="104"/>
+      <c r="B23" s="108"/>
+      <c r="C23" s="105"/>
+      <c r="D23" s="105"/>
       <c r="E23" s="67">
         <v>2</v>
       </c>
@@ -57956,9 +57956,9 @@
       <c r="H23" s="67"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="107"/>
-      <c r="C24" s="104"/>
-      <c r="D24" s="104"/>
+      <c r="B24" s="108"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
       <c r="E24" s="67">
         <v>3</v>
       </c>
@@ -57971,9 +57971,9 @@
       <c r="H24" s="67"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="107"/>
-      <c r="C25" s="104"/>
-      <c r="D25" s="104"/>
+      <c r="B25" s="108"/>
+      <c r="C25" s="105"/>
+      <c r="D25" s="105"/>
       <c r="E25" s="67">
         <v>4</v>
       </c>
@@ -57986,9 +57986,9 @@
       <c r="H25" s="67"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="107"/>
-      <c r="C26" s="104"/>
-      <c r="D26" s="104"/>
+      <c r="B26" s="108"/>
+      <c r="C26" s="105"/>
+      <c r="D26" s="105"/>
       <c r="E26" s="67">
         <v>5</v>
       </c>
@@ -58001,9 +58001,9 @@
       <c r="H26" s="67"/>
     </row>
     <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="108"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="105"/>
+      <c r="B27" s="109"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="106"/>
       <c r="E27" s="73">
         <v>6</v>
       </c>
@@ -58016,13 +58016,13 @@
       <c r="H27" s="73"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="103" t="s">
+      <c r="C28" s="104" t="s">
         <v>193</v>
       </c>
-      <c r="D28" s="103" t="s">
+      <c r="D28" s="104" t="s">
         <v>174</v>
       </c>
       <c r="E28" s="72">
@@ -58037,9 +58037,9 @@
       <c r="H28" s="72"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="107"/>
-      <c r="C29" s="104"/>
-      <c r="D29" s="104"/>
+      <c r="B29" s="108"/>
+      <c r="C29" s="105"/>
+      <c r="D29" s="105"/>
       <c r="E29" s="67">
         <v>2</v>
       </c>
@@ -58052,9 +58052,9 @@
       <c r="H29" s="67"/>
     </row>
     <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="108"/>
-      <c r="C30" s="105"/>
-      <c r="D30" s="105"/>
+      <c r="B30" s="109"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
       <c r="E30" s="73">
         <v>3</v>
       </c>
@@ -58078,7 +58078,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="109" t="s">
+      <c r="A35" s="103" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="78" t="s">
@@ -58092,7 +58092,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="109"/>
+      <c r="A36" s="103"/>
       <c r="B36" s="79" t="s">
         <v>150</v>
       </c>
@@ -58104,7 +58104,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="109"/>
+      <c r="A37" s="103"/>
       <c r="B37" s="76" t="s">
         <v>187</v>
       </c>
@@ -58116,7 +58116,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="109"/>
+      <c r="A38" s="103"/>
       <c r="B38" s="82" t="s">
         <v>173</v>
       </c>
@@ -58128,7 +58128,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="109" t="s">
+      <c r="A39" s="103" t="s">
         <v>179</v>
       </c>
       <c r="B39" s="78" t="s">
@@ -58142,7 +58142,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="109"/>
+      <c r="A40" s="103"/>
       <c r="B40" s="79" t="s">
         <v>150</v>
       </c>
@@ -58154,7 +58154,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="109"/>
+      <c r="A41" s="103"/>
       <c r="B41" s="76" t="s">
         <v>187</v>
       </c>
@@ -58166,7 +58166,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="109"/>
+      <c r="A42" s="103"/>
       <c r="B42" s="77" t="s">
         <v>262</v>
       </c>
@@ -58179,6 +58179,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D14:D17"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="L13:L18"/>
@@ -58195,25 +58214,6 @@
     <mergeCell ref="L8:L10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="J8:J10"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="D22:D27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G3:H13 G18:H30">
@@ -58260,7 +58260,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="A2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -58308,7 +58308,7 @@
       <c r="G3" s="27"/>
       <c r="H3" s="28"/>
       <c r="I3" s="29"/>
-      <c r="L3" s="109" t="s">
+      <c r="L3" s="103" t="s">
         <v>151</v>
       </c>
       <c r="M3" t="s">
@@ -58332,7 +58332,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="16"/>
       <c r="I4" s="17"/>
-      <c r="L4" s="109"/>
+      <c r="L4" s="103"/>
       <c r="M4" t="s">
         <v>179</v>
       </c>
@@ -58360,7 +58360,7 @@
       <c r="I5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="L5" s="109"/>
+      <c r="L5" s="103"/>
       <c r="M5" t="s">
         <v>70</v>
       </c>
@@ -58384,7 +58384,7 @@
       <c r="I6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="L6" s="109"/>
+      <c r="L6" s="103"/>
       <c r="M6" t="s">
         <v>172</v>
       </c>
@@ -58737,7 +58737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C64E373-7692-4CBF-88B4-6ED8CB4BCA4C}">
   <dimension ref="A1:S245"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -63655,7 +63655,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.6363465064491071E-3</v>
+        <v>1.0637577333653087E-2</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -63670,7 +63670,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>103.77376937729998</v>
+        <v>94.006367111089816</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -63682,18 +63682,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>7.615277065266845E-3</v>
+        <v>1.0448140743311489E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>7.615277065266845E-3</v>
+        <v>1.0448140743311489E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>3.7737693772999847E-2</v>
+        <v>-5.9936328889101845E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -63702,11 +63702,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0556341416257878E-2</v>
+        <v>2.0248353299682987E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.2941064350991033E-2</v>
+        <v>9.8002125563714983E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -63715,11 +63715,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.0456454445961859E-2</v>
+        <v>3.0384248931914666E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>9.9001130297039809E-3</v>
+        <v>1.0135895632231679E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -63728,11 +63728,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>4.2217443604239832E-2</v>
+        <v>4.3093932944054079E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1760989158277974E-2</v>
+        <v>1.2709684012139413E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -63741,11 +63741,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>5.3454988802460773E-2</v>
+        <v>5.211764129694977E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1237545198220941E-2</v>
+        <v>9.0237083528956902E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -63754,11 +63754,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>6.1066728495171307E-2</v>
+        <v>6.0627182154882032E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6117396927105341E-3</v>
+        <v>8.5095408579322629E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -63767,11 +63767,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3080795892930123E-2</v>
+        <v>7.2310966441153077E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2014067397758815E-2</v>
+        <v>1.1683784286271044E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -63780,11 +63780,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>8.3889859115354237E-2</v>
+        <v>8.3059845034726659E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0809063222424115E-2</v>
+        <v>1.0748878593573583E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -63793,11 +63793,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>9.1162698299237468E-2</v>
+        <v>9.5839486698069631E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2728391838832313E-3</v>
+        <v>1.2779641663342972E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -63806,11 +63806,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10030710243236833</v>
+        <v>0.10726147909930868</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1444041331308623E-3</v>
+        <v>1.1421992401239048E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -63819,11 +63819,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10736027503596025</v>
+        <v>0.11512872507179769</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0531726035919229E-3</v>
+        <v>7.8672459724890148E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -63832,11 +63832,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11437175635621827</v>
+        <v>0.12245389477126274</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.0114813202580145E-3</v>
+        <v>7.3251696994650478E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -63845,11 +63845,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12266224581931189</v>
+        <v>0.13412248353667916</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2904894630936171E-3</v>
+        <v>1.1668588765416418E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -63858,11 +63858,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13548368345587913</v>
+        <v>0.144449404952356</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2821437636567248E-2</v>
+        <v>1.0326921415676843E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -63871,11 +63871,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14612249984829051</v>
+        <v>0.15675217101045244</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0638816392411377E-2</v>
+        <v>1.2302766058096437E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -63884,11 +63884,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15412478011016065</v>
+        <v>0.1692366174887974</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0022802618701372E-3</v>
+        <v>1.2484446478344957E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -63897,11 +63897,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16459527234416424</v>
+        <v>0.18047905904114422</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0470492234003592E-2</v>
+        <v>1.1242441552346827E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -63910,11 +63910,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17487149432963386</v>
+        <v>0.1900852068567162</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0276221985469625E-2</v>
+        <v>9.6061478155719804E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -63923,11 +63923,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18309058362253303</v>
+        <v>0.20211396933940864</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>8.2190892928991621E-3</v>
+        <v>1.202876248269244E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test sleep reconnect + correction numerotation des pin DHT et windDir
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/192d16467d0539cb/Documents/5.Bricolage/5.StationMeteo/StationMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6697A7-D972-4BCC-82E3-A4495661F06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CD6697A7-D972-4BCC-82E3-A4495661F06C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{24DF6705-1DE3-4101-819F-B3D62AA811AB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
@@ -2132,6 +2132,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2148,9 +2151,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -32278,7 +32278,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>1.0045257372787122E-2</v>
+        <v>1.0286160452821803E-2</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -32293,7 +32293,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>99.54946527393389</v>
+        <v>97.21800516203983</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -32305,18 +32305,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>8.0569557899721079E-3</v>
+        <v>1.1662036407941634E-2</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>8.0569557899721079E-3</v>
+        <v>1.1662036407941634E-2</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>-4.5053472606610967E-3</v>
+        <v>-2.7819948379601698E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -32325,11 +32325,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.0492896296728277E-2</v>
+        <v>2.3236855554728968E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.243594050675617E-2</v>
+        <v>1.1574819146787334E-2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -32338,11 +32338,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>2.9278235221830283E-2</v>
+        <v>3.1703691291407439E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>8.7853389251020056E-3</v>
+        <v>8.4668357366784706E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -32351,11 +32351,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.7997010487068897E-2</v>
+        <v>3.8889575819330918E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7187752652386138E-3</v>
+        <v>7.1858845279234793E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -32364,11 +32364,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.9442095054663078E-2</v>
+        <v>5.0847723311248406E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1445084567594181E-2</v>
+        <v>1.1958147491917488E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -32377,11 +32377,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.6723881785815264E-2</v>
+        <v>5.9496185840499656E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2817867311521858E-3</v>
+        <v>8.6484625292512496E-3</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -32390,11 +32390,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.7402930749807577E-2</v>
+        <v>6.8724038417192282E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0679048963992313E-2</v>
+        <v>9.2278525766926259E-3</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -32403,11 +32403,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.6755770772829829E-2</v>
+        <v>8.1083791925512419E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>9.3528400230222519E-3</v>
+        <v>1.2359753508320137E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -32416,11 +32416,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.4334480952172164E-2</v>
+        <v>9.3307129894114868E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>7.578710179342335E-3</v>
+        <v>1.2223337968602449E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -32429,11 +32429,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5049324291741066E-2</v>
+        <v>0.10525645418045065</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0714843339568902E-2</v>
+        <v>1.1949324286335786E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -32442,11 +32442,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1077439539230353</v>
+        <v>0.11681964594515577</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2694629631294238E-2</v>
+        <v>1.1563191764705119E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -32455,11 +32455,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11896777710051748</v>
+        <v>0.12394087200540968</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>1.1223823177482176E-2</v>
+        <v>7.1212260602539074E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -32468,11 +32468,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12739258949113394</v>
+        <v>0.13190243593994164</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>8.4248123906164596E-3</v>
+        <v>7.9615639345319567E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -32481,11 +32481,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13726350066544654</v>
+        <v>0.14405640096240047</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>9.8709111743126021E-3</v>
+        <v>1.2153965022458829E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -32494,11 +32494,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14508902164453236</v>
+        <v>0.15428679304554296</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8255209790858149E-3</v>
+        <v>1.0230392083142498E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -32507,11 +32507,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15424837081569739</v>
+        <v>0.16720737055955501</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>9.1593491711650377E-3</v>
+        <v>1.2920577514012044E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -32520,11 +32520,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16515649821480077</v>
+        <v>0.17705596510636373</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0908127399103379E-2</v>
+        <v>9.8485945468087255E-3</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -32533,11 +32533,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17804854674794976</v>
+        <v>0.18480451513038595</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2892048533148986E-2</v>
+        <v>7.7485500240222216E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -32546,11 +32546,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19085989008295534</v>
+        <v>0.19543704860361427</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2811343335005582E-2</v>
+        <v>1.0632533473228317E-2</v>
       </c>
     </row>
   </sheetData>
@@ -58234,13 +58234,13 @@
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="115" t="s">
         <v>188</v>
       </c>
       <c r="E3" s="72">
@@ -58251,13 +58251,13 @@
       </c>
       <c r="G3" s="72"/>
       <c r="H3" s="72"/>
-      <c r="J3" s="114" t="s">
+      <c r="J3" s="115" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="114" t="s">
+      <c r="K3" s="115" t="s">
         <v>194</v>
       </c>
-      <c r="L3" s="114" t="s">
+      <c r="L3" s="115" t="s">
         <v>195</v>
       </c>
       <c r="M3" s="72">
@@ -58266,9 +58266,9 @@
       <c r="N3" s="72"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B4" s="118"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
+      <c r="B4" s="119"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
       <c r="E4" s="67">
         <v>2</v>
       </c>
@@ -58277,18 +58277,18 @@
       </c>
       <c r="G4" s="67"/>
       <c r="H4" s="67"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
       <c r="M4" s="67">
         <v>2</v>
       </c>
       <c r="N4" s="67"/>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B5" s="118"/>
-      <c r="C5" s="115"/>
-      <c r="D5" s="115"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
       <c r="E5" s="67">
         <v>3</v>
       </c>
@@ -58297,18 +58297,18 @@
       </c>
       <c r="G5" s="67"/>
       <c r="H5" s="67"/>
-      <c r="J5" s="115"/>
-      <c r="K5" s="115"/>
-      <c r="L5" s="115"/>
+      <c r="J5" s="116"/>
+      <c r="K5" s="116"/>
+      <c r="L5" s="116"/>
       <c r="M5" s="67">
         <v>3</v>
       </c>
       <c r="N5" s="67"/>
     </row>
     <row r="6" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="119"/>
-      <c r="C6" s="116"/>
-      <c r="D6" s="116"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
       <c r="E6" s="73">
         <v>4</v>
       </c>
@@ -58317,22 +58317,22 @@
       </c>
       <c r="G6" s="73"/>
       <c r="H6" s="73"/>
-      <c r="J6" s="115"/>
-      <c r="K6" s="115"/>
-      <c r="L6" s="115"/>
+      <c r="J6" s="116"/>
+      <c r="K6" s="116"/>
+      <c r="L6" s="116"/>
       <c r="M6" s="67">
         <v>4</v>
       </c>
       <c r="N6" s="67"/>
     </row>
     <row r="7" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C7" s="114" t="s">
+      <c r="C7" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="D7" s="114" t="s">
+      <c r="D7" s="115" t="s">
         <v>171</v>
       </c>
       <c r="E7" s="72">
@@ -58345,18 +58345,18 @@
         <v>275</v>
       </c>
       <c r="H7" s="72"/>
-      <c r="J7" s="116"/>
-      <c r="K7" s="116"/>
-      <c r="L7" s="116"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
       <c r="M7" s="73">
         <v>5</v>
       </c>
       <c r="N7" s="73"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="118"/>
-      <c r="C8" s="115"/>
-      <c r="D8" s="115"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
       <c r="E8" s="67">
         <v>2</v>
       </c>
@@ -58367,13 +58367,13 @@
         <v>283</v>
       </c>
       <c r="H8" s="67"/>
-      <c r="J8" s="114" t="s">
+      <c r="J8" s="115" t="s">
         <v>189</v>
       </c>
-      <c r="K8" s="114" t="s">
+      <c r="K8" s="115" t="s">
         <v>194</v>
       </c>
-      <c r="L8" s="114" t="s">
+      <c r="L8" s="115" t="s">
         <v>196</v>
       </c>
       <c r="M8" s="72">
@@ -58384,9 +58384,9 @@
       </c>
     </row>
     <row r="9" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="119"/>
-      <c r="C9" s="116"/>
-      <c r="D9" s="116"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="117"/>
+      <c r="D9" s="117"/>
       <c r="E9" s="73">
         <v>3</v>
       </c>
@@ -58397,9 +58397,9 @@
         <v>274</v>
       </c>
       <c r="H9" s="73"/>
-      <c r="J9" s="115"/>
-      <c r="K9" s="115"/>
-      <c r="L9" s="115"/>
+      <c r="J9" s="116"/>
+      <c r="K9" s="116"/>
+      <c r="L9" s="116"/>
       <c r="M9" s="67">
         <v>2</v>
       </c>
@@ -58408,13 +58408,13 @@
       </c>
     </row>
     <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="117" t="s">
+      <c r="B10" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C10" s="114" t="s">
+      <c r="C10" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="D10" s="114" t="s">
+      <c r="D10" s="115" t="s">
         <v>70</v>
       </c>
       <c r="E10" s="72">
@@ -58429,9 +58429,9 @@
       <c r="H10" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J10" s="116"/>
-      <c r="K10" s="116"/>
-      <c r="L10" s="116"/>
+      <c r="J10" s="117"/>
+      <c r="K10" s="117"/>
+      <c r="L10" s="117"/>
       <c r="M10" s="73">
         <v>3</v>
       </c>
@@ -58440,9 +58440,9 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B11" s="118"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="115"/>
+      <c r="B11" s="119"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
       <c r="E11" s="67">
         <v>2</v>
       </c>
@@ -58455,13 +58455,13 @@
       <c r="H11" s="67" t="s">
         <v>269</v>
       </c>
-      <c r="J11" s="114" t="s">
+      <c r="J11" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="K11" s="114" t="s">
+      <c r="K11" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="L11" s="114" t="s">
+      <c r="L11" s="115" t="s">
         <v>198</v>
       </c>
       <c r="M11">
@@ -58472,9 +58472,9 @@
       </c>
     </row>
     <row r="12" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="118"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
       <c r="E12" s="67">
         <v>3</v>
       </c>
@@ -58487,9 +58487,9 @@
       <c r="H12" s="67" t="s">
         <v>268</v>
       </c>
-      <c r="J12" s="120"/>
-      <c r="K12" s="120"/>
-      <c r="L12" s="120"/>
+      <c r="J12" s="114"/>
+      <c r="K12" s="114"/>
+      <c r="L12" s="114"/>
       <c r="M12">
         <v>2</v>
       </c>
@@ -58498,9 +58498,9 @@
       </c>
     </row>
     <row r="13" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="119"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
+      <c r="B13" s="120"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
       <c r="E13" s="73">
         <v>4</v>
       </c>
@@ -58513,13 +58513,13 @@
       <c r="H13" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="J13" s="114" t="s">
+      <c r="J13" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="K13" s="114" t="s">
+      <c r="K13" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="L13" s="114" t="s">
+      <c r="L13" s="115" t="s">
         <v>199</v>
       </c>
       <c r="M13" s="72">
@@ -58530,13 +58530,13 @@
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="117" t="s">
+      <c r="B14" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="114" t="s">
+      <c r="C14" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="D14" s="114" t="s">
+      <c r="D14" s="115" t="s">
         <v>172</v>
       </c>
       <c r="E14" s="72">
@@ -58551,16 +58551,16 @@
       <c r="H14" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J14" s="115"/>
-      <c r="K14" s="115"/>
-      <c r="L14" s="115"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="116"/>
       <c r="M14" s="67"/>
       <c r="N14" s="67"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B15" s="118"/>
-      <c r="C15" s="115"/>
-      <c r="D15" s="115"/>
+      <c r="B15" s="119"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
       <c r="E15" s="67">
         <v>2</v>
       </c>
@@ -58573,16 +58573,16 @@
       <c r="H15" s="67" t="s">
         <v>269</v>
       </c>
-      <c r="J15" s="115"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
+      <c r="J15" s="116"/>
+      <c r="K15" s="116"/>
+      <c r="L15" s="116"/>
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B16" s="118"/>
-      <c r="C16" s="115"/>
-      <c r="D16" s="115"/>
+      <c r="B16" s="119"/>
+      <c r="C16" s="116"/>
+      <c r="D16" s="116"/>
       <c r="E16" s="67">
         <v>3</v>
       </c>
@@ -58595,16 +58595,16 @@
       <c r="H16" s="67" t="s">
         <v>268</v>
       </c>
-      <c r="J16" s="115"/>
-      <c r="K16" s="115"/>
-      <c r="L16" s="115"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
+      <c r="L16" s="116"/>
       <c r="M16" s="67"/>
       <c r="N16" s="67"/>
     </row>
     <row r="17" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="119"/>
-      <c r="C17" s="116"/>
-      <c r="D17" s="116"/>
+      <c r="B17" s="120"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
       <c r="E17" s="73">
         <v>4</v>
       </c>
@@ -58617,20 +58617,20 @@
       <c r="H17" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="J17" s="115"/>
-      <c r="K17" s="115"/>
-      <c r="L17" s="115"/>
+      <c r="J17" s="116"/>
+      <c r="K17" s="116"/>
+      <c r="L17" s="116"/>
       <c r="M17" s="67"/>
       <c r="N17" s="67"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B18" s="117" t="s">
+      <c r="B18" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C18" s="114" t="s">
+      <c r="C18" s="115" t="s">
         <v>192</v>
       </c>
-      <c r="D18" s="114" t="s">
+      <c r="D18" s="115" t="s">
         <v>179</v>
       </c>
       <c r="E18" s="72">
@@ -58645,9 +58645,9 @@
       <c r="H18" s="72" t="s">
         <v>278</v>
       </c>
-      <c r="J18" s="115"/>
-      <c r="K18" s="115"/>
-      <c r="L18" s="115"/>
+      <c r="J18" s="116"/>
+      <c r="K18" s="116"/>
+      <c r="L18" s="116"/>
       <c r="M18" s="67">
         <v>2</v>
       </c>
@@ -58656,9 +58656,9 @@
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B19" s="118"/>
-      <c r="C19" s="115"/>
-      <c r="D19" s="115"/>
+      <c r="B19" s="119"/>
+      <c r="C19" s="116"/>
+      <c r="D19" s="116"/>
       <c r="E19" s="67">
         <v>2</v>
       </c>
@@ -58673,9 +58673,9 @@
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="118"/>
-      <c r="C20" s="115"/>
-      <c r="D20" s="115"/>
+      <c r="B20" s="119"/>
+      <c r="C20" s="116"/>
+      <c r="D20" s="116"/>
       <c r="E20" s="67">
         <v>3</v>
       </c>
@@ -58690,9 +58690,9 @@
       </c>
     </row>
     <row r="21" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="119"/>
-      <c r="C21" s="116"/>
-      <c r="D21" s="116"/>
+      <c r="B21" s="120"/>
+      <c r="C21" s="117"/>
+      <c r="D21" s="117"/>
       <c r="E21" s="73">
         <v>4</v>
       </c>
@@ -58707,13 +58707,13 @@
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="117" t="s">
+      <c r="B22" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C22" s="114" t="s">
+      <c r="C22" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="D22" s="114" t="s">
+      <c r="D22" s="115" t="s">
         <v>261</v>
       </c>
       <c r="E22" s="72">
@@ -58728,9 +58728,9 @@
       <c r="H22" s="72"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="118"/>
-      <c r="C23" s="115"/>
-      <c r="D23" s="115"/>
+      <c r="B23" s="119"/>
+      <c r="C23" s="116"/>
+      <c r="D23" s="116"/>
       <c r="E23" s="67">
         <v>2</v>
       </c>
@@ -58743,9 +58743,9 @@
       <c r="H23" s="67"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="118"/>
-      <c r="C24" s="115"/>
-      <c r="D24" s="115"/>
+      <c r="B24" s="119"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
       <c r="E24" s="67">
         <v>3</v>
       </c>
@@ -58758,9 +58758,9 @@
       <c r="H24" s="67"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="118"/>
-      <c r="C25" s="115"/>
-      <c r="D25" s="115"/>
+      <c r="B25" s="119"/>
+      <c r="C25" s="116"/>
+      <c r="D25" s="116"/>
       <c r="E25" s="67">
         <v>4</v>
       </c>
@@ -58773,9 +58773,9 @@
       <c r="H25" s="67"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="118"/>
-      <c r="C26" s="115"/>
-      <c r="D26" s="115"/>
+      <c r="B26" s="119"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="116"/>
       <c r="E26" s="67">
         <v>5</v>
       </c>
@@ -58788,9 +58788,9 @@
       <c r="H26" s="67"/>
     </row>
     <row r="27" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="119"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="116"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
       <c r="E27" s="73">
         <v>6</v>
       </c>
@@ -58803,13 +58803,13 @@
       <c r="H27" s="73"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="117" t="s">
+      <c r="B28" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="C28" s="114" t="s">
+      <c r="C28" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="D28" s="114" t="s">
+      <c r="D28" s="115" t="s">
         <v>174</v>
       </c>
       <c r="E28" s="72">
@@ -58824,9 +58824,9 @@
       <c r="H28" s="72"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="118"/>
-      <c r="C29" s="115"/>
-      <c r="D29" s="115"/>
+      <c r="B29" s="119"/>
+      <c r="C29" s="116"/>
+      <c r="D29" s="116"/>
       <c r="E29" s="67">
         <v>2</v>
       </c>
@@ -58839,9 +58839,9 @@
       <c r="H29" s="67"/>
     </row>
     <row r="30" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="119"/>
-      <c r="C30" s="116"/>
-      <c r="D30" s="116"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
       <c r="E30" s="73">
         <v>3</v>
       </c>
@@ -58865,7 +58865,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="120" t="s">
+      <c r="A35" s="114" t="s">
         <v>70</v>
       </c>
       <c r="B35" s="78" t="s">
@@ -58879,7 +58879,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="120"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="79" t="s">
         <v>150</v>
       </c>
@@ -58891,7 +58891,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="120"/>
+      <c r="A37" s="114"/>
       <c r="B37" s="76" t="s">
         <v>187</v>
       </c>
@@ -58903,7 +58903,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="120"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="82" t="s">
         <v>173</v>
       </c>
@@ -58915,7 +58915,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="120" t="s">
+      <c r="A39" s="114" t="s">
         <v>179</v>
       </c>
       <c r="B39" s="78" t="s">
@@ -58929,7 +58929,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="120"/>
+      <c r="A40" s="114"/>
       <c r="B40" s="79" t="s">
         <v>150</v>
       </c>
@@ -58941,7 +58941,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="120"/>
+      <c r="A41" s="114"/>
       <c r="B41" s="76" t="s">
         <v>187</v>
       </c>
@@ -58953,7 +58953,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="120"/>
+      <c r="A42" s="114"/>
       <c r="B42" s="77" t="s">
         <v>262</v>
       </c>
@@ -58966,6 +58966,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="D18:D21"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="C22:C27"/>
+    <mergeCell ref="B22:B27"/>
+    <mergeCell ref="D22:D27"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="L3:L7"/>
+    <mergeCell ref="K3:K7"/>
+    <mergeCell ref="J3:J7"/>
+    <mergeCell ref="D3:D6"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="D14:D17"/>
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="L13:L18"/>
@@ -58982,25 +59001,6 @@
     <mergeCell ref="L8:L10"/>
     <mergeCell ref="K8:K10"/>
     <mergeCell ref="J8:J10"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="L3:L7"/>
-    <mergeCell ref="K3:K7"/>
-    <mergeCell ref="J3:J7"/>
-    <mergeCell ref="D3:D6"/>
-    <mergeCell ref="C3:C6"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="D14:D17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="C22:C27"/>
-    <mergeCell ref="B22:B27"/>
-    <mergeCell ref="D22:D27"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G3:H13 G18:H30">
@@ -59047,8 +59047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
   <dimension ref="B2:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -59101,7 +59101,7 @@
       <c r="J3" s="27"/>
       <c r="K3" s="28"/>
       <c r="L3" s="29"/>
-      <c r="O3" s="120" t="s">
+      <c r="O3" s="114" t="s">
         <v>151</v>
       </c>
       <c r="P3" t="s">
@@ -59131,7 +59131,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="16"/>
       <c r="L4" s="17"/>
-      <c r="O4" s="120"/>
+      <c r="O4" s="114"/>
       <c r="P4" t="s">
         <v>179</v>
       </c>
@@ -59165,7 +59165,7 @@
       <c r="L5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O5" s="120"/>
+      <c r="O5" s="114"/>
       <c r="P5" t="s">
         <v>70</v>
       </c>
@@ -59195,7 +59195,7 @@
       <c r="L6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="120"/>
+      <c r="O6" s="114"/>
       <c r="P6" t="s">
         <v>172</v>
       </c>
@@ -59446,9 +59446,6 @@
       <c r="B19" s="100" t="s">
         <v>357</v>
       </c>
-      <c r="C19" s="100" t="s">
-        <v>362</v>
-      </c>
       <c r="D19" s="100"/>
       <c r="I19" s="24" t="s">
         <v>5</v>
@@ -59495,7 +59492,9 @@
       <c r="B22" s="100" t="s">
         <v>360</v>
       </c>
-      <c r="C22" s="100"/>
+      <c r="C22" s="100" t="s">
+        <v>362</v>
+      </c>
       <c r="D22" s="100"/>
       <c r="I22" s="24" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
correction angle adafruit IO
</commit_message>
<xml_diff>
--- a/SuiviProjet.xlsx
+++ b/SuiviProjet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/192d16467d0539cb/Documents/5.Bricolage/5.StationMeteo/StationMeteo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="114_{1340477D-1E51-4084-91B9-DFF34E9BEA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3A8CE77A-CB81-46F3-BA66-899740396A2B}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="114_{1340477D-1E51-4084-91B9-DFF34E9BEA3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{57F4E5C7-CE2E-42DD-88BC-1CA614A764DD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
+    <workbookView xWindow="11520" yWindow="540" windowWidth="11316" windowHeight="8184" firstSheet="5" activeTab="10" xr2:uid="{700A1A7B-3F76-47D1-986E-B358D29F4025}"/>
   </bookViews>
   <sheets>
     <sheet name="Achat" sheetId="11" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="413">
   <si>
     <t>Produit</t>
   </si>
@@ -1295,9 +1295,6 @@
     <t>D0</t>
   </si>
   <si>
-    <t>Wake up</t>
-  </si>
-  <si>
     <t>I²C SCL</t>
   </si>
   <si>
@@ -1314,6 +1311,18 @@
   </si>
   <si>
     <t>Ready transfert</t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>Wake up (on RST)</t>
+  </si>
+  <si>
+    <t>mesure :</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -1494,13 +1503,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1518,6 +1520,14 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2106,28 +2116,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2156,7 +2166,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
@@ -32281,7 +32291,7 @@
       </c>
       <c r="F6">
         <f ca="1">AVERAGE(C8:C26)</f>
-        <v>9.6860012005028778E-3</v>
+        <v>9.2246226740240415E-3</v>
       </c>
       <c r="G6" t="s">
         <v>31</v>
@@ -32296,7 +32306,7 @@
       </c>
       <c r="F7">
         <f ca="1">1/F6</f>
-        <v>103.24177948151421</v>
+        <v>108.40551807240173</v>
       </c>
       <c r="G7" t="s">
         <v>29</v>
@@ -32308,18 +32318,18 @@
       </c>
       <c r="B8">
         <f t="shared" ref="B8:B26" ca="1" si="0">B7+B$3+(RAND()*2-1)*B$3*B$4</f>
-        <v>1.1097321003934683E-2</v>
+        <v>7.9891741999420732E-3</v>
       </c>
       <c r="C8">
         <f ca="1">B8-B7</f>
-        <v>1.1097321003934683E-2</v>
+        <v>7.9891741999420732E-3</v>
       </c>
       <c r="E8" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6">
         <f ca="1">(F7-B2)/B2</f>
-        <v>3.2417794815142148E-2</v>
+        <v>8.4055180724017339E-2</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -32328,11 +32338,11 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.1431292346972244E-2</v>
+        <v>1.5391916492330973E-2</v>
       </c>
       <c r="C9">
         <f ca="1">B9-B8</f>
-        <v>1.0333971343037561E-2</v>
+        <v>7.4027422923888999E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -32341,11 +32351,11 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1503022722577656E-2</v>
+        <v>2.4121427867210658E-2</v>
       </c>
       <c r="C10">
         <f t="shared" ref="C10:C26" ca="1" si="1">B10-B9</f>
-        <v>1.0071730375605412E-2</v>
+        <v>8.7295113748796851E-3</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -32354,11 +32364,11 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>3.867836138775696E-2</v>
+        <v>3.2382193267706243E-2</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1753386651793039E-3</v>
+        <v>8.2607654004955844E-3</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -32367,11 +32377,11 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>4.7607582467864167E-2</v>
+        <v>4.0237674625782024E-2</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9292210801072067E-3</v>
+        <v>7.8554813580757818E-3</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -32380,11 +32390,11 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>5.7088767792706413E-2</v>
+        <v>5.2483987223428417E-2</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>9.4811853248422465E-3</v>
+        <v>1.2246312597646393E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -32393,11 +32403,11 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>6.9090636839560696E-2</v>
+        <v>6.2940440653459204E-2</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2001869046854283E-2</v>
+        <v>1.0456453430030786E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -32406,11 +32416,11 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>7.7952219760664271E-2</v>
+        <v>7.0571927645758772E-2</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>8.8615829211035752E-3</v>
+        <v>7.6314869922995687E-3</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -32419,11 +32429,11 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>8.8083384937158074E-2</v>
+        <v>7.7896558423985199E-2</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0131165176493803E-2</v>
+        <v>7.3246307782264264E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -32432,11 +32442,11 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.6152224469678457E-2</v>
+        <v>8.6599384485343933E-2</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>8.0688395325203832E-3</v>
+        <v>8.7028260613587344E-3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -32445,11 +32455,11 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10488533286847726</v>
+        <v>9.4915838855129234E-2</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7331083987988029E-3</v>
+        <v>8.3164543697853005E-3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -32458,11 +32468,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11204436297472695</v>
+        <v>0.10339283440266003</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1590301062496864E-3</v>
+        <v>8.4769955475307995E-3</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -32471,11 +32481,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.12160268119198536</v>
+        <v>0.11156306136242883</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>9.5583182172584158E-3</v>
+        <v>8.1702269597687949E-3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -32484,11 +32494,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.13361628888299928</v>
+        <v>0.12038086002756172</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2013607691013922E-2</v>
+        <v>8.8177986651328949E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -32497,11 +32507,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.14124212465426988</v>
+        <v>0.1330942239065763</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>7.6258357712706004E-3</v>
+        <v>1.2713363879014575E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -32510,11 +32520,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.15382432896050927</v>
+        <v>0.14485855217174182</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2582204306239381E-2</v>
+        <v>1.1764328265165519E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -32523,11 +32533,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16616976363016936</v>
+        <v>0.15710834839861765</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>1.2345434669660094E-2</v>
+        <v>1.2249796226875831E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -32536,11 +32546,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.17685396642902151</v>
+        <v>0.16452648859675353</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>1.0684202798852155E-2</v>
+        <v>7.4181401981358863E-3</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -32549,11 +32559,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18403402280955466</v>
+        <v>0.17526783080645678</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>7.1800563805331508E-3</v>
+        <v>1.0741342209703242E-2</v>
       </c>
     </row>
   </sheetData>
@@ -32563,10 +32573,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD7DA879-7295-4B28-AB1F-AC4478E5196C}">
-  <dimension ref="A2:AA58"/>
+  <dimension ref="A2:AC58"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V19" sqref="V19"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -32578,7 +32588,7 @@
     <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
@@ -32603,8 +32613,14 @@
       <c r="V2" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="Y2" t="s">
+        <v>411</v>
+      </c>
+      <c r="Z2">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>3.84</v>
       </c>
@@ -32640,11 +32656,14 @@
       <c r="V3" s="97" t="s">
         <v>321</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Y3" t="s">
+        <v>412</v>
+      </c>
+      <c r="AB3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>1.98</v>
       </c>
@@ -32690,15 +32709,19 @@
       <c r="V4">
         <v>0</v>
       </c>
-      <c r="Z4">
+      <c r="Y4">
+        <f>ABS(V4-Z$2)</f>
+        <v>359</v>
+      </c>
+      <c r="AB4">
         <v>0</v>
       </c>
-      <c r="AA4">
-        <f>MOD(Z4+180,360)</f>
+      <c r="AC4">
+        <f>MOD(AB4+180,360)</f>
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>2.25</v>
       </c>
@@ -32734,15 +32757,23 @@
       <c r="V5">
         <v>23</v>
       </c>
-      <c r="Z5">
+      <c r="W5">
+        <f>V5-V4</f>
         <v>23</v>
       </c>
-      <c r="AA5">
-        <f t="shared" ref="AA5:AA19" si="5">MOD(Z5+180,360)</f>
+      <c r="Y5">
+        <f t="shared" ref="Y5:Y20" si="5">ABS(V5-Z$2)</f>
+        <v>336</v>
+      </c>
+      <c r="AB5">
+        <v>23</v>
+      </c>
+      <c r="AC5">
+        <f t="shared" ref="AC5:AC20" si="6">MOD(AB5+180,360)</f>
         <v>203</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>0.41</v>
       </c>
@@ -32772,7 +32803,7 @@
         <v>41</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" ref="J6" si="6">CONCATENATE(J4, H5, ", ", H6, I6, ", ")</f>
+        <f t="shared" ref="J6" si="7">CONCATENATE(J4, H5, ", ", H6, I6, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, </v>
       </c>
       <c r="R6" t="s">
@@ -32785,15 +32816,23 @@
       <c r="V6">
         <v>45</v>
       </c>
-      <c r="Z6">
+      <c r="W6">
+        <f t="shared" ref="W6:W20" si="8">V6-V5</f>
+        <v>22</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="5"/>
+        <v>314</v>
+      </c>
+      <c r="AB6">
         <v>45</v>
       </c>
-      <c r="AA6">
-        <f t="shared" si="5"/>
+      <c r="AC6">
+        <f t="shared" si="6"/>
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>0.45</v>
       </c>
@@ -32829,15 +32868,23 @@
       <c r="V7">
         <v>68</v>
       </c>
-      <c r="Z7">
+      <c r="W7">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="5"/>
+        <v>291</v>
+      </c>
+      <c r="AB7">
         <v>68</v>
       </c>
-      <c r="AA7">
-        <f t="shared" si="5"/>
+      <c r="AC7">
+        <f t="shared" si="6"/>
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>0.32</v>
       </c>
@@ -32867,7 +32914,7 @@
         <v>41</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" ref="J8" si="7">CONCATENATE(J6, H7, ", ", H8, I8, ", ")</f>
+        <f t="shared" ref="J8" si="9">CONCATENATE(J6, H7, ", ", H8, I8, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, </v>
       </c>
       <c r="R8" t="s">
@@ -32880,15 +32927,23 @@
       <c r="V8">
         <v>90</v>
       </c>
-      <c r="Z8">
+      <c r="W8">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="5"/>
+        <v>269</v>
+      </c>
+      <c r="AB8">
         <v>90</v>
       </c>
-      <c r="AA8">
-        <f t="shared" si="5"/>
+      <c r="AC8">
+        <f t="shared" si="6"/>
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>0.9</v>
       </c>
@@ -32924,15 +32979,23 @@
       <c r="V9">
         <v>113</v>
       </c>
-      <c r="Z9">
+      <c r="W9">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="5"/>
+        <v>246</v>
+      </c>
+      <c r="AB9">
         <v>113</v>
       </c>
-      <c r="AA9">
-        <f t="shared" si="5"/>
+      <c r="AC9">
+        <f t="shared" si="6"/>
         <v>293</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>0.62</v>
       </c>
@@ -32962,7 +33025,7 @@
         <v>41</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10" si="8">CONCATENATE(J8, H9, ", ", H10, I10, ", ")</f>
+        <f t="shared" ref="J10" si="10">CONCATENATE(J8, H9, ", ", H10, I10, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, 135, 157.5, </v>
       </c>
       <c r="R10" t="s">
@@ -32975,15 +33038,23 @@
       <c r="V10">
         <v>135</v>
       </c>
-      <c r="Z10">
+      <c r="W10">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="5"/>
+        <v>224</v>
+      </c>
+      <c r="AB10">
         <v>135</v>
       </c>
-      <c r="AA10">
-        <f t="shared" si="5"/>
+      <c r="AC10">
+        <f t="shared" si="6"/>
         <v>315</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>1.4</v>
       </c>
@@ -33019,15 +33090,23 @@
       <c r="V11">
         <v>158</v>
       </c>
-      <c r="Z11">
+      <c r="W11">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="5"/>
+        <v>201</v>
+      </c>
+      <c r="AB11">
         <v>156</v>
       </c>
-      <c r="AA11">
-        <f t="shared" si="5"/>
+      <c r="AC11">
+        <f t="shared" si="6"/>
         <v>336</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>1.19</v>
       </c>
@@ -33057,7 +33136,7 @@
         <v>41</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" ref="J12" si="9">CONCATENATE(J10, H11, ", ", H12, I12, ", ")</f>
+        <f t="shared" ref="J12" si="11">CONCATENATE(J10, H11, ", ", H12, I12, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, 135, 157.5, 180, 202.5, </v>
       </c>
       <c r="R12" t="s">
@@ -33070,15 +33149,23 @@
       <c r="V12">
         <v>180</v>
       </c>
-      <c r="Z12">
+      <c r="W12">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="5"/>
+        <v>179</v>
+      </c>
+      <c r="AB12">
         <v>180</v>
       </c>
-      <c r="AA12">
-        <f t="shared" si="5"/>
+      <c r="AC12">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>3.08</v>
       </c>
@@ -33114,15 +33201,23 @@
       <c r="V13">
         <v>203</v>
       </c>
-      <c r="Z13">
+      <c r="W13">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="5"/>
+        <v>156</v>
+      </c>
+      <c r="AB13">
         <v>203</v>
       </c>
-      <c r="AA13">
-        <f t="shared" si="5"/>
+      <c r="AC13">
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>2.93</v>
       </c>
@@ -33152,7 +33247,7 @@
         <v>41</v>
       </c>
       <c r="J14" t="str">
-        <f t="shared" ref="J14" si="10">CONCATENATE(J12, H13, ", ", H14, I14, ", ")</f>
+        <f t="shared" ref="J14" si="12">CONCATENATE(J12, H13, ", ", H14, I14, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, 135, 157.5, 180, 202.5, 225, 247.5, </v>
       </c>
       <c r="R14" t="s">
@@ -33165,15 +33260,23 @@
       <c r="V14">
         <v>225</v>
       </c>
-      <c r="Z14">
+      <c r="W14">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="5"/>
+        <v>134</v>
+      </c>
+      <c r="AB14">
         <v>225</v>
       </c>
-      <c r="AA14">
-        <f t="shared" si="5"/>
+      <c r="AC14">
+        <f t="shared" si="6"/>
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>4.62</v>
       </c>
@@ -33209,15 +33312,23 @@
       <c r="V15">
         <v>248</v>
       </c>
-      <c r="Z15">
+      <c r="W15">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" si="5"/>
+        <v>111</v>
+      </c>
+      <c r="AB15">
         <v>248</v>
       </c>
-      <c r="AA15">
-        <f t="shared" si="5"/>
+      <c r="AC15">
+        <f t="shared" si="6"/>
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>4.04</v>
       </c>
@@ -33247,7 +33358,7 @@
         <v>41</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" ref="J16" si="11">CONCATENATE(J14, H15, ", ", H16, I16, ", ")</f>
+        <f t="shared" ref="J16" si="13">CONCATENATE(J14, H15, ", ", H16, I16, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, 135, 157.5, 180, 202.5, 225, 247.5, 270, 292.5, </v>
       </c>
       <c r="R16" t="s">
@@ -33260,15 +33371,23 @@
       <c r="V16">
         <v>270</v>
       </c>
-      <c r="Z16">
+      <c r="W16">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" si="5"/>
+        <v>89</v>
+      </c>
+      <c r="AB16">
         <v>270</v>
       </c>
-      <c r="AA16">
-        <f t="shared" si="5"/>
+      <c r="AC16">
+        <f t="shared" si="6"/>
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>4.33</v>
       </c>
@@ -33304,15 +33423,23 @@
       <c r="V17">
         <v>293</v>
       </c>
-      <c r="Z17">
+      <c r="W17">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" si="5"/>
+        <v>66</v>
+      </c>
+      <c r="AB17">
         <v>293</v>
       </c>
-      <c r="AA17">
-        <f t="shared" si="5"/>
+      <c r="AC17">
+        <f t="shared" si="6"/>
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>3.43</v>
       </c>
@@ -33342,7 +33469,7 @@
         <v>41</v>
       </c>
       <c r="J18" t="str">
-        <f t="shared" ref="J18" si="12">CONCATENATE(J16, H17, ", ", H18, I18, ", ")</f>
+        <f t="shared" ref="J18" si="14">CONCATENATE(J16, H17, ", ", H18, I18, ", ")</f>
         <v xml:space="preserve">erreur0, 22.5, 45, 67.5, 90, 112.5, 135, 157.5, 180, 202.5, 225, 247.5, 270, 292.5, 315, 337.5, </v>
       </c>
       <c r="R18" t="s">
@@ -33355,15 +33482,23 @@
       <c r="V18">
         <v>313</v>
       </c>
-      <c r="Z18">
+      <c r="W18">
+        <f t="shared" si="8"/>
+        <v>20</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="AB18">
         <v>315</v>
       </c>
-      <c r="AA18">
-        <f t="shared" si="5"/>
+      <c r="AC18">
+        <f t="shared" si="6"/>
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C19" s="9">
         <v>360</v>
       </c>
@@ -33373,15 +33508,43 @@
       <c r="V19">
         <v>336</v>
       </c>
-      <c r="Z19">
+      <c r="W19">
+        <f t="shared" si="8"/>
+        <v>23</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AB19">
         <v>338</v>
       </c>
-      <c r="AA19">
+      <c r="AC19">
+        <f t="shared" si="6"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="V20">
+        <v>360</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="Y20">
         <f t="shared" si="5"/>
-        <v>158</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="AB20">
+        <v>360</v>
+      </c>
+      <c r="AC20">
+        <f t="shared" si="6"/>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>65.471999999999994</v>
       </c>
@@ -33407,7 +33570,7 @@
         <v>if(WindAngle &lt; 5) return("Nord");</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>83.885999999999996</v>
       </c>
@@ -33416,7 +33579,7 @@
       </c>
       <c r="C23" s="7"/>
       <c r="D23">
-        <f t="shared" ref="D23:D37" si="13">(A24+A23)/2</f>
+        <f t="shared" ref="D23:D37" si="15">(A24+A23)/2</f>
         <v>87.978000000000009</v>
       </c>
       <c r="F23" s="7"/>
@@ -33431,11 +33594,11 @@
         <v>62</v>
       </c>
       <c r="O23" s="7" t="str">
-        <f t="shared" ref="O23:O37" si="14">_xlfn.CONCAT("if(WindAngle &lt; ",K23+5, ") return(""",M23,""");")</f>
+        <f t="shared" ref="O23:O37" si="16">_xlfn.CONCAT("if(WindAngle &lt; ",K23+5, ") return(""",M23,""");")</f>
         <v>if(WindAngle &lt; 27,5) return("Nord");</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>92.070000000000007</v>
       </c>
@@ -33444,12 +33607,12 @@
       </c>
       <c r="C24" s="7"/>
       <c r="D24">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>109.46100000000001</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7" t="str">
-        <f t="shared" ref="G24:G37" si="15">_xlfn.CONCAT("if (WindAnalog &lt; ", ROUND(D24,0), ") return(", ROUND(B24, 1), ");")</f>
+        <f t="shared" ref="G24:G37" si="17">_xlfn.CONCAT("if (WindAnalog &lt; ", ROUND(D24,0), ") return(", ROUND(B24, 1), ");")</f>
         <v>if (WindAnalog &lt; 109) return(90);</v>
       </c>
       <c r="K24">
@@ -33459,11 +33622,11 @@
         <v>63</v>
       </c>
       <c r="O24" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 50) return("Nord-Est");</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>126.852</v>
       </c>
@@ -33472,12 +33635,12 @@
       </c>
       <c r="C25" s="7"/>
       <c r="D25">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>155.49600000000001</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 155) return(160);</v>
       </c>
       <c r="K25">
@@ -33487,11 +33650,11 @@
         <v>64</v>
       </c>
       <c r="O25" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 72,5) return("Est");</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>184.14000000000001</v>
       </c>
@@ -33500,12 +33663,12 @@
       </c>
       <c r="C26" s="7"/>
       <c r="D26">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>213.80700000000002</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 214) return(135);</v>
       </c>
       <c r="K26">
@@ -33515,11 +33678,11 @@
         <v>64</v>
       </c>
       <c r="O26" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 95) return("Est");</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>243.47399999999999</v>
       </c>
@@ -33528,12 +33691,12 @@
       </c>
       <c r="C27" s="7"/>
       <c r="D27">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>264.95699999999999</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 265) return(200);</v>
       </c>
       <c r="K27">
@@ -33543,11 +33706,11 @@
         <v>64</v>
       </c>
       <c r="O27" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 117,5) return("Est");</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>286.43999999999994</v>
       </c>
@@ -33556,12 +33719,12 @@
       </c>
       <c r="C28" s="7"/>
       <c r="D28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>345.774</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 346) return(180);</v>
       </c>
       <c r="K28">
@@ -33571,11 +33734,11 @@
         <v>65</v>
       </c>
       <c r="O28" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 140) return("Sud-Est");</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>405.108</v>
       </c>
@@ -33584,12 +33747,12 @@
       </c>
       <c r="C29" s="7"/>
       <c r="D29">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>432.72900000000004</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 433) return(20);</v>
       </c>
       <c r="K29">
@@ -33599,11 +33762,11 @@
         <v>66</v>
       </c>
       <c r="O29" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 162,5) return("Sud");</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>460.35</v>
       </c>
@@ -33612,12 +33775,12 @@
       </c>
       <c r="C30" s="7"/>
       <c r="D30">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>529.91399999999999</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 530) return(45);</v>
       </c>
       <c r="K30">
@@ -33627,11 +33790,11 @@
         <v>66</v>
       </c>
       <c r="O30" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 185) return("Sud");</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>599.47800000000007</v>
       </c>
@@ -33640,12 +33803,12 @@
       </c>
       <c r="C31" s="7"/>
       <c r="D31">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>614.82300000000009</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 615) return(250);</v>
       </c>
       <c r="K31">
@@ -33655,11 +33818,11 @@
         <v>66</v>
       </c>
       <c r="O31" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 207,5) return("Sud");</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>630.16800000000001</v>
       </c>
@@ -33668,12 +33831,12 @@
       </c>
       <c r="C32" s="7"/>
       <c r="D32">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>665.97299999999996</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 666) return(225);</v>
       </c>
       <c r="K32">
@@ -33683,7 +33846,7 @@
         <v>67</v>
       </c>
       <c r="O32" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 230) return("Sud-Ouest");</v>
       </c>
     </row>
@@ -33696,12 +33859,12 @@
       </c>
       <c r="C33" s="7"/>
       <c r="D33">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>743.721</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 744) return(340);</v>
       </c>
       <c r="K33">
@@ -33711,7 +33874,7 @@
         <v>68</v>
       </c>
       <c r="O33" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 252,5) return("Ouest");</v>
       </c>
     </row>
@@ -33724,12 +33887,12 @@
       </c>
       <c r="C34" s="7"/>
       <c r="D34">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>806.12400000000002</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 806) return(0);</v>
       </c>
       <c r="K34">
@@ -33739,7 +33902,7 @@
         <v>68</v>
       </c>
       <c r="O34" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 275) return("Ouest");</v>
       </c>
     </row>
@@ -33752,12 +33915,12 @@
       </c>
       <c r="C35" s="7"/>
       <c r="D35">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>856.25099999999998</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 856) return(290);</v>
       </c>
       <c r="K35">
@@ -33767,7 +33930,7 @@
         <v>68</v>
       </c>
       <c r="O35" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 297,5) return("Ouest");</v>
       </c>
     </row>
@@ -33780,12 +33943,12 @@
       </c>
       <c r="C36" s="7"/>
       <c r="D36">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>915.58500000000004</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 916) return(315);</v>
       </c>
       <c r="K36">
@@ -33795,7 +33958,7 @@
         <v>69</v>
       </c>
       <c r="O36" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 320) return("Nord-Ouest");</v>
       </c>
     </row>
@@ -33808,12 +33971,12 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>984.12599999999998</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="7" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>if (WindAnalog &lt; 984) return(270);</v>
       </c>
       <c r="K37">
@@ -33823,7 +33986,7 @@
         <v>62</v>
       </c>
       <c r="O37" s="7" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>if(WindAngle &lt; 342,5) return("Nord");</v>
       </c>
     </row>
@@ -33845,7 +34008,7 @@
         <v>65.536000000000001</v>
       </c>
       <c r="B43">
-        <f t="shared" ref="B43:B57" si="16">(A43+A44)/2</f>
+        <f t="shared" ref="B43:B57" si="18">(A43+A44)/2</f>
         <v>75.775999999999996</v>
       </c>
       <c r="C43" s="7">
@@ -33863,7 +34026,7 @@
         <v>86.015999999999991</v>
       </c>
       <c r="B44">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>90.623999999999995</v>
       </c>
       <c r="C44" s="7">
@@ -33872,7 +34035,7 @@
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="7" t="str">
-        <f t="shared" ref="G44:G58" si="17">_xlfn.CONCAT("if (WindAnalog &lt; ", ROUND(B44,0), ") return(", ROUND(C44, 1), ");")</f>
+        <f t="shared" ref="G44:G58" si="19">_xlfn.CONCAT("if (WindAnalog &lt; ", ROUND(B44,0), ") return(", ROUND(C44, 1), ");")</f>
         <v>if (WindAnalog &lt; 91) return(67,5);</v>
       </c>
     </row>
@@ -33881,7 +34044,7 @@
         <v>95.231999999999999</v>
       </c>
       <c r="B45">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>113.152</v>
       </c>
       <c r="C45" s="7">
@@ -33890,7 +34053,7 @@
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 113) return(90);</v>
       </c>
     </row>
@@ -33899,7 +34062,7 @@
         <v>131.072</v>
       </c>
       <c r="B46">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>160.768</v>
       </c>
       <c r="C46" s="7">
@@ -33908,7 +34071,7 @@
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 161) return(157,5);</v>
       </c>
     </row>
@@ -33917,7 +34080,7 @@
         <v>190.464</v>
       </c>
       <c r="B47">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>221.184</v>
       </c>
       <c r="C47" s="7">
@@ -33926,7 +34089,7 @@
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
       <c r="G47" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 221) return(135);</v>
       </c>
     </row>
@@ -33935,7 +34098,7 @@
         <v>251.904</v>
       </c>
       <c r="B48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>274.43200000000002</v>
       </c>
       <c r="C48" s="7">
@@ -33944,7 +34107,7 @@
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
       <c r="G48" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 274) return(202,5);</v>
       </c>
     </row>
@@ -33953,7 +34116,7 @@
         <v>296.95999999999998</v>
       </c>
       <c r="B49">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>359.42399999999998</v>
       </c>
       <c r="C49" s="7">
@@ -33962,7 +34125,7 @@
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 359) return(180);</v>
       </c>
     </row>
@@ -33971,7 +34134,7 @@
         <v>421.88800000000003</v>
       </c>
       <c r="B50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>450.56</v>
       </c>
       <c r="C50" s="7">
@@ -33980,7 +34143,7 @@
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
       <c r="G50" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 451) return(22,5);</v>
       </c>
     </row>
@@ -33989,7 +34152,7 @@
         <v>479.23199999999997</v>
       </c>
       <c r="B51">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>550.91200000000003</v>
       </c>
       <c r="C51" s="7">
@@ -33998,7 +34161,7 @@
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
       <c r="G51" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 551) return(45);</v>
       </c>
     </row>
@@ -34007,7 +34170,7 @@
         <v>622.59199999999998</v>
       </c>
       <c r="B52">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>638.976</v>
       </c>
       <c r="C52" s="7">
@@ -34016,7 +34179,7 @@
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
       <c r="G52" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 639) return(247,5);</v>
       </c>
     </row>
@@ -34025,7 +34188,7 @@
         <v>655.36</v>
       </c>
       <c r="B53">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>693.24800000000005</v>
       </c>
       <c r="C53" s="7">
@@ -34034,7 +34197,7 @@
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
       <c r="G53" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 693) return(225);</v>
       </c>
     </row>
@@ -34043,7 +34206,7 @@
         <v>731.13599999999997</v>
       </c>
       <c r="B54">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>774.14400000000001</v>
       </c>
       <c r="C54" s="7">
@@ -34052,7 +34215,7 @@
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
       <c r="G54" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 774) return(337,5);</v>
       </c>
     </row>
@@ -34061,7 +34224,7 @@
         <v>817.15200000000004</v>
       </c>
       <c r="B55">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>838.65600000000006</v>
       </c>
       <c r="C55" s="7">
@@ -34070,7 +34233,7 @@
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
       <c r="G55" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 839) return(0);</v>
       </c>
     </row>
@@ -34079,7 +34242,7 @@
         <v>860.16000000000008</v>
       </c>
       <c r="B56">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>890.88000000000011</v>
       </c>
       <c r="C56" s="7">
@@ -34088,7 +34251,7 @@
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 891) return(292,5);</v>
       </c>
     </row>
@@ -34097,7 +34260,7 @@
         <v>921.6</v>
       </c>
       <c r="B57">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>951.29600000000005</v>
       </c>
       <c r="C57" s="7">
@@ -34106,7 +34269,7 @@
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 951) return(315);</v>
       </c>
     </row>
@@ -34123,7 +34286,7 @@
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="7" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>if (WindAnalog &lt; 1023) return(270);</v>
       </c>
     </row>
@@ -59048,44 +59211,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7B9E23-8CD5-4E87-87C5-78B003674011}">
-  <dimension ref="B2:Q27"/>
+  <dimension ref="B2:S27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="7.5546875" customWidth="1"/>
     <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" style="5"/>
-    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" customWidth="1"/>
-    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" style="5"/>
+    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" ht="63" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:19" ht="63" customHeight="1" x14ac:dyDescent="0.6">
       <c r="B2" s="121" t="s">
         <v>348</v>
       </c>
       <c r="C2" s="121"/>
       <c r="D2" s="121"/>
-      <c r="G2" t="s">
+      <c r="F2" s="121" t="s">
         <v>391</v>
       </c>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31" t="s">
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="M2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="N2" s="41" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:17" ht="21" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:19" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="101" t="s">
         <v>349</v>
       </c>
@@ -59098,23 +59264,26 @@
       <c r="F3" s="111" t="s">
         <v>184</v>
       </c>
-      <c r="I3" s="26">
+      <c r="G3" s="111" t="s">
+        <v>409</v>
+      </c>
+      <c r="K3" s="26">
         <v>0</v>
       </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="28"/>
-      <c r="L3" s="29"/>
-      <c r="O3" s="114" t="s">
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="29"/>
+      <c r="Q3" s="114" t="s">
         <v>151</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>177</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="100">
         <v>0</v>
       </c>
@@ -59125,24 +59294,27 @@
       <c r="F4" t="s">
         <v>402</v>
       </c>
-      <c r="G4" t="s">
-        <v>403</v>
-      </c>
-      <c r="I4" s="23">
+      <c r="G4">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>410</v>
+      </c>
+      <c r="K4" s="23">
         <v>1</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="17"/>
-      <c r="O4" s="114"/>
-      <c r="P4" t="s">
+      <c r="L4" s="20"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="17"/>
+      <c r="Q4" s="114"/>
+      <c r="R4" t="s">
         <v>179</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="100">
         <v>1</v>
       </c>
@@ -59153,30 +59325,33 @@
       <c r="F5" t="s">
         <v>392</v>
       </c>
-      <c r="G5" t="s">
-        <v>404</v>
-      </c>
-      <c r="I5" s="23">
+      <c r="G5">
+        <v>5</v>
+      </c>
+      <c r="H5" t="s">
+        <v>403</v>
+      </c>
+      <c r="K5" s="23">
         <v>2</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="L5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="M5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="N5" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="O5" s="114"/>
-      <c r="P5" t="s">
+      <c r="Q5" s="114"/>
+      <c r="R5" t="s">
         <v>70</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="S5" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B6" s="100">
         <v>2</v>
       </c>
@@ -59185,28 +59360,31 @@
       <c r="F6" t="s">
         <v>393</v>
       </c>
-      <c r="G6" t="s">
-        <v>405</v>
-      </c>
-      <c r="I6" s="23">
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>404</v>
+      </c>
+      <c r="K6" s="23">
         <v>3</v>
       </c>
-      <c r="J6" s="21"/>
-      <c r="K6" s="16" t="s">
+      <c r="L6" s="21"/>
+      <c r="M6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L6" s="17" t="s">
+      <c r="N6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="114"/>
-      <c r="P6" t="s">
+      <c r="Q6" s="114"/>
+      <c r="R6" t="s">
         <v>172</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="S6" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B7" s="100">
         <v>3</v>
       </c>
@@ -59217,16 +59395,19 @@
       <c r="F7" t="s">
         <v>394</v>
       </c>
-      <c r="I7" s="23">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="23">
         <v>4</v>
       </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="17" t="s">
+      <c r="L7" s="21"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="17" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="100">
         <v>4</v>
       </c>
@@ -59237,16 +59418,19 @@
       <c r="F8" t="s">
         <v>395</v>
       </c>
-      <c r="I8" s="23">
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="23">
         <v>5</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="17" t="s">
+      <c r="L8" s="21"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" s="100">
         <v>5</v>
       </c>
@@ -59255,41 +59439,47 @@
       <c r="F9" t="s">
         <v>396</v>
       </c>
-      <c r="G9" t="s">
-        <v>406</v>
-      </c>
-      <c r="I9" s="23">
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9" t="s">
+        <v>405</v>
+      </c>
+      <c r="K9" s="23">
         <v>6</v>
       </c>
-      <c r="J9" s="21"/>
-      <c r="K9" s="16" t="s">
+      <c r="L9" s="21"/>
+      <c r="M9" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="L9" s="17"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="N9" s="17"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10" s="100">
         <v>6</v>
       </c>
       <c r="C10" s="100"/>
       <c r="D10" s="100" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F10" t="s">
         <v>397</v>
       </c>
-      <c r="I10" s="23">
+      <c r="G10">
+        <v>12</v>
+      </c>
+      <c r="K10" s="23">
         <v>7</v>
       </c>
-      <c r="J10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="M10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="L10" s="17"/>
-    </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="N10" s="17"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B11" s="100">
         <v>7</v>
       </c>
@@ -59298,14 +59488,17 @@
       <c r="F11" t="s">
         <v>398</v>
       </c>
-      <c r="I11" s="23">
+      <c r="G11">
+        <v>13</v>
+      </c>
+      <c r="K11" s="23">
         <v>8</v>
       </c>
-      <c r="J11" s="21"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="17"/>
-    </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="L11" s="21"/>
+      <c r="M11" s="16"/>
+      <c r="N11" s="17"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B12" s="100">
         <v>8</v>
       </c>
@@ -59316,16 +59509,19 @@
       <c r="F12" t="s">
         <v>399</v>
       </c>
-      <c r="I12" s="23">
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="K12" s="23">
         <v>9</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="L12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="K12" s="16"/>
-      <c r="L12" s="17"/>
-    </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.35">
+      <c r="M12" s="16"/>
+      <c r="N12" s="17"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B13" s="100">
         <v>9</v>
       </c>
@@ -59336,20 +59532,20 @@
       <c r="F13" t="s">
         <v>400</v>
       </c>
-      <c r="I13" s="23">
+      <c r="K13" s="23">
         <v>10</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="L13" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="16" t="s">
+      <c r="M13" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="17" t="s">
+      <c r="N13" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="100">
         <v>10</v>
       </c>
@@ -59360,20 +59556,20 @@
       <c r="F14" t="s">
         <v>401</v>
       </c>
-      <c r="I14" s="23">
+      <c r="K14" s="23">
         <v>11</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="L14" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="M14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="L14" s="17" t="s">
+      <c r="N14" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B15" s="100">
         <v>11</v>
       </c>
@@ -59383,20 +59579,20 @@
       <c r="D15" s="100" t="s">
         <v>366</v>
       </c>
-      <c r="I15" s="23">
+      <c r="K15" s="23">
         <v>12</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="L15" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="16" t="s">
+      <c r="M15" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="L15" s="17" t="s">
+      <c r="N15" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="100">
         <v>12</v>
       </c>
@@ -59404,22 +59600,22 @@
         <v>74</v>
       </c>
       <c r="D16" s="100" t="s">
-        <v>409</v>
-      </c>
-      <c r="I16" s="33">
+        <v>408</v>
+      </c>
+      <c r="K16" s="33">
         <v>13</v>
       </c>
-      <c r="J16" s="34" t="s">
+      <c r="L16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="M16" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="L16" s="36" t="s">
+      <c r="N16" s="36" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B17" s="100">
         <v>13</v>
       </c>
@@ -59427,73 +59623,73 @@
         <v>355</v>
       </c>
       <c r="D17" s="112" t="s">
-        <v>407</v>
-      </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="40"/>
-    </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+        <v>406</v>
+      </c>
+      <c r="K17" s="38"/>
+      <c r="L17" s="39"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="40"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B18" s="100" t="s">
         <v>356</v>
       </c>
       <c r="C18" s="100"/>
       <c r="D18" s="100"/>
-      <c r="I18" s="37" t="s">
+      <c r="K18" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="27"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="29"/>
-    </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="L18" s="27"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="29"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B19" s="100" t="s">
         <v>357</v>
       </c>
       <c r="D19" s="100"/>
-      <c r="I19" s="24" t="s">
+      <c r="K19" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="20"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="17"/>
-    </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="L19" s="20"/>
+      <c r="M19" s="16"/>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B20" s="100" t="s">
         <v>358</v>
       </c>
       <c r="C20" s="100"/>
       <c r="D20" s="100"/>
-      <c r="I20" s="24" t="s">
+      <c r="K20" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="L20" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K20" s="16"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="M20" s="16"/>
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B21" s="100" t="s">
         <v>359</v>
       </c>
       <c r="C21" s="100"/>
       <c r="D21" s="100"/>
-      <c r="I21" s="24" t="s">
+      <c r="K21" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="L21" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="K21" s="16" t="s">
+      <c r="M21" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="L21" s="17" t="s">
+      <c r="N21" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B22" s="100" t="s">
         <v>360</v>
       </c>
@@ -59501,14 +59697,14 @@
         <v>362</v>
       </c>
       <c r="D22" s="100"/>
-      <c r="I22" s="24" t="s">
+      <c r="K22" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J22" s="20"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="17"/>
-    </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="L22" s="20"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B23" s="100" t="s">
         <v>361</v>
       </c>
@@ -59516,14 +59712,14 @@
         <v>175</v>
       </c>
       <c r="D23" s="100"/>
-      <c r="I23" s="25" t="s">
+      <c r="K23" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="J23" s="22"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="19"/>
-    </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="L23" s="22"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="19"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B24" s="100">
         <v>20</v>
       </c>
@@ -59531,9 +59727,9 @@
         <v>149</v>
       </c>
       <c r="D24" s="123"/>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="K24" s="14"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B25" s="100">
         <v>21</v>
       </c>
@@ -59542,28 +59738,28 @@
       </c>
       <c r="D25" s="124"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="I26" s="14" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="K26" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>70</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="J27" t="s">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="L27" t="s">
         <v>71</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="O3:O6"/>
+  <mergeCells count="11">
+    <mergeCell ref="Q3:Q6"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C25:D25"/>
@@ -59573,6 +59769,7 @@
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="F2:H2"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>